<commit_message>
Tabla de contenidos grado 8
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdgarJosué\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion09\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -990,76 +995,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1140,6 +1079,72 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1200,7 +1205,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1235,7 +1240,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1446,2370 +1451,2364 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GH90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K26" sqref="A26:XFD26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="16" customWidth="1"/>
-    <col min="3" max="3" width="23" style="16" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="16" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="16" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" style="47" customWidth="1"/>
-    <col min="7" max="7" width="25.85546875" style="16" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="47" customWidth="1"/>
-    <col min="9" max="9" width="11" style="47" customWidth="1"/>
-    <col min="10" max="10" width="37.28515625" style="16" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" style="16" customWidth="1"/>
-    <col min="12" max="12" width="17.42578125" style="16" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" style="16" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" style="16" customWidth="1"/>
-    <col min="15" max="15" width="19.7109375" style="47" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" style="47" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" style="47" customWidth="1"/>
-    <col min="18" max="18" width="12" style="16" customWidth="1"/>
-    <col min="19" max="19" width="17.85546875" style="16" customWidth="1"/>
-    <col min="20" max="20" width="22.42578125" style="16" customWidth="1"/>
-    <col min="21" max="21" width="15.5703125" style="16" customWidth="1"/>
-    <col min="22" max="16384" width="11.42578125" style="16"/>
+    <col min="1" max="1" width="18.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="25" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="25" customWidth="1"/>
+    <col min="9" max="9" width="11" style="25" customWidth="1"/>
+    <col min="10" max="10" width="37.28515625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="3" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="19.7109375" style="25" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" style="25" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" style="25" customWidth="1"/>
+    <col min="18" max="18" width="12" style="3" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" style="3" customWidth="1"/>
+    <col min="20" max="20" width="22.42578125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="15.5703125" style="3" customWidth="1"/>
+    <col min="22" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="40" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="K1" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="M1" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="11"/>
-      <c r="O1" s="12" t="s">
+      <c r="N1" s="50"/>
+      <c r="O1" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="12" t="s">
+      <c r="P1" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="13" t="s">
+      <c r="Q1" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="13" t="s">
+      <c r="S1" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="15" t="s">
+      <c r="T1" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="13" t="s">
+      <c r="U1" s="33" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:190" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="25" t="s">
+      <c r="A2" s="43"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="N2" s="25" t="s">
+      <c r="N2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="13"/>
-    </row>
-    <row r="3" spans="1:190" ht="22.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="27" t="s">
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="35"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="34"/>
+      <c r="U2" s="33"/>
+    </row>
+    <row r="3" spans="1:190" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E3" s="31"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="33" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="H3" s="32">
+      <c r="H3" s="10">
         <v>1</v>
       </c>
-      <c r="I3" s="34" t="s">
+      <c r="I3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="35" t="s">
+      <c r="J3" s="13" t="s">
         <v>169</v>
       </c>
-      <c r="K3" s="36" t="s">
+      <c r="K3" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="33" t="s">
+      <c r="L3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="37" t="s">
+      <c r="M3" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="37"/>
-      <c r="O3" s="32" t="s">
+      <c r="N3" s="15"/>
+      <c r="O3" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="P3" s="32" t="s">
+      <c r="P3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="Q3" s="38">
+      <c r="Q3" s="16">
         <v>6</v>
       </c>
-      <c r="R3" s="39" t="s">
+      <c r="R3" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="S3" s="38" t="s">
+      <c r="S3" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="T3" s="40" t="s">
+      <c r="T3" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="U3" s="38" t="s">
+      <c r="U3" s="16" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="27" t="s">
+    <row r="4" spans="1:190" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E4" s="31"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="41" t="s">
+      <c r="E4" s="9"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="H4" s="32">
+      <c r="H4" s="10">
         <v>2</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="42" t="s">
+      <c r="J4" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="K4" s="36" t="s">
+      <c r="K4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="33" t="s">
+      <c r="L4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="37"/>
-      <c r="N4" s="37" t="s">
+      <c r="M4" s="15"/>
+      <c r="N4" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="32" t="s">
+      <c r="O4" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="P4" s="32" t="s">
+      <c r="P4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="38">
+      <c r="Q4" s="16">
         <v>6</v>
       </c>
-      <c r="R4" s="39" t="s">
+      <c r="R4" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S4" s="38" t="s">
+      <c r="S4" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T4" s="40" t="s">
+      <c r="T4" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="U4" s="38" t="s">
+      <c r="U4" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="5" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
+    <row r="5" spans="1:190" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E5" s="31"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="41" t="s">
+      <c r="E5" s="9"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="H5" s="32">
+      <c r="H5" s="10">
         <v>3</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="I5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="42" t="s">
+      <c r="J5" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="K5" s="36" t="s">
+      <c r="K5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="33" t="s">
+      <c r="L5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="37"/>
-      <c r="N5" s="37" t="s">
+      <c r="M5" s="15"/>
+      <c r="N5" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="O5" s="32" t="s">
+      <c r="O5" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="P5" s="32" t="s">
+      <c r="P5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="38">
+      <c r="Q5" s="16">
         <v>6</v>
       </c>
-      <c r="R5" s="39" t="s">
+      <c r="R5" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S5" s="38" t="s">
+      <c r="S5" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T5" s="40" t="s">
+      <c r="T5" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="U5" s="38" t="s">
+      <c r="U5" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="6" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
+    <row r="6" spans="1:190" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E6" s="31"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="41" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="H6" s="32">
+      <c r="H6" s="10">
         <v>4</v>
       </c>
-      <c r="I6" s="34" t="s">
+      <c r="I6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="42" t="s">
+      <c r="J6" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="K6" s="36" t="s">
+      <c r="K6" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="33" t="s">
+      <c r="L6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37" t="s">
+      <c r="M6" s="15"/>
+      <c r="N6" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="32" t="s">
+      <c r="O6" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="P6" s="32" t="s">
+      <c r="P6" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="38">
+      <c r="Q6" s="16">
         <v>6</v>
       </c>
-      <c r="R6" s="39" t="s">
+      <c r="R6" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S6" s="38" t="s">
+      <c r="S6" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T6" s="40" t="s">
+      <c r="T6" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="U6" s="38" t="s">
+      <c r="U6" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="7" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+    <row r="7" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="41" t="s">
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="H7" s="32">
+      <c r="H7" s="10">
         <v>5</v>
       </c>
-      <c r="I7" s="34" t="s">
+      <c r="I7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="42" t="s">
+      <c r="J7" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="K7" s="36" t="s">
+      <c r="K7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="33" t="s">
+      <c r="L7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="37"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="32" t="s">
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="P7" s="32" t="s">
+      <c r="P7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="43">
+      <c r="Q7" s="21">
         <v>9</v>
       </c>
-      <c r="R7" s="44" t="s">
+      <c r="R7" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="S7" s="43" t="s">
+      <c r="S7" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="T7" s="45" t="s">
+      <c r="T7" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="U7" s="43" t="s">
+      <c r="U7" s="21" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="27" t="s">
+    <row r="8" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="41" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="H8" s="32">
+      <c r="H8" s="10">
         <v>6</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="46" t="s">
+      <c r="J8" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="K8" s="36" t="s">
+      <c r="K8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="33" t="s">
+      <c r="L8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="M8" s="37" t="s">
+      <c r="M8" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="N8" s="37"/>
-      <c r="O8" s="32" t="s">
+      <c r="N8" s="15"/>
+      <c r="O8" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="P8" s="32" t="s">
+      <c r="P8" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="38">
+      <c r="Q8" s="16">
         <v>6</v>
       </c>
-      <c r="R8" s="39" t="s">
+      <c r="R8" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="S8" s="38" t="s">
+      <c r="S8" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="T8" s="40" t="s">
+      <c r="T8" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="U8" s="38" t="s">
+      <c r="U8" s="16" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:190" s="48" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="27" t="s">
+    <row r="9" spans="1:190" s="26" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="41" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="19" t="s">
         <v>149</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="10">
         <v>7</v>
       </c>
-      <c r="I9" s="34" t="s">
+      <c r="I9" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="42" t="s">
+      <c r="J9" s="20" t="s">
         <v>175</v>
       </c>
-      <c r="K9" s="36" t="s">
+      <c r="K9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="33" t="s">
+      <c r="L9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="37"/>
-      <c r="N9" s="37" t="s">
+      <c r="M9" s="15"/>
+      <c r="N9" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="O9" s="32" t="s">
+      <c r="O9" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="P9" s="32" t="s">
+      <c r="P9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="38">
+      <c r="Q9" s="16">
         <v>6</v>
       </c>
-      <c r="R9" s="39" t="s">
+      <c r="R9" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S9" s="38" t="s">
+      <c r="S9" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T9" s="40" t="s">
+      <c r="T9" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="U9" s="38" t="s">
+      <c r="U9" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="V9" s="47"/>
-      <c r="W9" s="47"/>
-      <c r="X9" s="47"/>
-      <c r="Y9" s="47"/>
-      <c r="Z9" s="47"/>
-      <c r="AA9" s="47"/>
-      <c r="AB9" s="47"/>
-      <c r="AC9" s="47"/>
-      <c r="AD9" s="47"/>
-      <c r="AE9" s="47"/>
-      <c r="AF9" s="47"/>
-      <c r="AG9" s="47"/>
-      <c r="AH9" s="47"/>
-      <c r="AI9" s="47"/>
-      <c r="AJ9" s="47"/>
-      <c r="AK9" s="47"/>
-      <c r="AL9" s="47"/>
-      <c r="AM9" s="47"/>
-      <c r="AN9" s="47"/>
-      <c r="AO9" s="47"/>
-      <c r="AP9" s="47"/>
-      <c r="AQ9" s="47"/>
-      <c r="AR9" s="47"/>
-      <c r="AS9" s="47"/>
-      <c r="AT9" s="47"/>
-      <c r="AU9" s="47"/>
-      <c r="AV9" s="47"/>
-      <c r="AW9" s="47"/>
-      <c r="AX9" s="47"/>
-      <c r="AY9" s="47"/>
-      <c r="AZ9" s="47"/>
-      <c r="BA9" s="47"/>
-      <c r="BB9" s="47"/>
-      <c r="BC9" s="47"/>
-      <c r="BD9" s="47"/>
-      <c r="BE9" s="47"/>
-      <c r="BF9" s="47"/>
-      <c r="BG9" s="47"/>
-      <c r="BH9" s="47"/>
-      <c r="BI9" s="47"/>
-      <c r="BJ9" s="47"/>
-      <c r="BK9" s="47"/>
-      <c r="BL9" s="47"/>
-      <c r="BM9" s="47"/>
-      <c r="BN9" s="47"/>
-      <c r="BO9" s="47"/>
-      <c r="BP9" s="47"/>
-      <c r="BQ9" s="47"/>
-      <c r="BR9" s="47"/>
-      <c r="BS9" s="47"/>
-      <c r="BT9" s="47"/>
-      <c r="BU9" s="47"/>
-      <c r="BV9" s="47"/>
-      <c r="BW9" s="47"/>
-      <c r="BX9" s="47"/>
-      <c r="BY9" s="47"/>
-      <c r="BZ9" s="47"/>
-      <c r="CA9" s="47"/>
-      <c r="CB9" s="47"/>
-      <c r="CC9" s="47"/>
-      <c r="CD9" s="47"/>
-      <c r="CE9" s="47"/>
-      <c r="CF9" s="47"/>
-      <c r="CG9" s="47"/>
-      <c r="CH9" s="47"/>
-      <c r="CI9" s="47"/>
-      <c r="CJ9" s="47"/>
-      <c r="CK9" s="47"/>
-      <c r="CL9" s="47"/>
-      <c r="CM9" s="47"/>
-      <c r="CN9" s="47"/>
-      <c r="CO9" s="47"/>
-      <c r="CP9" s="47"/>
-      <c r="CQ9" s="47"/>
-      <c r="CR9" s="47"/>
-      <c r="CS9" s="47"/>
-      <c r="CT9" s="47"/>
-      <c r="CU9" s="47"/>
-      <c r="CV9" s="47"/>
-      <c r="CW9" s="47"/>
-      <c r="CX9" s="47"/>
-      <c r="CY9" s="47"/>
-      <c r="CZ9" s="47"/>
-      <c r="DA9" s="47"/>
-      <c r="DB9" s="47"/>
-      <c r="DC9" s="47"/>
-      <c r="DD9" s="47"/>
-      <c r="DE9" s="47"/>
-      <c r="DF9" s="47"/>
-      <c r="DG9" s="47"/>
-      <c r="DH9" s="47"/>
-      <c r="DI9" s="47"/>
-      <c r="DJ9" s="47"/>
-      <c r="DK9" s="47"/>
-      <c r="DL9" s="47"/>
-      <c r="DM9" s="47"/>
-      <c r="DN9" s="47"/>
-      <c r="DO9" s="47"/>
-      <c r="DP9" s="47"/>
-      <c r="DQ9" s="47"/>
-      <c r="DR9" s="47"/>
-      <c r="DS9" s="47"/>
-      <c r="DT9" s="47"/>
-      <c r="DU9" s="47"/>
-      <c r="DV9" s="47"/>
-      <c r="DW9" s="47"/>
-      <c r="DX9" s="47"/>
-      <c r="DY9" s="47"/>
-      <c r="DZ9" s="47"/>
-      <c r="EA9" s="47"/>
-      <c r="EB9" s="47"/>
-      <c r="EC9" s="47"/>
-      <c r="ED9" s="47"/>
-      <c r="EE9" s="47"/>
-      <c r="EF9" s="47"/>
-      <c r="EG9" s="47"/>
-      <c r="EH9" s="47"/>
-      <c r="EI9" s="47"/>
-      <c r="EJ9" s="47"/>
-      <c r="EK9" s="47"/>
-      <c r="EL9" s="47"/>
-      <c r="EM9" s="47"/>
-      <c r="EN9" s="47"/>
-      <c r="EO9" s="47"/>
-      <c r="EP9" s="47"/>
-      <c r="EQ9" s="47"/>
-      <c r="ER9" s="47"/>
-      <c r="ES9" s="47"/>
-      <c r="ET9" s="47"/>
-      <c r="EU9" s="47"/>
-      <c r="EV9" s="47"/>
-      <c r="EW9" s="47"/>
-      <c r="EX9" s="47"/>
-      <c r="EY9" s="47"/>
-      <c r="EZ9" s="47"/>
-      <c r="FA9" s="47"/>
-      <c r="FB9" s="47"/>
-      <c r="FC9" s="47"/>
-      <c r="FD9" s="47"/>
-      <c r="FE9" s="47"/>
-      <c r="FF9" s="47"/>
-      <c r="FG9" s="47"/>
-      <c r="FH9" s="47"/>
-      <c r="FI9" s="47"/>
-      <c r="FJ9" s="47"/>
-      <c r="FK9" s="47"/>
-      <c r="FL9" s="47"/>
-      <c r="FM9" s="47"/>
-      <c r="FN9" s="47"/>
-      <c r="FO9" s="47"/>
-      <c r="FP9" s="47"/>
-      <c r="FQ9" s="47"/>
-      <c r="FR9" s="47"/>
-      <c r="FS9" s="47"/>
-      <c r="FT9" s="47"/>
-      <c r="FU9" s="47"/>
-      <c r="FV9" s="47"/>
-      <c r="FW9" s="47"/>
-      <c r="FX9" s="47"/>
-      <c r="FY9" s="47"/>
-      <c r="FZ9" s="47"/>
-      <c r="GA9" s="47"/>
-      <c r="GB9" s="47"/>
-      <c r="GC9" s="47"/>
-      <c r="GD9" s="47"/>
-      <c r="GE9" s="47"/>
-      <c r="GF9" s="47"/>
-      <c r="GG9" s="47"/>
-      <c r="GH9" s="47"/>
-    </row>
-    <row r="10" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="27" t="s">
+      <c r="V9" s="25"/>
+      <c r="W9" s="25"/>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
+      <c r="AA9" s="25"/>
+      <c r="AB9" s="25"/>
+      <c r="AC9" s="25"/>
+      <c r="AD9" s="25"/>
+      <c r="AE9" s="25"/>
+      <c r="AF9" s="25"/>
+      <c r="AG9" s="25"/>
+      <c r="AH9" s="25"/>
+      <c r="AI9" s="25"/>
+      <c r="AJ9" s="25"/>
+      <c r="AK9" s="25"/>
+      <c r="AL9" s="25"/>
+      <c r="AM9" s="25"/>
+      <c r="AN9" s="25"/>
+      <c r="AO9" s="25"/>
+      <c r="AP9" s="25"/>
+      <c r="AQ9" s="25"/>
+      <c r="AR9" s="25"/>
+      <c r="AS9" s="25"/>
+      <c r="AT9" s="25"/>
+      <c r="AU9" s="25"/>
+      <c r="AV9" s="25"/>
+      <c r="AW9" s="25"/>
+      <c r="AX9" s="25"/>
+      <c r="AY9" s="25"/>
+      <c r="AZ9" s="25"/>
+      <c r="BA9" s="25"/>
+      <c r="BB9" s="25"/>
+      <c r="BC9" s="25"/>
+      <c r="BD9" s="25"/>
+      <c r="BE9" s="25"/>
+      <c r="BF9" s="25"/>
+      <c r="BG9" s="25"/>
+      <c r="BH9" s="25"/>
+      <c r="BI9" s="25"/>
+      <c r="BJ9" s="25"/>
+      <c r="BK9" s="25"/>
+      <c r="BL9" s="25"/>
+      <c r="BM9" s="25"/>
+      <c r="BN9" s="25"/>
+      <c r="BO9" s="25"/>
+      <c r="BP9" s="25"/>
+      <c r="BQ9" s="25"/>
+      <c r="BR9" s="25"/>
+      <c r="BS9" s="25"/>
+      <c r="BT9" s="25"/>
+      <c r="BU9" s="25"/>
+      <c r="BV9" s="25"/>
+      <c r="BW9" s="25"/>
+      <c r="BX9" s="25"/>
+      <c r="BY9" s="25"/>
+      <c r="BZ9" s="25"/>
+      <c r="CA9" s="25"/>
+      <c r="CB9" s="25"/>
+      <c r="CC9" s="25"/>
+      <c r="CD9" s="25"/>
+      <c r="CE9" s="25"/>
+      <c r="CF9" s="25"/>
+      <c r="CG9" s="25"/>
+      <c r="CH9" s="25"/>
+      <c r="CI9" s="25"/>
+      <c r="CJ9" s="25"/>
+      <c r="CK9" s="25"/>
+      <c r="CL9" s="25"/>
+      <c r="CM9" s="25"/>
+      <c r="CN9" s="25"/>
+      <c r="CO9" s="25"/>
+      <c r="CP9" s="25"/>
+      <c r="CQ9" s="25"/>
+      <c r="CR9" s="25"/>
+      <c r="CS9" s="25"/>
+      <c r="CT9" s="25"/>
+      <c r="CU9" s="25"/>
+      <c r="CV9" s="25"/>
+      <c r="CW9" s="25"/>
+      <c r="CX9" s="25"/>
+      <c r="CY9" s="25"/>
+      <c r="CZ9" s="25"/>
+      <c r="DA9" s="25"/>
+      <c r="DB9" s="25"/>
+      <c r="DC9" s="25"/>
+      <c r="DD9" s="25"/>
+      <c r="DE9" s="25"/>
+      <c r="DF9" s="25"/>
+      <c r="DG9" s="25"/>
+      <c r="DH9" s="25"/>
+      <c r="DI9" s="25"/>
+      <c r="DJ9" s="25"/>
+      <c r="DK9" s="25"/>
+      <c r="DL9" s="25"/>
+      <c r="DM9" s="25"/>
+      <c r="DN9" s="25"/>
+      <c r="DO9" s="25"/>
+      <c r="DP9" s="25"/>
+      <c r="DQ9" s="25"/>
+      <c r="DR9" s="25"/>
+      <c r="DS9" s="25"/>
+      <c r="DT9" s="25"/>
+      <c r="DU9" s="25"/>
+      <c r="DV9" s="25"/>
+      <c r="DW9" s="25"/>
+      <c r="DX9" s="25"/>
+      <c r="DY9" s="25"/>
+      <c r="DZ9" s="25"/>
+      <c r="EA9" s="25"/>
+      <c r="EB9" s="25"/>
+      <c r="EC9" s="25"/>
+      <c r="ED9" s="25"/>
+      <c r="EE9" s="25"/>
+      <c r="EF9" s="25"/>
+      <c r="EG9" s="25"/>
+      <c r="EH9" s="25"/>
+      <c r="EI9" s="25"/>
+      <c r="EJ9" s="25"/>
+      <c r="EK9" s="25"/>
+      <c r="EL9" s="25"/>
+      <c r="EM9" s="25"/>
+      <c r="EN9" s="25"/>
+      <c r="EO9" s="25"/>
+      <c r="EP9" s="25"/>
+      <c r="EQ9" s="25"/>
+      <c r="ER9" s="25"/>
+      <c r="ES9" s="25"/>
+      <c r="ET9" s="25"/>
+      <c r="EU9" s="25"/>
+      <c r="EV9" s="25"/>
+      <c r="EW9" s="25"/>
+      <c r="EX9" s="25"/>
+      <c r="EY9" s="25"/>
+      <c r="EZ9" s="25"/>
+      <c r="FA9" s="25"/>
+      <c r="FB9" s="25"/>
+      <c r="FC9" s="25"/>
+      <c r="FD9" s="25"/>
+      <c r="FE9" s="25"/>
+      <c r="FF9" s="25"/>
+      <c r="FG9" s="25"/>
+      <c r="FH9" s="25"/>
+      <c r="FI9" s="25"/>
+      <c r="FJ9" s="25"/>
+      <c r="FK9" s="25"/>
+      <c r="FL9" s="25"/>
+      <c r="FM9" s="25"/>
+      <c r="FN9" s="25"/>
+      <c r="FO9" s="25"/>
+      <c r="FP9" s="25"/>
+      <c r="FQ9" s="25"/>
+      <c r="FR9" s="25"/>
+      <c r="FS9" s="25"/>
+      <c r="FT9" s="25"/>
+      <c r="FU9" s="25"/>
+      <c r="FV9" s="25"/>
+      <c r="FW9" s="25"/>
+      <c r="FX9" s="25"/>
+      <c r="FY9" s="25"/>
+      <c r="FZ9" s="25"/>
+      <c r="GA9" s="25"/>
+      <c r="GB9" s="25"/>
+      <c r="GC9" s="25"/>
+      <c r="GD9" s="25"/>
+      <c r="GE9" s="25"/>
+      <c r="GF9" s="25"/>
+      <c r="GG9" s="25"/>
+      <c r="GH9" s="25"/>
+    </row>
+    <row r="10" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="41" t="s">
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="H10" s="32">
+      <c r="H10" s="10">
         <v>8</v>
       </c>
-      <c r="I10" s="34" t="s">
+      <c r="I10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="42" t="s">
+      <c r="J10" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="K10" s="36" t="s">
+      <c r="K10" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="33" t="s">
+      <c r="L10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="37" t="s">
+      <c r="M10" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="N10" s="37"/>
-      <c r="O10" s="32" t="s">
+      <c r="N10" s="15"/>
+      <c r="O10" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="P10" s="32" t="s">
+      <c r="P10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="38">
+      <c r="Q10" s="16">
         <v>6</v>
       </c>
-      <c r="R10" s="39" t="s">
+      <c r="R10" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S10" s="38" t="s">
+      <c r="S10" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="T10" s="40" t="s">
+      <c r="T10" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="U10" s="38" t="s">
+      <c r="U10" s="16" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="11" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="s">
+    <row r="11" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="41" t="s">
+      <c r="E11" s="9"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="H11" s="32">
+      <c r="H11" s="10">
         <v>9</v>
       </c>
-      <c r="I11" s="34" t="s">
+      <c r="I11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="42" t="s">
+      <c r="J11" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="K11" s="36" t="s">
+      <c r="K11" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="33" t="s">
+      <c r="L11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="37"/>
-      <c r="N11" s="37" t="s">
+      <c r="M11" s="15"/>
+      <c r="N11" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="O11" s="32" t="s">
+      <c r="O11" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="P11" s="32" t="s">
+      <c r="P11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="38">
+      <c r="Q11" s="16">
         <v>6</v>
       </c>
-      <c r="R11" s="39" t="s">
+      <c r="R11" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S11" s="38" t="s">
+      <c r="S11" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T11" s="40" t="s">
+      <c r="T11" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="U11" s="38" t="s">
+      <c r="U11" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="27" t="s">
+    <row r="12" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="41" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="H12" s="32">
+      <c r="H12" s="10">
         <v>10</v>
       </c>
-      <c r="I12" s="34" t="s">
+      <c r="I12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="42" t="s">
+      <c r="J12" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="K12" s="36" t="s">
+      <c r="K12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="33" t="s">
+      <c r="L12" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M12" s="37"/>
-      <c r="N12" s="37" t="s">
+      <c r="M12" s="15"/>
+      <c r="N12" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="O12" s="32" t="s">
+      <c r="O12" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="P12" s="32" t="s">
+      <c r="P12" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="38">
+      <c r="Q12" s="16">
         <v>6</v>
       </c>
-      <c r="R12" s="39" t="s">
+      <c r="R12" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S12" s="38" t="s">
+      <c r="S12" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T12" s="40" t="s">
+      <c r="T12" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="U12" s="38" t="s">
+      <c r="U12" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="13" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="27" t="s">
+    <row r="13" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="41" t="s">
+      <c r="E13" s="9"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="H13" s="32">
+      <c r="H13" s="10">
         <v>11</v>
       </c>
-      <c r="I13" s="34" t="s">
+      <c r="I13" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="42" t="s">
+      <c r="J13" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="K13" s="36" t="s">
+      <c r="K13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="33" t="s">
+      <c r="L13" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="37" t="s">
+      <c r="M13" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="N13" s="37"/>
-      <c r="O13" s="32" t="s">
+      <c r="N13" s="15"/>
+      <c r="O13" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="P13" s="32" t="s">
+      <c r="P13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q13" s="38">
+      <c r="Q13" s="16">
         <v>6</v>
       </c>
-      <c r="R13" s="39" t="s">
+      <c r="R13" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S13" s="38" t="s">
+      <c r="S13" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="T13" s="40" t="s">
+      <c r="T13" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="U13" s="38" t="s">
+      <c r="U13" s="16" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="14" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="27" t="s">
+    <row r="14" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="41" t="s">
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="H14" s="32">
+      <c r="H14" s="10">
         <v>12</v>
       </c>
-      <c r="I14" s="34" t="s">
+      <c r="I14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="42" t="s">
+      <c r="J14" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="K14" s="36" t="s">
+      <c r="K14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="33" t="s">
+      <c r="L14" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="37"/>
-      <c r="N14" s="37" t="s">
+      <c r="M14" s="15"/>
+      <c r="N14" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="O14" s="32" t="s">
+      <c r="O14" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="P14" s="32" t="s">
+      <c r="P14" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="38">
+      <c r="Q14" s="16">
         <v>6</v>
       </c>
-      <c r="R14" s="39" t="s">
+      <c r="R14" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S14" s="38" t="s">
+      <c r="S14" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T14" s="40" t="s">
+      <c r="T14" s="18" t="s">
         <v>237</v>
       </c>
-      <c r="U14" s="38" t="s">
+      <c r="U14" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="15" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="27" t="s">
+    <row r="15" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="41" t="s">
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="H15" s="32">
+      <c r="H15" s="10">
         <v>13</v>
       </c>
-      <c r="I15" s="34" t="s">
+      <c r="I15" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="42" t="s">
+      <c r="J15" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="K15" s="36" t="s">
+      <c r="K15" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="33" t="s">
+      <c r="L15" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="37"/>
-      <c r="N15" s="37" t="s">
+      <c r="M15" s="15"/>
+      <c r="N15" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="O15" s="32" t="s">
+      <c r="O15" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="P15" s="32" t="s">
+      <c r="P15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="38">
+      <c r="Q15" s="16">
         <v>6</v>
       </c>
-      <c r="R15" s="39" t="s">
+      <c r="R15" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S15" s="38" t="s">
+      <c r="S15" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T15" s="40" t="s">
+      <c r="T15" s="18" t="s">
         <v>239</v>
       </c>
-      <c r="U15" s="38" t="s">
+      <c r="U15" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="16" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="27" t="s">
+    <row r="16" spans="1:190" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="41" t="s">
+      <c r="E16" s="9"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="H16" s="32">
+      <c r="H16" s="10">
         <v>14</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="I16" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="42" t="s">
+      <c r="J16" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="K16" s="36" t="s">
+      <c r="K16" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="33" t="s">
+      <c r="L16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M16" s="37"/>
-      <c r="N16" s="37" t="s">
+      <c r="M16" s="15"/>
+      <c r="N16" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="O16" s="32" t="s">
+      <c r="O16" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="P16" s="32" t="s">
+      <c r="P16" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="38">
+      <c r="Q16" s="16">
         <v>6</v>
       </c>
-      <c r="R16" s="39" t="s">
+      <c r="R16" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S16" s="38" t="s">
+      <c r="S16" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T16" s="40" t="s">
+      <c r="T16" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="U16" s="38" t="s">
+      <c r="U16" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="s">
+    <row r="17" spans="1:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="41" t="s">
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="10">
         <v>15</v>
       </c>
-      <c r="I17" s="34" t="s">
+      <c r="I17" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="42" t="s">
+      <c r="J17" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="K17" s="36" t="s">
+      <c r="K17" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="33" t="s">
+      <c r="L17" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="37"/>
-      <c r="N17" s="37" t="s">
+      <c r="M17" s="15"/>
+      <c r="N17" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="O17" s="32" t="s">
+      <c r="O17" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="P17" s="32" t="s">
+      <c r="P17" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q17" s="38">
+      <c r="Q17" s="16">
         <v>6</v>
       </c>
-      <c r="R17" s="39" t="s">
+      <c r="R17" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S17" s="38" t="s">
+      <c r="S17" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T17" s="40" t="s">
+      <c r="T17" s="18" t="s">
         <v>125</v>
       </c>
-      <c r="U17" s="38" t="s">
+      <c r="U17" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="18" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="27" t="s">
+    <row r="18" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E18" s="31"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="41" t="s">
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="H18" s="32">
+      <c r="H18" s="10">
         <v>16</v>
       </c>
-      <c r="I18" s="34" t="s">
+      <c r="I18" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="42" t="s">
+      <c r="J18" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="K18" s="36" t="s">
+      <c r="K18" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="33" t="s">
+      <c r="L18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M18" s="37"/>
-      <c r="N18" s="37" t="s">
+      <c r="M18" s="15"/>
+      <c r="N18" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="O18" s="32" t="s">
+      <c r="O18" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="P18" s="32" t="s">
+      <c r="P18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="38">
+      <c r="Q18" s="16">
         <v>6</v>
       </c>
-      <c r="R18" s="39" t="s">
+      <c r="R18" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S18" s="38" t="s">
+      <c r="S18" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T18" s="40" t="s">
+      <c r="T18" s="18" t="s">
         <v>240</v>
       </c>
-      <c r="U18" s="38" t="s">
+      <c r="U18" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
+    <row r="19" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="E19" s="31" t="s">
+      <c r="E19" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="F19" s="32"/>
-      <c r="G19" s="41" t="s">
+      <c r="F19" s="10"/>
+      <c r="G19" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="H19" s="32">
+      <c r="H19" s="10">
         <v>17</v>
       </c>
-      <c r="I19" s="34" t="s">
+      <c r="I19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="42" t="s">
+      <c r="J19" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="K19" s="36" t="s">
+      <c r="K19" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L19" s="33" t="s">
+      <c r="L19" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="37"/>
-      <c r="N19" s="37" t="s">
+      <c r="M19" s="15"/>
+      <c r="N19" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="O19" s="32" t="s">
+      <c r="O19" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="P19" s="32" t="s">
+      <c r="P19" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="38">
+      <c r="Q19" s="16">
         <v>6</v>
       </c>
-      <c r="R19" s="39" t="s">
+      <c r="R19" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S19" s="38" t="s">
+      <c r="S19" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T19" s="40" t="s">
+      <c r="T19" s="18" t="s">
         <v>241</v>
       </c>
-      <c r="U19" s="38" t="s">
+      <c r="U19" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="27" t="s">
+    <row r="20" spans="1:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="E20" s="31"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="41" t="s">
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="H20" s="32">
+      <c r="H20" s="10">
         <v>18</v>
       </c>
-      <c r="I20" s="34" t="s">
+      <c r="I20" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="42" t="s">
+      <c r="J20" s="20" t="s">
         <v>186</v>
       </c>
-      <c r="K20" s="36" t="s">
+      <c r="K20" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L20" s="33" t="s">
+      <c r="L20" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="37"/>
-      <c r="N20" s="37" t="s">
+      <c r="M20" s="15"/>
+      <c r="N20" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="O20" s="32" t="s">
+      <c r="O20" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="P20" s="32" t="s">
+      <c r="P20" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="38">
+      <c r="Q20" s="16">
         <v>6</v>
       </c>
-      <c r="R20" s="39" t="s">
+      <c r="R20" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S20" s="38" t="s">
+      <c r="S20" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T20" s="40" t="s">
+      <c r="T20" s="18" t="s">
         <v>238</v>
       </c>
-      <c r="U20" s="38" t="s">
+      <c r="U20" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="21" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="27" t="s">
+    <row r="21" spans="1:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="E21" s="31"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="41" t="s">
+      <c r="E21" s="9"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="H21" s="32">
+      <c r="H21" s="10">
         <v>19</v>
       </c>
-      <c r="I21" s="34" t="s">
+      <c r="I21" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="42" t="s">
+      <c r="J21" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="K21" s="36" t="s">
+      <c r="K21" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L21" s="33" t="s">
+      <c r="L21" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M21" s="37"/>
-      <c r="N21" s="37" t="s">
+      <c r="M21" s="15"/>
+      <c r="N21" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="O21" s="32" t="s">
+      <c r="O21" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="P21" s="32" t="s">
+      <c r="P21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q21" s="38">
+      <c r="Q21" s="16">
         <v>6</v>
       </c>
-      <c r="R21" s="39" t="s">
+      <c r="R21" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S21" s="38" t="s">
+      <c r="S21" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T21" s="40" t="s">
+      <c r="T21" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="U21" s="38" t="s">
+      <c r="U21" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="27" t="s">
+    <row r="22" spans="1:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="E22" s="31"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="41" t="s">
+      <c r="E22" s="9"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="H22" s="32">
+      <c r="H22" s="10">
         <v>20</v>
       </c>
-      <c r="I22" s="34" t="s">
+      <c r="I22" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="46" t="s">
+      <c r="J22" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="K22" s="36" t="s">
+      <c r="K22" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L22" s="33" t="s">
+      <c r="L22" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37" t="s">
+      <c r="M22" s="15"/>
+      <c r="N22" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="O22" s="32" t="s">
+      <c r="O22" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="P22" s="32" t="s">
+      <c r="P22" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="38">
+      <c r="Q22" s="16">
         <v>6</v>
       </c>
-      <c r="R22" s="39" t="s">
+      <c r="R22" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S22" s="38" t="s">
+      <c r="S22" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T22" s="40" t="s">
+      <c r="T22" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="U22" s="38" t="s">
+      <c r="U22" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="27" t="s">
+    <row r="23" spans="1:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="E23" s="31"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="41" t="s">
+      <c r="E23" s="9"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="H23" s="32">
+      <c r="H23" s="10">
         <v>21</v>
       </c>
-      <c r="I23" s="34" t="s">
+      <c r="I23" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="42" t="s">
+      <c r="J23" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="K23" s="36" t="s">
+      <c r="K23" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="33" t="s">
+      <c r="L23" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M23" s="37"/>
-      <c r="N23" s="37" t="s">
+      <c r="M23" s="15"/>
+      <c r="N23" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="O23" s="32" t="s">
+      <c r="O23" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="P23" s="32" t="s">
+      <c r="P23" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="38">
+      <c r="Q23" s="16">
         <v>6</v>
       </c>
-      <c r="R23" s="39" t="s">
+      <c r="R23" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S23" s="38" t="s">
+      <c r="S23" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T23" s="40" t="s">
+      <c r="T23" s="18" t="s">
         <v>242</v>
       </c>
-      <c r="U23" s="38" t="s">
+      <c r="U23" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="27" t="s">
+    <row r="24" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="E24" s="31"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="41" t="s">
+      <c r="E24" s="9"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="H24" s="32">
+      <c r="H24" s="10">
         <v>22</v>
       </c>
-      <c r="I24" s="34" t="s">
+      <c r="I24" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="42" t="s">
+      <c r="J24" s="20" t="s">
         <v>190</v>
       </c>
-      <c r="K24" s="36" t="s">
+      <c r="K24" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L24" s="33" t="s">
+      <c r="L24" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37" t="s">
+      <c r="M24" s="15"/>
+      <c r="N24" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="O24" s="32" t="s">
+      <c r="O24" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="P24" s="32" t="s">
+      <c r="P24" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="38">
+      <c r="Q24" s="16">
         <v>6</v>
       </c>
-      <c r="R24" s="39" t="s">
+      <c r="R24" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S24" s="38" t="s">
+      <c r="S24" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T24" s="40" t="s">
+      <c r="T24" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="U24" s="38" t="s">
+      <c r="U24" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="27" t="s">
+    <row r="25" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D25" s="30" t="s">
+      <c r="D25" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="E25" s="31"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="41" t="s">
+      <c r="E25" s="9"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="H25" s="32">
+      <c r="H25" s="10">
         <v>23</v>
       </c>
-      <c r="I25" s="34" t="s">
+      <c r="I25" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="46" t="s">
+      <c r="J25" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="K25" s="36" t="s">
+      <c r="K25" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L25" s="33" t="s">
+      <c r="L25" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="M25" s="37" t="s">
+      <c r="M25" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="N25" s="37"/>
-      <c r="O25" s="32" t="s">
+      <c r="N25" s="15"/>
+      <c r="O25" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="P25" s="32" t="s">
+      <c r="P25" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q25" s="38">
+      <c r="Q25" s="16">
         <v>6</v>
       </c>
-      <c r="R25" s="39" t="s">
+      <c r="R25" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S25" s="38" t="s">
+      <c r="S25" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="T25" s="40" t="s">
+      <c r="T25" s="18" t="s">
         <v>236</v>
       </c>
-      <c r="U25" s="38" t="s">
+      <c r="U25" s="16" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="27" t="s">
+    <row r="26" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D26" s="30" t="s">
+      <c r="D26" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="E26" s="31" t="s">
+      <c r="E26" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="F26" s="32"/>
-      <c r="G26" s="41" t="s">
+      <c r="F26" s="10"/>
+      <c r="G26" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="H26" s="32">
+      <c r="H26" s="10">
         <v>24</v>
       </c>
-      <c r="I26" s="34" t="s">
+      <c r="I26" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="42" t="s">
+      <c r="J26" s="20" t="s">
         <v>224</v>
       </c>
-      <c r="K26" s="36" t="s">
+      <c r="K26" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="33" t="s">
+      <c r="L26" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M26" s="37"/>
-      <c r="N26" s="37" t="s">
+      <c r="M26" s="15"/>
+      <c r="N26" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="O26" s="32" t="s">
+      <c r="O26" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="P26" s="32" t="s">
+      <c r="P26" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="38">
+      <c r="Q26" s="16">
         <v>6</v>
       </c>
-      <c r="R26" s="39" t="s">
+      <c r="R26" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S26" s="38" t="s">
+      <c r="S26" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T26" s="40" t="s">
+      <c r="T26" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="U26" s="38" t="s">
+      <c r="U26" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="27" t="s">
+    <row r="27" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D27" s="30" t="s">
+      <c r="D27" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="E27" s="31"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="41" t="s">
+      <c r="E27" s="9"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="H27" s="32">
+      <c r="H27" s="10">
         <v>25</v>
       </c>
-      <c r="I27" s="34" t="s">
+      <c r="I27" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="42" t="s">
+      <c r="J27" s="20" t="s">
         <v>222</v>
       </c>
-      <c r="K27" s="36" t="s">
+      <c r="K27" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L27" s="33" t="s">
+      <c r="L27" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M27" s="37"/>
-      <c r="N27" s="37" t="s">
+      <c r="M27" s="15"/>
+      <c r="N27" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="O27" s="32" t="s">
+      <c r="O27" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="P27" s="32" t="s">
+      <c r="P27" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="38">
+      <c r="Q27" s="16">
         <v>6</v>
       </c>
-      <c r="R27" s="39" t="s">
+      <c r="R27" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S27" s="38" t="s">
+      <c r="S27" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T27" s="40" t="s">
+      <c r="T27" s="18" t="s">
         <v>243</v>
       </c>
-      <c r="U27" s="38" t="s">
+      <c r="U27" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="27" t="s">
+    <row r="28" spans="1:21" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="41" t="s">
+      <c r="E28" s="9"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="H28" s="32">
+      <c r="H28" s="10">
         <v>26</v>
       </c>
-      <c r="I28" s="34" t="s">
+      <c r="I28" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="42" t="s">
+      <c r="J28" s="20" t="s">
         <v>223</v>
       </c>
-      <c r="K28" s="36" t="s">
+      <c r="K28" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L28" s="33" t="s">
+      <c r="L28" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M28" s="37"/>
-      <c r="N28" s="37" t="s">
+      <c r="M28" s="15"/>
+      <c r="N28" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="O28" s="32" t="s">
+      <c r="O28" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="P28" s="32" t="s">
+      <c r="P28" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q28" s="38">
+      <c r="Q28" s="16">
         <v>6</v>
       </c>
-      <c r="R28" s="39" t="s">
+      <c r="R28" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S28" s="38" t="s">
+      <c r="S28" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T28" s="40" t="s">
+      <c r="T28" s="18" t="s">
         <v>244</v>
       </c>
-      <c r="U28" s="38" t="s">
+      <c r="U28" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="29" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="s">
+    <row r="29" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D29" s="30" t="s">
+      <c r="D29" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="41" t="s">
+      <c r="E29" s="9"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="H29" s="32">
+      <c r="H29" s="10">
         <v>27</v>
       </c>
-      <c r="I29" s="34" t="s">
+      <c r="I29" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="42" t="s">
+      <c r="J29" s="20" t="s">
         <v>192</v>
       </c>
-      <c r="K29" s="36" t="s">
+      <c r="K29" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L29" s="33" t="s">
+      <c r="L29" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="M29" s="37"/>
-      <c r="N29" s="37"/>
-      <c r="O29" s="32"/>
-      <c r="P29" s="32" t="s">
+      <c r="M29" s="15"/>
+      <c r="N29" s="15"/>
+      <c r="O29" s="10"/>
+      <c r="P29" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q29" s="49"/>
-      <c r="R29" s="50"/>
-      <c r="S29" s="49"/>
-      <c r="T29" s="51"/>
-      <c r="U29" s="49"/>
-    </row>
-    <row r="30" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="27" t="s">
+      <c r="Q29" s="27"/>
+      <c r="R29" s="28"/>
+      <c r="S29" s="27"/>
+      <c r="T29" s="29"/>
+      <c r="U29" s="27"/>
+    </row>
+    <row r="30" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="41" t="s">
+      <c r="E30" s="9"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="H30" s="32">
+      <c r="H30" s="10">
         <v>28</v>
       </c>
-      <c r="I30" s="34" t="s">
+      <c r="I30" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J30" s="42" t="s">
+      <c r="J30" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="K30" s="36" t="s">
+      <c r="K30" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L30" s="33" t="s">
+      <c r="L30" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M30" s="37"/>
-      <c r="N30" s="37" t="s">
+      <c r="M30" s="15"/>
+      <c r="N30" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="O30" s="32" t="s">
+      <c r="O30" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="P30" s="32" t="s">
+      <c r="P30" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="Q30" s="38">
+      <c r="Q30" s="16">
         <v>6</v>
       </c>
-      <c r="R30" s="39" t="s">
+      <c r="R30" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S30" s="38" t="s">
+      <c r="S30" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T30" s="40" t="s">
+      <c r="T30" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="U30" s="38" t="s">
+      <c r="U30" s="16" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="27" t="s">
+    <row r="31" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D31" s="30" t="s">
+      <c r="D31" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="E31" s="31"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="41" t="s">
+      <c r="E31" s="9"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="19" t="s">
         <v>247</v>
       </c>
-      <c r="H31" s="32">
+      <c r="H31" s="10">
         <v>29</v>
       </c>
-      <c r="I31" s="34" t="s">
+      <c r="I31" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J31" s="42" t="s">
+      <c r="J31" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="K31" s="36" t="s">
+      <c r="K31" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="L31" s="33" t="s">
+      <c r="L31" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="M31" s="37"/>
-      <c r="N31" s="37" t="s">
+      <c r="M31" s="15"/>
+      <c r="N31" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="O31" s="32"/>
-      <c r="P31" s="32" t="s">
+      <c r="O31" s="10"/>
+      <c r="P31" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="Q31" s="38">
+      <c r="Q31" s="16">
         <v>6</v>
       </c>
-      <c r="R31" s="39" t="s">
+      <c r="R31" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="S31" s="38" t="s">
+      <c r="S31" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="T31" s="40" t="s">
+      <c r="T31" s="18" t="s">
         <v>245</v>
       </c>
-      <c r="U31" s="38" t="s">
+      <c r="U31" s="16" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="27"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="32"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="36"/>
-      <c r="L32" s="33"/>
-      <c r="M32" s="37"/>
-      <c r="N32" s="37"/>
-      <c r="O32" s="32"/>
-      <c r="P32" s="32"/>
-      <c r="Q32" s="49"/>
-      <c r="R32" s="50"/>
-      <c r="S32" s="49"/>
-      <c r="T32" s="52"/>
-      <c r="U32" s="49"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="15"/>
+      <c r="O32" s="10"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="27"/>
+      <c r="R32" s="28"/>
+      <c r="S32" s="27"/>
+      <c r="T32" s="30"/>
+      <c r="U32" s="27"/>
     </row>
     <row r="33" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="27"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="32"/>
-      <c r="I33" s="34"/>
-      <c r="J33" s="42"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="33"/>
-      <c r="M33" s="37"/>
-      <c r="N33" s="37"/>
-      <c r="O33" s="32"/>
-      <c r="P33" s="32"/>
-      <c r="Q33" s="49"/>
-      <c r="R33" s="50"/>
-      <c r="S33" s="49"/>
-      <c r="T33" s="52"/>
-      <c r="U33" s="49"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="15"/>
+      <c r="N33" s="15"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+      <c r="Q33" s="27"/>
+      <c r="R33" s="28"/>
+      <c r="S33" s="27"/>
+      <c r="T33" s="30"/>
+      <c r="U33" s="27"/>
     </row>
     <row r="34" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="27"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="42"/>
-      <c r="K34" s="36"/>
-      <c r="L34" s="33"/>
-      <c r="M34" s="37"/>
-      <c r="N34" s="37"/>
-      <c r="O34" s="32"/>
-      <c r="P34" s="32"/>
-      <c r="Q34" s="49"/>
-      <c r="R34" s="50"/>
-      <c r="S34" s="49"/>
-      <c r="T34" s="52"/>
-      <c r="U34" s="49"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="10"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="27"/>
+      <c r="R34" s="28"/>
+      <c r="S34" s="27"/>
+      <c r="T34" s="30"/>
+      <c r="U34" s="27"/>
     </row>
     <row r="35" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="27"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="34"/>
-      <c r="J35" s="42"/>
-      <c r="K35" s="36"/>
-      <c r="L35" s="33"/>
-      <c r="M35" s="37"/>
-      <c r="N35" s="37"/>
-      <c r="O35" s="32"/>
-      <c r="P35" s="32"/>
-      <c r="Q35" s="49"/>
-      <c r="R35" s="50"/>
-      <c r="S35" s="49"/>
-      <c r="T35" s="52"/>
-      <c r="U35" s="49"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="8"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="15"/>
+      <c r="N35" s="15"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="27"/>
+      <c r="R35" s="28"/>
+      <c r="S35" s="27"/>
+      <c r="T35" s="30"/>
+      <c r="U35" s="27"/>
     </row>
     <row r="36" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="27"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="41"/>
-      <c r="H36" s="32"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="42"/>
-      <c r="K36" s="36"/>
-      <c r="L36" s="33"/>
-      <c r="M36" s="37"/>
-      <c r="N36" s="37"/>
-      <c r="O36" s="32"/>
-      <c r="P36" s="32"/>
-      <c r="Q36" s="49"/>
-      <c r="R36" s="50"/>
-      <c r="S36" s="49"/>
-      <c r="T36" s="52"/>
-      <c r="U36" s="49"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="15"/>
+      <c r="N36" s="15"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="10"/>
+      <c r="Q36" s="27"/>
+      <c r="R36" s="28"/>
+      <c r="S36" s="27"/>
+      <c r="T36" s="30"/>
+      <c r="U36" s="27"/>
     </row>
     <row r="37" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="27"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="42"/>
-      <c r="K37" s="36"/>
-      <c r="L37" s="33"/>
-      <c r="M37" s="37"/>
-      <c r="N37" s="37"/>
-      <c r="O37" s="32"/>
-      <c r="P37" s="32"/>
-      <c r="Q37" s="49"/>
-      <c r="R37" s="50"/>
-      <c r="S37" s="49"/>
-      <c r="T37" s="52"/>
-      <c r="U37" s="49"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="27"/>
+      <c r="R37" s="28"/>
+      <c r="S37" s="27"/>
+      <c r="T37" s="30"/>
+      <c r="U37" s="27"/>
     </row>
     <row r="38" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="27"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="29"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="41"/>
-      <c r="H38" s="32"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="42"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="33"/>
-      <c r="M38" s="37"/>
-      <c r="N38" s="37"/>
-      <c r="O38" s="32"/>
-      <c r="P38" s="32"/>
-      <c r="Q38" s="49"/>
-      <c r="R38" s="50"/>
-      <c r="S38" s="49"/>
-      <c r="T38" s="52"/>
-      <c r="U38" s="49"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="11"/>
+      <c r="M38" s="15"/>
+      <c r="N38" s="15"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="27"/>
+      <c r="R38" s="28"/>
+      <c r="S38" s="27"/>
+      <c r="T38" s="30"/>
+      <c r="U38" s="27"/>
     </row>
     <row r="39" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="27"/>
-      <c r="B39" s="28"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="32"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="42"/>
-      <c r="K39" s="36"/>
-      <c r="L39" s="33"/>
-      <c r="M39" s="37"/>
-      <c r="N39" s="37"/>
-      <c r="O39" s="32"/>
-      <c r="P39" s="32"/>
-      <c r="Q39" s="49"/>
-      <c r="R39" s="50"/>
-      <c r="S39" s="49"/>
-      <c r="T39" s="52"/>
-      <c r="U39" s="49"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="15"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="27"/>
+      <c r="R39" s="28"/>
+      <c r="S39" s="27"/>
+      <c r="T39" s="30"/>
+      <c r="U39" s="27"/>
     </row>
     <row r="54" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="16" t="s">
+      <c r="A54" s="3" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="16" t="s">
+      <c r="A55" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="3" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="16" t="s">
+      <c r="A57" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="16" t="s">
+      <c r="A58" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="16" t="s">
+      <c r="A59" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="3" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="16" t="s">
+      <c r="A61" s="3" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="16" t="s">
+      <c r="A62" s="3" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="16" t="s">
+      <c r="A63" s="3" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="3" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="16" t="s">
+      <c r="A65" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="16" t="s">
+      <c r="A66" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="16" t="s">
+      <c r="A67" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="16" t="s">
+      <c r="A68" s="3" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="16" t="s">
+      <c r="A69" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="16" t="s">
+      <c r="A70" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="16" t="s">
+      <c r="A71" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="16" t="s">
+      <c r="A72" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="16" t="s">
+      <c r="A73" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="16" t="s">
+      <c r="A74" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="16" t="s">
+      <c r="A75" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="16" t="s">
+      <c r="A76" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="16" t="s">
+      <c r="A77" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="16" t="s">
+      <c r="A78" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="16" t="s">
+      <c r="A79" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="16" t="s">
+      <c r="A80" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="16" t="s">
+      <c r="A81" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="16" t="s">
+      <c r="A82" s="3" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="16" t="s">
+      <c r="A83" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="16" t="s">
+      <c r="A84" s="3" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="16" t="s">
+      <c r="A85" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="16" t="s">
+      <c r="A86" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="16" t="s">
+      <c r="A87" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="16" t="s">
+      <c r="A88" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="16" t="s">
+      <c r="A89" s="3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="16" t="s">
+      <c r="A90" s="3" t="s">
         <v>115</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -3824,6 +3823,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Asignación de autores en greco Mat 8 tema 9
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EdgarJosué\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion09\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado08\guion09\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="256">
   <si>
     <t>Asignatura</t>
   </si>
@@ -783,6 +783,18 @@
   </si>
   <si>
     <t>Interactivo para abordar la construcción de cuadriláteros con regla y compás</t>
+  </si>
+  <si>
+    <t>Jeimmy</t>
+  </si>
+  <si>
+    <t>Diana Suárez</t>
+  </si>
+  <si>
+    <t>Adriana Lasprilla</t>
+  </si>
+  <si>
+    <t>Johanna Vera</t>
   </si>
 </sst>
 </file>
@@ -1145,21 +1157,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1170,6 +1167,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1209,6 +1212,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1517,9 +1529,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GH90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J27" sqref="J27"/>
+      <selection pane="bottomLeft" activeCell="G25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1549,94 +1561,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="G1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="58" t="s">
+      <c r="J1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="56" t="s">
+      <c r="K1" s="53" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="54" t="s">
+      <c r="L1" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="60" t="s">
+      <c r="M1" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="60"/>
-      <c r="O1" s="41" t="s">
+      <c r="N1" s="57"/>
+      <c r="O1" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="41" t="s">
+      <c r="P1" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="43" t="s">
+      <c r="Q1" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="45" t="s">
+      <c r="R1" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="43" t="s">
+      <c r="S1" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="44" t="s">
+      <c r="T1" s="61" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="43" t="s">
+      <c r="U1" s="60" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:190" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="62"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="55"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="52"/>
       <c r="M2" s="4" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="43"/>
-      <c r="R2" s="45"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="43"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="60"/>
     </row>
     <row r="3" spans="1:190" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -1696,6 +1708,9 @@
       <c r="U3" s="14" t="s">
         <v>200</v>
       </c>
+      <c r="V3" s="3" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="4" spans="1:190" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
@@ -1755,6 +1770,9 @@
       <c r="U4" s="14" t="s">
         <v>201</v>
       </c>
+      <c r="V4" s="3" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="5" spans="1:190" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -1814,6 +1832,9 @@
       <c r="U5" s="14" t="s">
         <v>201</v>
       </c>
+      <c r="V5" s="3" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="6" spans="1:190" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -1873,6 +1894,9 @@
       <c r="U6" s="14" t="s">
         <v>201</v>
       </c>
+      <c r="V6" s="3" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="7" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -1992,6 +2016,9 @@
       <c r="U8" s="14" t="s">
         <v>200</v>
       </c>
+      <c r="V8" s="3" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="9" spans="1:190" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
@@ -2051,7 +2078,9 @@
       <c r="U9" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="V9" s="7"/>
+      <c r="V9" s="7" t="s">
+        <v>252</v>
+      </c>
       <c r="W9" s="7"/>
       <c r="X9" s="7"/>
       <c r="Y9" s="7"/>
@@ -2279,6 +2308,9 @@
       <c r="U10" s="14" t="s">
         <v>207</v>
       </c>
+      <c r="V10" s="3" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="11" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
@@ -2338,6 +2370,9 @@
       <c r="U11" s="14" t="s">
         <v>201</v>
       </c>
+      <c r="V11" s="3" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="12" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
@@ -2397,6 +2432,9 @@
       <c r="U12" s="14" t="s">
         <v>201</v>
       </c>
+      <c r="V12" s="3" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="13" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
@@ -2456,6 +2494,9 @@
       <c r="U13" s="14" t="s">
         <v>207</v>
       </c>
+      <c r="V13" s="3" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="14" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
@@ -2515,6 +2556,9 @@
       <c r="U14" s="14" t="s">
         <v>201</v>
       </c>
+      <c r="V14" s="3" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="15" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
@@ -2574,6 +2618,9 @@
       <c r="U15" s="14" t="s">
         <v>201</v>
       </c>
+      <c r="V15" s="3" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="16" spans="1:190" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
@@ -2633,8 +2680,11 @@
       <c r="U16" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V16" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -2692,8 +2742,11 @@
       <c r="U17" s="36" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V17" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
@@ -2751,8 +2804,11 @@
       <c r="U18" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V18" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
@@ -2812,8 +2868,11 @@
       <c r="U19" s="14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V19" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>15</v>
       </c>
@@ -2871,8 +2930,11 @@
       <c r="U20" s="6" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V20" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>15</v>
       </c>
@@ -2930,8 +2992,11 @@
       <c r="U21" s="6" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V21" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>15</v>
       </c>
@@ -2989,8 +3054,11 @@
       <c r="U22" s="6" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V22" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>15</v>
       </c>
@@ -3048,8 +3116,11 @@
       <c r="U23" s="6" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="24" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V23" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>15</v>
       </c>
@@ -3107,8 +3178,11 @@
       <c r="U24" s="6" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="25" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V24" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>15</v>
       </c>
@@ -3166,8 +3240,11 @@
       <c r="U25" s="6" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V25" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>15</v>
       </c>
@@ -3227,8 +3304,11 @@
       <c r="U26" s="6" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V26" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="30" t="s">
         <v>15</v>
       </c>
@@ -3286,8 +3366,11 @@
       <c r="U27" s="33" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V27" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="30" t="s">
         <v>15</v>
       </c>
@@ -3345,8 +3428,11 @@
       <c r="U28" s="33" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V28" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="30" t="s">
         <v>15</v>
       </c>
@@ -3391,7 +3477,7 @@
       <c r="T29" s="35"/>
       <c r="U29" s="31"/>
     </row>
-    <row r="30" spans="1:21" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="30" t="s">
         <v>15</v>
       </c>
@@ -3449,8 +3535,11 @@
       <c r="U30" s="33" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V30" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="30" t="s">
         <v>15</v>
       </c>
@@ -3506,8 +3595,11 @@
       <c r="U31" s="33" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V31" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="23"/>
       <c r="B32" s="23"/>
       <c r="C32" s="23"/>
@@ -3909,6 +4001,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -3923,12 +4021,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambio de autores en recursos mat 8 tema 9
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="257">
   <si>
     <t>Asignatura</t>
   </si>
@@ -794,7 +794,10 @@
     <t>Adriana Lasprilla</t>
   </si>
   <si>
-    <t>Johanna Vera</t>
+    <t>Julián Martínez</t>
+  </si>
+  <si>
+    <t>Julián Martíne</t>
   </si>
 </sst>
 </file>
@@ -1157,6 +1160,21 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1167,12 +1185,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1212,15 +1224,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1529,9 +1532,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GH90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G25" sqref="A25:XFD25"/>
+      <selection pane="bottomLeft" activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1561,94 +1564,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="51" t="s">
+      <c r="G1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="55" t="s">
+      <c r="J1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="K1" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="L1" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="57" t="s">
+      <c r="M1" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="57"/>
-      <c r="O1" s="45" t="s">
+      <c r="N1" s="60"/>
+      <c r="O1" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="45" t="s">
+      <c r="P1" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="60" t="s">
+      <c r="Q1" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="62" t="s">
+      <c r="R1" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="60" t="s">
+      <c r="S1" s="43" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="61" t="s">
+      <c r="T1" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="60" t="s">
+      <c r="U1" s="43" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:190" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="52"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="59"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="55"/>
       <c r="M2" s="4" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="60"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="60"/>
-      <c r="T2" s="61"/>
-      <c r="U2" s="60"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="43"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="43"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="43"/>
     </row>
     <row r="3" spans="1:190" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -2495,7 +2498,7 @@
         <v>207</v>
       </c>
       <c r="V13" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3241,7 +3244,7 @@
         <v>207</v>
       </c>
       <c r="V25" s="3" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4001,12 +4004,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4021,6 +4018,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Recurso para subir en GRECO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="272">
   <si>
     <t>Asignatura</t>
   </si>
@@ -809,27 +809,15 @@
     <t>Duda sobre si se puede debido al tamaño</t>
   </si>
   <si>
-    <t>En proceso 3</t>
-  </si>
-  <si>
     <t>No se necesita</t>
   </si>
   <si>
     <t>Listos 1</t>
   </si>
   <si>
-    <t>Listos 6</t>
-  </si>
-  <si>
-    <t>Faltan 23</t>
-  </si>
-  <si>
     <t>Listos 3</t>
   </si>
   <si>
-    <t>faltan 23</t>
-  </si>
-  <si>
     <t>Reconoce las características de las líneas notables de un triángulo</t>
   </si>
   <si>
@@ -837,6 +825,24 @@
   </si>
   <si>
     <t>Faltan 26</t>
+  </si>
+  <si>
+    <t>Esperando imágenes</t>
+  </si>
+  <si>
+    <t>En proceso 4</t>
+  </si>
+  <si>
+    <t>faltan 22</t>
+  </si>
+  <si>
+    <t>Listos 7</t>
+  </si>
+  <si>
+    <t>Faltan 22</t>
+  </si>
+  <si>
+    <t>Recurso offLine, esperando imágenes</t>
   </si>
 </sst>
 </file>
@@ -1225,7 +1231,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1418,9 +1424,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1481,81 +1484,6 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1585,6 +1513,81 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1892,9 +1895,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GH90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V36" sqref="V36"/>
+      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1926,94 +1929,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="103" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="98" t="s">
+      <c r="B1" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="109" t="s">
+      <c r="C1" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="103" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="98" t="s">
+      <c r="E1" s="101" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="95" t="s">
+      <c r="F1" s="96" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="102" t="s">
+      <c r="G1" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="96" t="s">
+      <c r="H1" s="97" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="95" t="s">
+      <c r="I1" s="96" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="106" t="s">
+      <c r="J1" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="104" t="s">
+      <c r="K1" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="102" t="s">
+      <c r="L1" s="105" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="108" t="s">
+      <c r="M1" s="111" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="108"/>
-      <c r="O1" s="87" t="s">
+      <c r="N1" s="111"/>
+      <c r="O1" s="99" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="87" t="s">
+      <c r="P1" s="99" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="89" t="s">
+      <c r="Q1" s="115" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="93" t="s">
+      <c r="R1" s="119" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="89" t="s">
+      <c r="S1" s="115" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="91" t="s">
+      <c r="T1" s="117" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="89" t="s">
+      <c r="U1" s="115" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:190" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="101"/>
-      <c r="B2" s="99"/>
-      <c r="C2" s="110"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="99"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="97"/>
-      <c r="I2" s="96"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="103"/>
+      <c r="A2" s="104"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="106"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="110"/>
+      <c r="K2" s="108"/>
+      <c r="L2" s="106"/>
       <c r="M2" s="45" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="90"/>
-      <c r="R2" s="94"/>
-      <c r="S2" s="90"/>
-      <c r="T2" s="92"/>
-      <c r="U2" s="90"/>
+      <c r="O2" s="100"/>
+      <c r="P2" s="100"/>
+      <c r="Q2" s="116"/>
+      <c r="R2" s="120"/>
+      <c r="S2" s="116"/>
+      <c r="T2" s="118"/>
+      <c r="U2" s="116"/>
       <c r="V2" s="38" t="s">
         <v>256</v>
       </c>
@@ -2304,55 +2307,55 @@
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="43"/>
-      <c r="G7" s="112" t="s">
+      <c r="G7" s="86" t="s">
         <v>145</v>
       </c>
-      <c r="H7" s="113">
+      <c r="H7" s="87">
         <v>5</v>
       </c>
-      <c r="I7" s="114" t="s">
+      <c r="I7" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="113" t="s">
+      <c r="J7" s="87" t="s">
         <v>227</v>
       </c>
-      <c r="K7" s="115" t="s">
+      <c r="K7" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="114" t="s">
+      <c r="L7" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="114"/>
-      <c r="N7" s="114"/>
-      <c r="O7" s="113" t="s">
+      <c r="M7" s="88"/>
+      <c r="N7" s="88"/>
+      <c r="O7" s="87" t="s">
         <v>171</v>
       </c>
-      <c r="P7" s="113" t="s">
+      <c r="P7" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="116">
+      <c r="Q7" s="90">
         <v>9</v>
       </c>
-      <c r="R7" s="116" t="s">
+      <c r="R7" s="90" t="s">
         <v>128</v>
       </c>
-      <c r="S7" s="116" t="s">
+      <c r="S7" s="90" t="s">
         <v>220</v>
       </c>
-      <c r="T7" s="116" t="s">
+      <c r="T7" s="90" t="s">
         <v>221</v>
       </c>
-      <c r="U7" s="116" t="s">
+      <c r="U7" s="90" t="s">
         <v>222</v>
       </c>
       <c r="V7" s="60" t="s">
         <v>223</v>
       </c>
-      <c r="W7" s="118">
+      <c r="W7" s="92">
         <v>42416</v>
       </c>
       <c r="X7" s="65" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2434,55 +2437,61 @@
       </c>
       <c r="E9" s="18"/>
       <c r="F9" s="44"/>
-      <c r="G9" s="53" t="s">
+      <c r="G9" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="39">
         <v>7</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="I9" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="18" t="s">
+      <c r="J9" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="K9" s="19" t="s">
+      <c r="K9" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="19" t="s">
+      <c r="L9" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="19"/>
-      <c r="N9" s="19" t="s">
+      <c r="M9" s="40"/>
+      <c r="N9" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="O9" s="18" t="s">
+      <c r="O9" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="P9" s="18" t="s">
+      <c r="P9" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="32">
+      <c r="Q9" s="41">
         <v>6</v>
       </c>
-      <c r="R9" s="32" t="s">
+      <c r="R9" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="S9" s="32" t="s">
+      <c r="S9" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="T9" s="33" t="s">
+      <c r="T9" s="42" t="s">
         <v>125</v>
       </c>
-      <c r="U9" s="32" t="s">
+      <c r="U9" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="V9" s="32" t="s">
+      <c r="V9" s="60" t="s">
         <v>251</v>
       </c>
-      <c r="W9" s="32"/>
-      <c r="X9" s="66"/>
-      <c r="Y9" s="6"/>
+      <c r="W9" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="X9" s="64">
+        <v>42417</v>
+      </c>
+      <c r="Y9" s="6" t="s">
+        <v>271</v>
+      </c>
       <c r="Z9" s="6"/>
       <c r="AA9" s="6"/>
       <c r="AB9" s="6"/>
@@ -2728,57 +2737,57 @@
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="43"/>
-      <c r="G11" s="119" t="s">
-        <v>267</v>
-      </c>
-      <c r="H11" s="113">
+      <c r="G11" s="93" t="s">
+        <v>263</v>
+      </c>
+      <c r="H11" s="87">
         <v>9</v>
       </c>
-      <c r="I11" s="114" t="s">
+      <c r="I11" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="113" t="s">
+      <c r="J11" s="87" t="s">
         <v>231</v>
       </c>
-      <c r="K11" s="114" t="s">
+      <c r="K11" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="114" t="s">
+      <c r="L11" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="114"/>
-      <c r="N11" s="114" t="s">
+      <c r="M11" s="88"/>
+      <c r="N11" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="O11" s="120" t="s">
+      <c r="O11" s="94" t="s">
         <v>218</v>
       </c>
-      <c r="P11" s="113" t="s">
+      <c r="P11" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="117">
+      <c r="Q11" s="91">
         <v>6</v>
       </c>
-      <c r="R11" s="117" t="s">
+      <c r="R11" s="91" t="s">
         <v>123</v>
       </c>
-      <c r="S11" s="117" t="s">
+      <c r="S11" s="91" t="s">
         <v>124</v>
       </c>
-      <c r="T11" s="121" t="s">
+      <c r="T11" s="95" t="s">
         <v>210</v>
       </c>
-      <c r="U11" s="117" t="s">
+      <c r="U11" s="91" t="s">
         <v>200</v>
       </c>
       <c r="V11" s="60" t="s">
         <v>251</v>
       </c>
-      <c r="W11" s="118">
+      <c r="W11" s="92">
         <v>42416</v>
       </c>
       <c r="X11" s="65" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3289,11 +3298,11 @@
       <c r="U19" s="57" t="s">
         <v>200</v>
       </c>
-      <c r="V19" s="67" t="s">
+      <c r="V19" s="66" t="s">
         <v>252</v>
       </c>
-      <c r="W19" s="67"/>
-      <c r="X19" s="68"/>
+      <c r="W19" s="66"/>
+      <c r="X19" s="67"/>
     </row>
     <row r="20" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
@@ -3309,48 +3318,48 @@
         <v>193</v>
       </c>
       <c r="E20" s="8"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="73" t="s">
+      <c r="F20" s="68"/>
+      <c r="G20" s="72" t="s">
         <v>240</v>
       </c>
-      <c r="H20" s="74">
+      <c r="H20" s="73">
         <v>18</v>
       </c>
-      <c r="I20" s="75" t="s">
+      <c r="I20" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="74" t="s">
+      <c r="J20" s="73" t="s">
         <v>241</v>
       </c>
-      <c r="K20" s="75" t="s">
+      <c r="K20" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="L20" s="75" t="s">
+      <c r="L20" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="75"/>
-      <c r="N20" s="75" t="s">
+      <c r="M20" s="74"/>
+      <c r="N20" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="O20" s="74" t="s">
+      <c r="O20" s="73" t="s">
         <v>183</v>
       </c>
-      <c r="P20" s="74" t="s">
+      <c r="P20" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="76">
+      <c r="Q20" s="75">
         <v>6</v>
       </c>
-      <c r="R20" s="76" t="s">
+      <c r="R20" s="75" t="s">
         <v>123</v>
       </c>
-      <c r="S20" s="76" t="s">
+      <c r="S20" s="75" t="s">
         <v>124</v>
       </c>
-      <c r="T20" s="77" t="s">
+      <c r="T20" s="76" t="s">
         <v>210</v>
       </c>
-      <c r="U20" s="76" t="s">
+      <c r="U20" s="75" t="s">
         <v>200</v>
       </c>
       <c r="V20" s="62" t="s">
@@ -3373,8 +3382,8 @@
         <v>193</v>
       </c>
       <c r="E21" s="8"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="78" t="s">
+      <c r="F21" s="68"/>
+      <c r="G21" s="77" t="s">
         <v>154</v>
       </c>
       <c r="H21" s="35">
@@ -3437,8 +3446,8 @@
         <v>193</v>
       </c>
       <c r="E22" s="8"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="78" t="s">
+      <c r="F22" s="68"/>
+      <c r="G22" s="77" t="s">
         <v>242</v>
       </c>
       <c r="H22" s="35">
@@ -3501,8 +3510,8 @@
         <v>193</v>
       </c>
       <c r="E23" s="8"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="78" t="s">
+      <c r="F23" s="68"/>
+      <c r="G23" s="77" t="s">
         <v>155</v>
       </c>
       <c r="H23" s="35">
@@ -3565,8 +3574,8 @@
         <v>193</v>
       </c>
       <c r="E24" s="8"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="78" t="s">
+      <c r="F24" s="68"/>
+      <c r="G24" s="77" t="s">
         <v>249</v>
       </c>
       <c r="H24" s="35">
@@ -3629,8 +3638,8 @@
         <v>193</v>
       </c>
       <c r="E25" s="8"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="78" t="s">
+      <c r="F25" s="68"/>
+      <c r="G25" s="77" t="s">
         <v>156</v>
       </c>
       <c r="H25" s="35">
@@ -3695,55 +3704,55 @@
       <c r="E26" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="F26" s="69"/>
-      <c r="G26" s="79" t="s">
+      <c r="F26" s="68"/>
+      <c r="G26" s="78" t="s">
         <v>157</v>
       </c>
-      <c r="H26" s="80">
+      <c r="H26" s="79">
         <v>24</v>
       </c>
-      <c r="I26" s="81" t="s">
+      <c r="I26" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="80" t="s">
+      <c r="J26" s="79" t="s">
         <v>196</v>
       </c>
-      <c r="K26" s="81" t="s">
+      <c r="K26" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="81" t="s">
+      <c r="L26" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="M26" s="81"/>
-      <c r="N26" s="81" t="s">
+      <c r="M26" s="80"/>
+      <c r="N26" s="80" t="s">
         <v>121</v>
       </c>
-      <c r="O26" s="80" t="s">
+      <c r="O26" s="79" t="s">
         <v>189</v>
       </c>
-      <c r="P26" s="80" t="s">
+      <c r="P26" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="82">
+      <c r="Q26" s="81">
         <v>6</v>
       </c>
-      <c r="R26" s="82" t="s">
+      <c r="R26" s="81" t="s">
         <v>123</v>
       </c>
-      <c r="S26" s="82" t="s">
+      <c r="S26" s="81" t="s">
         <v>124</v>
       </c>
-      <c r="T26" s="83" t="s">
+      <c r="T26" s="82" t="s">
         <v>136</v>
       </c>
-      <c r="U26" s="82" t="s">
+      <c r="U26" s="81" t="s">
         <v>200</v>
       </c>
-      <c r="V26" s="67" t="s">
+      <c r="V26" s="66" t="s">
         <v>252</v>
       </c>
-      <c r="W26" s="67"/>
-      <c r="X26" s="68"/>
+      <c r="W26" s="66"/>
+      <c r="X26" s="67"/>
     </row>
     <row r="27" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="27" t="s">
@@ -3760,16 +3769,16 @@
       </c>
       <c r="E27" s="28"/>
       <c r="F27" s="28"/>
-      <c r="G27" s="70" t="s">
+      <c r="G27" s="69" t="s">
         <v>245</v>
       </c>
-      <c r="H27" s="70">
+      <c r="H27" s="69">
         <v>25</v>
       </c>
       <c r="I27" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="70" t="s">
+      <c r="J27" s="69" t="s">
         <v>195</v>
       </c>
       <c r="K27" s="27" t="s">
@@ -3782,25 +3791,25 @@
       <c r="N27" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="O27" s="70" t="s">
+      <c r="O27" s="69" t="s">
         <v>190</v>
       </c>
-      <c r="P27" s="70" t="s">
+      <c r="P27" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="71">
+      <c r="Q27" s="70">
         <v>6</v>
       </c>
-      <c r="R27" s="71" t="s">
+      <c r="R27" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="S27" s="71" t="s">
+      <c r="S27" s="70" t="s">
         <v>124</v>
       </c>
-      <c r="T27" s="72" t="s">
+      <c r="T27" s="71" t="s">
         <v>215</v>
       </c>
-      <c r="U27" s="71" t="s">
+      <c r="U27" s="70" t="s">
         <v>200</v>
       </c>
       <c r="V27" s="61" t="s">
@@ -3888,39 +3897,39 @@
       </c>
       <c r="E29" s="28"/>
       <c r="F29" s="28"/>
-      <c r="G29" s="84" t="s">
+      <c r="G29" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="H29" s="84">
+      <c r="H29" s="83">
         <v>27</v>
       </c>
-      <c r="I29" s="85" t="s">
+      <c r="I29" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="84" t="s">
+      <c r="J29" s="83" t="s">
         <v>247</v>
       </c>
-      <c r="K29" s="85" t="s">
+      <c r="K29" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="L29" s="85" t="s">
+      <c r="L29" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="M29" s="85"/>
-      <c r="N29" s="85"/>
-      <c r="O29" s="84"/>
-      <c r="P29" s="84" t="s">
+      <c r="M29" s="84"/>
+      <c r="N29" s="84"/>
+      <c r="O29" s="83"/>
+      <c r="P29" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="Q29" s="84"/>
-      <c r="R29" s="84"/>
-      <c r="S29" s="84"/>
-      <c r="T29" s="86"/>
-      <c r="U29" s="84"/>
+      <c r="Q29" s="83"/>
+      <c r="R29" s="83"/>
+      <c r="S29" s="83"/>
+      <c r="T29" s="85"/>
+      <c r="U29" s="83"/>
       <c r="V29" s="60"/>
       <c r="W29" s="60"/>
       <c r="X29" s="59" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="30" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4096,10 +4105,10 @@
       <c r="U33" s="24"/>
       <c r="V33" s="25"/>
       <c r="W33" s="3" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="X33" s="3" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
     </row>
     <row r="34" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4125,13 +4134,13 @@
       <c r="T34" s="24"/>
       <c r="U34" s="24"/>
       <c r="V34" s="25" t="s">
-        <v>263</v>
+        <v>269</v>
       </c>
       <c r="W34" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="X34" s="3" t="s">
         <v>262</v>
-      </c>
-      <c r="X34" s="3" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4157,13 +4166,13 @@
       <c r="T35" s="24"/>
       <c r="U35" s="24"/>
       <c r="V35" s="25" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="W35" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="X35" s="3" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="36" spans="1:24" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4473,6 +4482,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4487,12 +4502,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambio de motor en recurso MA_08_09_CO_REC120
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="273">
   <si>
     <t>Asignatura</t>
   </si>
@@ -474,9 +474,6 @@
   </si>
   <si>
     <t xml:space="preserve">Los criterios de congruencia en triángulos </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Completa la demostración de congruencia de triángulos </t>
   </si>
   <si>
     <t xml:space="preserve">Analiza demostraciones </t>
@@ -830,19 +827,25 @@
     <t>Esperando imágenes</t>
   </si>
   <si>
-    <t>En proceso 4</t>
-  </si>
-  <si>
-    <t>faltan 22</t>
-  </si>
-  <si>
-    <t>Listos 7</t>
-  </si>
-  <si>
-    <t>Faltan 22</t>
-  </si>
-  <si>
     <t>Recurso offLine, esperando imágenes</t>
+  </si>
+  <si>
+    <t>Ordena la demostración de congruencia de triángulos</t>
+  </si>
+  <si>
+    <t>Se debe cambiar motor, recurso off-line enviado a Oliver</t>
+  </si>
+  <si>
+    <t>Listos 8</t>
+  </si>
+  <si>
+    <t>Faltan 21</t>
+  </si>
+  <si>
+    <t>En proceso 5</t>
+  </si>
+  <si>
+    <t>faltan 21</t>
   </si>
 </sst>
 </file>
@@ -1514,6 +1517,30 @@
     <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1523,12 +1550,6 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1569,24 +1590,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1895,9 +1898,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GH90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomLeft" activeCell="W35" sqref="W35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1929,102 +1932,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="101" t="s">
+      <c r="B1" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="112" t="s">
+      <c r="C1" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="103" t="s">
+      <c r="D1" s="109" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="101" t="s">
+      <c r="E1" s="107" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="96" t="s">
+      <c r="F1" s="104" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="105" t="s">
+      <c r="G1" s="111" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="97" t="s">
+      <c r="H1" s="105" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="96" t="s">
+      <c r="I1" s="104" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="109" t="s">
+      <c r="J1" s="115" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="107" t="s">
+      <c r="K1" s="113" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="105" t="s">
+      <c r="L1" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="111" t="s">
+      <c r="M1" s="117" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="111"/>
-      <c r="O1" s="99" t="s">
+      <c r="N1" s="117"/>
+      <c r="O1" s="96" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="99" t="s">
+      <c r="P1" s="96" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="115" t="s">
+      <c r="Q1" s="98" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="119" t="s">
+      <c r="R1" s="102" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="115" t="s">
+      <c r="S1" s="98" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="117" t="s">
+      <c r="T1" s="100" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="115" t="s">
+      <c r="U1" s="98" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:190" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="104"/>
-      <c r="B2" s="102"/>
-      <c r="C2" s="113"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="114"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="97"/>
-      <c r="J2" s="110"/>
-      <c r="K2" s="108"/>
-      <c r="L2" s="106"/>
+      <c r="A2" s="110"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="119"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="106"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="114"/>
+      <c r="L2" s="112"/>
       <c r="M2" s="45" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="100"/>
-      <c r="P2" s="100"/>
-      <c r="Q2" s="116"/>
-      <c r="R2" s="120"/>
-      <c r="S2" s="116"/>
-      <c r="T2" s="118"/>
-      <c r="U2" s="116"/>
+      <c r="O2" s="97"/>
+      <c r="P2" s="97"/>
+      <c r="Q2" s="99"/>
+      <c r="R2" s="103"/>
+      <c r="S2" s="99"/>
+      <c r="T2" s="101"/>
+      <c r="U2" s="99"/>
       <c r="V2" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="W2" s="36" t="s">
         <v>256</v>
       </c>
-      <c r="W2" s="36" t="s">
+      <c r="X2" s="37" t="s">
         <v>257</v>
-      </c>
-      <c r="X2" s="37" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:190" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -2043,7 +2046,7 @@
       <c r="E3" s="11"/>
       <c r="F3" s="43"/>
       <c r="G3" s="46" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="H3" s="47">
         <v>1</v>
@@ -2052,7 +2055,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K3" s="48" t="s">
         <v>20</v>
@@ -2065,7 +2068,7 @@
       </c>
       <c r="N3" s="48"/>
       <c r="O3" s="47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P3" s="47" t="s">
         <v>19</v>
@@ -2080,13 +2083,13 @@
         <v>131</v>
       </c>
       <c r="T3" s="50" t="s">
+        <v>197</v>
+      </c>
+      <c r="U3" s="49" t="s">
         <v>198</v>
       </c>
-      <c r="U3" s="49" t="s">
-        <v>199</v>
-      </c>
       <c r="V3" s="62" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="W3" s="62"/>
       <c r="X3" s="63"/>
@@ -2107,7 +2110,7 @@
       <c r="E4" s="11"/>
       <c r="F4" s="43"/>
       <c r="G4" s="51" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H4" s="39">
         <v>2</v>
@@ -2116,7 +2119,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="39" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K4" s="40" t="s">
         <v>20</v>
@@ -2129,7 +2132,7 @@
         <v>29</v>
       </c>
       <c r="O4" s="39" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P4" s="39" t="s">
         <v>19</v>
@@ -2147,10 +2150,10 @@
         <v>134</v>
       </c>
       <c r="U4" s="41" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V4" s="60" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="W4" s="59"/>
       <c r="X4" s="64">
@@ -2182,7 +2185,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="39" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K5" s="40" t="s">
         <v>20</v>
@@ -2195,7 +2198,7 @@
         <v>37</v>
       </c>
       <c r="O5" s="39" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P5" s="39" t="s">
         <v>19</v>
@@ -2210,13 +2213,13 @@
         <v>124</v>
       </c>
       <c r="T5" s="42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="U5" s="41" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V5" s="60" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W5" s="32"/>
       <c r="X5" s="64">
@@ -2248,7 +2251,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="39" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K6" s="40" t="s">
         <v>20</v>
@@ -2261,7 +2264,7 @@
         <v>29</v>
       </c>
       <c r="O6" s="39" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P6" s="39" t="s">
         <v>19</v>
@@ -2279,17 +2282,17 @@
         <v>135</v>
       </c>
       <c r="U6" s="41" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V6" s="60" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="W6" s="32"/>
       <c r="X6" s="64">
         <v>42416</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2317,7 +2320,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="87" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K7" s="89" t="s">
         <v>19</v>
@@ -2328,7 +2331,7 @@
       <c r="M7" s="88"/>
       <c r="N7" s="88"/>
       <c r="O7" s="87" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="P7" s="87" t="s">
         <v>19</v>
@@ -2340,22 +2343,22 @@
         <v>128</v>
       </c>
       <c r="S7" s="90" t="s">
+        <v>219</v>
+      </c>
+      <c r="T7" s="90" t="s">
         <v>220</v>
       </c>
-      <c r="T7" s="90" t="s">
+      <c r="U7" s="90" t="s">
         <v>221</v>
       </c>
-      <c r="U7" s="90" t="s">
+      <c r="V7" s="60" t="s">
         <v>222</v>
-      </c>
-      <c r="V7" s="60" t="s">
-        <v>223</v>
       </c>
       <c r="W7" s="92">
         <v>42416</v>
       </c>
       <c r="X7" s="65" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2383,7 +2386,7 @@
         <v>19</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K8" s="34" t="s">
         <v>20</v>
@@ -2396,7 +2399,7 @@
       </c>
       <c r="N8" s="34"/>
       <c r="O8" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P8" s="11" t="s">
         <v>19</v>
@@ -2414,10 +2417,10 @@
         <v>132</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="V8" s="59" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="W8" s="59"/>
       <c r="X8" s="65"/>
@@ -2447,7 +2450,7 @@
         <v>20</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K9" s="40" t="s">
         <v>20</v>
@@ -2460,7 +2463,7 @@
         <v>120</v>
       </c>
       <c r="O9" s="39" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="P9" s="39" t="s">
         <v>20</v>
@@ -2478,19 +2481,19 @@
         <v>125</v>
       </c>
       <c r="U9" s="41" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V9" s="60" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="W9" s="32" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="X9" s="64">
         <v>42417</v>
       </c>
       <c r="Y9" s="6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="Z9" s="6"/>
       <c r="AA9" s="6"/>
@@ -2674,7 +2677,7 @@
       <c r="E10" s="11"/>
       <c r="F10" s="43"/>
       <c r="G10" s="52" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="H10" s="11">
         <v>8</v>
@@ -2683,7 +2686,7 @@
         <v>19</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K10" s="34" t="s">
         <v>20</v>
@@ -2696,7 +2699,7 @@
       </c>
       <c r="N10" s="34"/>
       <c r="O10" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P10" s="11" t="s">
         <v>19</v>
@@ -2708,16 +2711,16 @@
         <v>123</v>
       </c>
       <c r="S10" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="T10" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="T10" s="13" t="s">
+      <c r="U10" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="U10" s="12" t="s">
-        <v>206</v>
-      </c>
       <c r="V10" s="59" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="W10" s="59"/>
       <c r="X10" s="65"/>
@@ -2738,7 +2741,7 @@
       <c r="E11" s="11"/>
       <c r="F11" s="43"/>
       <c r="G11" s="93" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H11" s="87">
         <v>9</v>
@@ -2747,7 +2750,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="87" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K11" s="88" t="s">
         <v>20</v>
@@ -2760,7 +2763,7 @@
         <v>27</v>
       </c>
       <c r="O11" s="94" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="P11" s="87" t="s">
         <v>19</v>
@@ -2775,19 +2778,19 @@
         <v>124</v>
       </c>
       <c r="T11" s="95" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="U11" s="91" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V11" s="60" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="W11" s="92">
         <v>42416</v>
       </c>
       <c r="X11" s="65" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="12" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2815,7 +2818,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K12" s="34" t="s">
         <v>20</v>
@@ -2828,7 +2831,7 @@
         <v>33</v>
       </c>
       <c r="O12" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P12" s="11" t="s">
         <v>19</v>
@@ -2846,10 +2849,10 @@
         <v>126</v>
       </c>
       <c r="U12" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V12" s="59" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W12" s="59"/>
       <c r="X12" s="65"/>
@@ -2879,7 +2882,7 @@
         <v>19</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K13" s="34" t="s">
         <v>20</v>
@@ -2892,7 +2895,7 @@
       </c>
       <c r="N13" s="34"/>
       <c r="O13" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P13" s="11" t="s">
         <v>19</v>
@@ -2904,16 +2907,16 @@
         <v>123</v>
       </c>
       <c r="S13" s="12" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T13" s="13" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="U13" s="12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="V13" s="59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="W13" s="59"/>
       <c r="X13" s="65"/>
@@ -2933,54 +2936,59 @@
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="43"/>
-      <c r="G14" s="52" t="s">
-        <v>150</v>
-      </c>
-      <c r="H14" s="11">
+      <c r="G14" s="51" t="s">
+        <v>267</v>
+      </c>
+      <c r="H14" s="39">
         <v>12</v>
       </c>
-      <c r="I14" s="34" t="s">
+      <c r="I14" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="K14" s="34" t="s">
+      <c r="J14" s="39" t="s">
+        <v>233</v>
+      </c>
+      <c r="K14" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="34" t="s">
+      <c r="L14" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="O14" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="P14" s="11" t="s">
+      <c r="M14" s="40"/>
+      <c r="N14" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="O14" s="39" t="s">
+        <v>176</v>
+      </c>
+      <c r="P14" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="12">
+      <c r="Q14" s="41">
         <v>6</v>
       </c>
-      <c r="R14" s="12" t="s">
+      <c r="R14" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="S14" s="12" t="s">
+      <c r="S14" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="T14" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="U14" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="V14" s="59" t="s">
-        <v>251</v>
+      <c r="T14" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="U14" s="41" t="s">
+        <v>199</v>
+      </c>
+      <c r="V14" s="60" t="s">
+        <v>250</v>
       </c>
       <c r="W14" s="59"/>
-      <c r="X14" s="65"/>
+      <c r="X14" s="64">
+        <v>42417</v>
+      </c>
+      <c r="Y14" s="3" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="15" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
@@ -2998,7 +3006,7 @@
       <c r="E15" s="11"/>
       <c r="F15" s="43"/>
       <c r="G15" s="52" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H15" s="11">
         <v>13</v>
@@ -3007,7 +3015,7 @@
         <v>20</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K15" s="34" t="s">
         <v>20</v>
@@ -3020,7 +3028,7 @@
         <v>48</v>
       </c>
       <c r="O15" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="P15" s="11" t="s">
         <v>19</v>
@@ -3035,13 +3043,13 @@
         <v>124</v>
       </c>
       <c r="T15" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="U15" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V15" s="59" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W15" s="59"/>
       <c r="X15" s="65"/>
@@ -3062,7 +3070,7 @@
       <c r="E16" s="11"/>
       <c r="F16" s="43"/>
       <c r="G16" s="52" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H16" s="11">
         <v>14</v>
@@ -3071,7 +3079,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K16" s="34" t="s">
         <v>20</v>
@@ -3084,7 +3092,7 @@
         <v>41</v>
       </c>
       <c r="O16" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P16" s="11" t="s">
         <v>19</v>
@@ -3102,10 +3110,10 @@
         <v>138</v>
       </c>
       <c r="U16" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V16" s="59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="W16" s="59"/>
       <c r="X16" s="65"/>
@@ -3126,7 +3134,7 @@
       <c r="E17" s="11"/>
       <c r="F17" s="43"/>
       <c r="G17" s="53" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H17" s="18">
         <v>15</v>
@@ -3135,7 +3143,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K17" s="19" t="s">
         <v>20</v>
@@ -3148,7 +3156,7 @@
         <v>120</v>
       </c>
       <c r="O17" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P17" s="18" t="s">
         <v>20</v>
@@ -3166,10 +3174,10 @@
         <v>125</v>
       </c>
       <c r="U17" s="32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V17" s="59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="W17" s="59"/>
       <c r="X17" s="65"/>
@@ -3190,7 +3198,7 @@
       <c r="E18" s="11"/>
       <c r="F18" s="43"/>
       <c r="G18" s="52" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H18" s="11">
         <v>16</v>
@@ -3199,7 +3207,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="11" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K18" s="34" t="s">
         <v>20</v>
@@ -3212,7 +3220,7 @@
         <v>39</v>
       </c>
       <c r="O18" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P18" s="11" t="s">
         <v>19</v>
@@ -3227,13 +3235,13 @@
         <v>124</v>
       </c>
       <c r="T18" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="U18" s="12" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V18" s="59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="W18" s="59"/>
       <c r="X18" s="65"/>
@@ -3256,7 +3264,7 @@
       </c>
       <c r="F19" s="43"/>
       <c r="G19" s="54" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H19" s="55">
         <v>17</v>
@@ -3265,7 +3273,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="55" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K19" s="56" t="s">
         <v>20</v>
@@ -3278,7 +3286,7 @@
         <v>121</v>
       </c>
       <c r="O19" s="55" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P19" s="55" t="s">
         <v>19</v>
@@ -3293,13 +3301,13 @@
         <v>124</v>
       </c>
       <c r="T19" s="58" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="U19" s="57" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V19" s="66" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W19" s="66"/>
       <c r="X19" s="67"/>
@@ -3315,12 +3323,12 @@
         <v>141</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="68"/>
       <c r="G20" s="72" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H20" s="73">
         <v>18</v>
@@ -3329,7 +3337,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="73" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K20" s="74" t="s">
         <v>20</v>
@@ -3342,7 +3350,7 @@
         <v>27</v>
       </c>
       <c r="O20" s="73" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="P20" s="73" t="s">
         <v>19</v>
@@ -3357,13 +3365,13 @@
         <v>124</v>
       </c>
       <c r="T20" s="76" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="U20" s="75" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V20" s="62" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W20" s="62"/>
       <c r="X20" s="63"/>
@@ -3379,12 +3387,12 @@
         <v>141</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="68"/>
       <c r="G21" s="77" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H21" s="35">
         <v>19</v>
@@ -3393,7 +3401,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K21" s="10" t="s">
         <v>20</v>
@@ -3406,7 +3414,7 @@
         <v>23</v>
       </c>
       <c r="O21" s="35" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="P21" s="35" t="s">
         <v>19</v>
@@ -3424,10 +3432,10 @@
         <v>133</v>
       </c>
       <c r="U21" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V21" s="59" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W21" s="59"/>
       <c r="X21" s="65"/>
@@ -3443,12 +3451,12 @@
         <v>141</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="68"/>
       <c r="G22" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H22" s="35">
         <v>20</v>
@@ -3457,7 +3465,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K22" s="10" t="s">
         <v>20</v>
@@ -3470,7 +3478,7 @@
         <v>29</v>
       </c>
       <c r="O22" s="35" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="P22" s="35" t="s">
         <v>19</v>
@@ -3485,13 +3493,13 @@
         <v>124</v>
       </c>
       <c r="T22" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="U22" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V22" s="59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="W22" s="59"/>
       <c r="X22" s="65"/>
@@ -3507,12 +3515,12 @@
         <v>141</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="68"/>
       <c r="G23" s="77" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H23" s="35">
         <v>21</v>
@@ -3521,7 +3529,7 @@
         <v>20</v>
       </c>
       <c r="J23" s="35" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K23" s="10" t="s">
         <v>20</v>
@@ -3534,7 +3542,7 @@
         <v>32</v>
       </c>
       <c r="O23" s="35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P23" s="35" t="s">
         <v>19</v>
@@ -3549,13 +3557,13 @@
         <v>124</v>
       </c>
       <c r="T23" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="U23" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V23" s="59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="W23" s="59"/>
       <c r="X23" s="65"/>
@@ -3571,12 +3579,12 @@
         <v>141</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="68"/>
       <c r="G24" s="77" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H24" s="35">
         <v>22</v>
@@ -3585,7 +3593,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K24" s="10" t="s">
         <v>20</v>
@@ -3598,7 +3606,7 @@
         <v>29</v>
       </c>
       <c r="O24" s="35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P24" s="35" t="s">
         <v>19</v>
@@ -3613,13 +3621,13 @@
         <v>124</v>
       </c>
       <c r="T24" s="15" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U24" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V24" s="59" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="W24" s="59"/>
       <c r="X24" s="65"/>
@@ -3635,12 +3643,12 @@
         <v>141</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="68"/>
       <c r="G25" s="77" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H25" s="35">
         <v>23</v>
@@ -3649,7 +3657,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K25" s="10" t="s">
         <v>20</v>
@@ -3662,7 +3670,7 @@
       </c>
       <c r="N25" s="10"/>
       <c r="O25" s="35" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="P25" s="35" t="s">
         <v>19</v>
@@ -3674,16 +3682,16 @@
         <v>123</v>
       </c>
       <c r="S25" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="T25" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="U25" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="V25" s="59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="W25" s="59"/>
       <c r="X25" s="65"/>
@@ -3699,14 +3707,14 @@
         <v>141</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>127</v>
       </c>
       <c r="F26" s="68"/>
       <c r="G26" s="78" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H26" s="79">
         <v>24</v>
@@ -3715,7 +3723,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="79" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K26" s="80" t="s">
         <v>20</v>
@@ -3728,7 +3736,7 @@
         <v>121</v>
       </c>
       <c r="O26" s="79" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P26" s="79" t="s">
         <v>19</v>
@@ -3746,10 +3754,10 @@
         <v>136</v>
       </c>
       <c r="U26" s="81" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V26" s="66" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W26" s="66"/>
       <c r="X26" s="67"/>
@@ -3765,12 +3773,12 @@
         <v>141</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E27" s="28"/>
       <c r="F27" s="28"/>
       <c r="G27" s="69" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H27" s="69">
         <v>25</v>
@@ -3779,7 +3787,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="69" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K27" s="27" t="s">
         <v>20</v>
@@ -3792,7 +3800,7 @@
         <v>120</v>
       </c>
       <c r="O27" s="69" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="P27" s="69" t="s">
         <v>19</v>
@@ -3807,13 +3815,13 @@
         <v>124</v>
       </c>
       <c r="T27" s="71" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="U27" s="70" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V27" s="61" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W27" s="61"/>
       <c r="X27" s="61"/>
@@ -3829,12 +3837,12 @@
         <v>141</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
       <c r="G28" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H28" s="28">
         <v>26</v>
@@ -3843,7 +3851,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="28" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K28" s="29" t="s">
         <v>20</v>
@@ -3856,7 +3864,7 @@
         <v>120</v>
       </c>
       <c r="O28" s="28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P28" s="28" t="s">
         <v>19</v>
@@ -3871,13 +3879,13 @@
         <v>124</v>
       </c>
       <c r="T28" s="31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="U28" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V28" s="59" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W28" s="59"/>
       <c r="X28" s="59"/>
@@ -3907,7 +3915,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="83" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K29" s="84" t="s">
         <v>20</v>
@@ -3929,7 +3937,7 @@
       <c r="V29" s="60"/>
       <c r="W29" s="60"/>
       <c r="X29" s="59" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3957,7 +3965,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K30" s="29" t="s">
         <v>20</v>
@@ -3988,10 +3996,10 @@
         <v>137</v>
       </c>
       <c r="U30" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V30" s="59" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W30" s="59"/>
       <c r="X30" s="59"/>
@@ -4007,12 +4015,12 @@
         <v>141</v>
       </c>
       <c r="D31" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E31" s="28"/>
       <c r="F31" s="28"/>
       <c r="G31" s="28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="H31" s="28">
         <v>29</v>
@@ -4021,7 +4029,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="28" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K31" s="29" t="s">
         <v>20</v>
@@ -4047,13 +4055,13 @@
         <v>124</v>
       </c>
       <c r="T31" s="31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="U31" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="V31" s="59" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="W31" s="59"/>
       <c r="X31" s="59"/>
@@ -4105,10 +4113,10 @@
       <c r="U33" s="24"/>
       <c r="V33" s="25"/>
       <c r="W33" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="X33" s="3" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
     </row>
     <row r="34" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4137,10 +4145,10 @@
         <v>269</v>
       </c>
       <c r="W34" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="X34" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="X34" s="3" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4169,10 +4177,10 @@
         <v>270</v>
       </c>
       <c r="W35" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="X35" s="3" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
     </row>
     <row r="36" spans="1:24" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4482,12 +4490,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4502,6 +4504,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Corrección de estilo guía didáctica MA_08_10_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="275">
   <si>
     <t>Asignatura</t>
   </si>
@@ -821,31 +821,37 @@
     <t>Esperando imágenes</t>
   </si>
   <si>
-    <t>Recurso offLine, esperando imágenes</t>
-  </si>
-  <si>
     <t>Ordena la demostración de congruencia de triángulos</t>
   </si>
   <si>
     <t>Se debe cambiar motor, recurso off-line enviado a Oliver</t>
   </si>
   <si>
-    <t>Listos 8</t>
-  </si>
-  <si>
-    <t>Faltan 21</t>
-  </si>
-  <si>
-    <t>En proceso 5</t>
-  </si>
-  <si>
-    <t>faltan 21</t>
-  </si>
-  <si>
     <t>En espera de solicitud gráfica.</t>
   </si>
   <si>
     <t>En proceso 0</t>
+  </si>
+  <si>
+    <t>Recurso regresado al autor</t>
+  </si>
+  <si>
+    <t>Recurso offLine, esperando imágenes, Pedro ya lo subio a GRECO</t>
+  </si>
+  <si>
+    <t>Listos 9</t>
+  </si>
+  <si>
+    <t>Faltan 20</t>
+  </si>
+  <si>
+    <t>En proceso 6</t>
+  </si>
+  <si>
+    <t>faltan 20</t>
+  </si>
+  <si>
+    <t>Regreso a la autora con comentarios 18/02/2016</t>
   </si>
 </sst>
 </file>
@@ -905,7 +911,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1005,6 +1011,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1234,7 +1252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1286,9 +1304,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1328,9 +1343,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1388,9 +1400,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1487,81 +1496,6 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1581,6 +1515,102 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1889,9 +1919,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GH90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W35" sqref="W35"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1899,9 +1929,9 @@
     <col min="1" max="1" width="12" style="3" customWidth="1"/>
     <col min="2" max="2" width="13.140625" style="3" customWidth="1"/>
     <col min="3" max="3" width="23" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" style="6" customWidth="1"/>
     <col min="7" max="7" width="55.85546875" style="3" customWidth="1"/>
     <col min="8" max="8" width="8" style="6" customWidth="1"/>
     <col min="9" max="9" width="5.5703125" style="6" customWidth="1"/>
@@ -1923,101 +1953,101 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="102" t="s">
+      <c r="C1" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="97" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="91" t="s">
+      <c r="E1" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="86" t="s">
+      <c r="F1" s="90" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="95" t="s">
+      <c r="G1" s="99" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="87" t="s">
+      <c r="H1" s="91" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="86" t="s">
+      <c r="I1" s="90" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="99" t="s">
+      <c r="J1" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="97" t="s">
+      <c r="K1" s="101" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="95" t="s">
+      <c r="L1" s="99" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="101" t="s">
+      <c r="M1" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="101"/>
-      <c r="O1" s="89" t="s">
+      <c r="N1" s="105"/>
+      <c r="O1" s="93" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="89" t="s">
+      <c r="P1" s="93" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="105" t="s">
+      <c r="Q1" s="109" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="109" t="s">
+      <c r="R1" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="105" t="s">
+      <c r="S1" s="109" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="107" t="s">
+      <c r="T1" s="111" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="105" t="s">
+      <c r="U1" s="109" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:190" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="94"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="96"/>
-      <c r="M2" s="45" t="s">
+      <c r="A2" s="98"/>
+      <c r="B2" s="96"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="N2" s="45" t="s">
+      <c r="N2" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="90"/>
-      <c r="P2" s="90"/>
-      <c r="Q2" s="106"/>
-      <c r="R2" s="110"/>
-      <c r="S2" s="106"/>
-      <c r="T2" s="108"/>
-      <c r="U2" s="106"/>
-      <c r="V2" s="38" t="s">
+      <c r="O2" s="94"/>
+      <c r="P2" s="94"/>
+      <c r="Q2" s="110"/>
+      <c r="R2" s="114"/>
+      <c r="S2" s="110"/>
+      <c r="T2" s="112"/>
+      <c r="U2" s="110"/>
+      <c r="V2" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="W2" s="36" t="s">
+      <c r="W2" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="X2" s="37" t="s">
+      <c r="X2" s="35" t="s">
         <v>257</v>
       </c>
     </row>
@@ -2035,55 +2065,55 @@
         <v>142</v>
       </c>
       <c r="E3" s="11"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="46" t="s">
+      <c r="F3" s="41"/>
+      <c r="G3" s="44" t="s">
         <v>223</v>
       </c>
-      <c r="H3" s="47">
+      <c r="H3" s="45">
         <v>1</v>
       </c>
-      <c r="I3" s="48" t="s">
+      <c r="I3" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="48" t="s">
+      <c r="J3" s="46" t="s">
         <v>224</v>
       </c>
-      <c r="K3" s="48" t="s">
+      <c r="K3" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="48" t="s">
+      <c r="L3" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="48" t="s">
+      <c r="M3" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="48"/>
-      <c r="O3" s="47" t="s">
+      <c r="N3" s="46"/>
+      <c r="O3" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="P3" s="47" t="s">
+      <c r="P3" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="49">
+      <c r="Q3" s="47">
         <v>6</v>
       </c>
-      <c r="R3" s="49" t="s">
+      <c r="R3" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="S3" s="49" t="s">
+      <c r="S3" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="T3" s="50" t="s">
+      <c r="T3" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="U3" s="49" t="s">
+      <c r="U3" s="47" t="s">
         <v>198</v>
       </c>
-      <c r="V3" s="62" t="s">
+      <c r="V3" s="59" t="s">
         <v>252</v>
       </c>
-      <c r="W3" s="62"/>
-      <c r="X3" s="63"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="60"/>
     </row>
     <row r="4" spans="1:190" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -2099,55 +2129,55 @@
         <v>142</v>
       </c>
       <c r="E4" s="11"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="51" t="s">
+      <c r="F4" s="41"/>
+      <c r="G4" s="49" t="s">
         <v>247</v>
       </c>
-      <c r="H4" s="39">
+      <c r="H4" s="37">
         <v>2</v>
       </c>
-      <c r="I4" s="40" t="s">
+      <c r="I4" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="39" t="s">
+      <c r="J4" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="K4" s="40" t="s">
+      <c r="K4" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="40" t="s">
+      <c r="L4" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40" t="s">
+      <c r="M4" s="38"/>
+      <c r="N4" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="39" t="s">
+      <c r="O4" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="P4" s="39" t="s">
+      <c r="P4" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="41">
+      <c r="Q4" s="39">
         <v>6</v>
       </c>
-      <c r="R4" s="41" t="s">
+      <c r="R4" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="S4" s="41" t="s">
+      <c r="S4" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="T4" s="42" t="s">
+      <c r="T4" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="U4" s="41" t="s">
+      <c r="U4" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="V4" s="60" t="s">
+      <c r="V4" s="57" t="s">
         <v>250</v>
       </c>
-      <c r="W4" s="59"/>
-      <c r="X4" s="64">
+      <c r="W4" s="56"/>
+      <c r="X4" s="61">
         <v>42416</v>
       </c>
     </row>
@@ -2165,55 +2195,55 @@
         <v>142</v>
       </c>
       <c r="E5" s="11"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="51" t="s">
+      <c r="F5" s="41"/>
+      <c r="G5" s="49" t="s">
         <v>143</v>
       </c>
-      <c r="H5" s="39">
+      <c r="H5" s="37">
         <v>3</v>
       </c>
-      <c r="I5" s="40" t="s">
+      <c r="I5" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="39" t="s">
+      <c r="J5" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="K5" s="40" t="s">
+      <c r="K5" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="40" t="s">
+      <c r="L5" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40" t="s">
+      <c r="M5" s="38"/>
+      <c r="N5" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="O5" s="39" t="s">
+      <c r="O5" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="P5" s="39" t="s">
+      <c r="P5" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="41">
+      <c r="Q5" s="39">
         <v>6</v>
       </c>
-      <c r="R5" s="41" t="s">
+      <c r="R5" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="S5" s="41" t="s">
+      <c r="S5" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="T5" s="42" t="s">
+      <c r="T5" s="40" t="s">
         <v>202</v>
       </c>
-      <c r="U5" s="41" t="s">
+      <c r="U5" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="V5" s="60" t="s">
+      <c r="V5" s="57" t="s">
         <v>251</v>
       </c>
-      <c r="W5" s="32"/>
-      <c r="X5" s="64">
+      <c r="W5" s="31"/>
+      <c r="X5" s="61">
         <v>42416</v>
       </c>
     </row>
@@ -2231,55 +2261,55 @@
         <v>142</v>
       </c>
       <c r="E6" s="11"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="51" t="s">
+      <c r="F6" s="41"/>
+      <c r="G6" s="49" t="s">
         <v>144</v>
       </c>
-      <c r="H6" s="39">
+      <c r="H6" s="37">
         <v>4</v>
       </c>
-      <c r="I6" s="40" t="s">
+      <c r="I6" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="39" t="s">
+      <c r="J6" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="K6" s="40" t="s">
+      <c r="K6" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="L6" s="40" t="s">
+      <c r="L6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="40"/>
-      <c r="N6" s="40" t="s">
+      <c r="M6" s="38"/>
+      <c r="N6" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="39" t="s">
+      <c r="O6" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="P6" s="39" t="s">
+      <c r="P6" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="41">
+      <c r="Q6" s="39">
         <v>6</v>
       </c>
-      <c r="R6" s="41" t="s">
+      <c r="R6" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="S6" s="41" t="s">
+      <c r="S6" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="T6" s="42" t="s">
+      <c r="T6" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="U6" s="41" t="s">
+      <c r="U6" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="V6" s="60" t="s">
+      <c r="V6" s="57" t="s">
         <v>250</v>
       </c>
-      <c r="W6" s="32"/>
-      <c r="X6" s="64">
+      <c r="W6" s="31"/>
+      <c r="X6" s="61">
         <v>42416</v>
       </c>
       <c r="Y6" s="3" t="s">
@@ -2300,55 +2330,55 @@
         <v>142</v>
       </c>
       <c r="E7" s="11"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="112" t="s">
+      <c r="F7" s="41"/>
+      <c r="G7" s="84" t="s">
         <v>145</v>
       </c>
-      <c r="H7" s="83">
+      <c r="H7" s="80">
         <v>5</v>
       </c>
-      <c r="I7" s="84" t="s">
+      <c r="I7" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="83" t="s">
+      <c r="J7" s="80" t="s">
         <v>226</v>
       </c>
-      <c r="K7" s="113" t="s">
+      <c r="K7" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="84" t="s">
+      <c r="L7" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="84"/>
-      <c r="N7" s="84"/>
-      <c r="O7" s="83" t="s">
+      <c r="M7" s="81"/>
+      <c r="N7" s="81"/>
+      <c r="O7" s="80" t="s">
         <v>170</v>
       </c>
-      <c r="P7" s="83" t="s">
+      <c r="P7" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="114">
+      <c r="Q7" s="86">
         <v>9</v>
       </c>
-      <c r="R7" s="114" t="s">
+      <c r="R7" s="86" t="s">
         <v>128</v>
       </c>
-      <c r="S7" s="114" t="s">
+      <c r="S7" s="86" t="s">
         <v>219</v>
       </c>
-      <c r="T7" s="114" t="s">
+      <c r="T7" s="86" t="s">
         <v>220</v>
       </c>
-      <c r="U7" s="114" t="s">
+      <c r="U7" s="86" t="s">
         <v>221</v>
       </c>
-      <c r="V7" s="60" t="s">
+      <c r="V7" s="57" t="s">
         <v>222</v>
       </c>
-      <c r="W7" s="111">
+      <c r="W7" s="83">
         <v>42416</v>
       </c>
-      <c r="X7" s="65" t="s">
+      <c r="X7" s="62" t="s">
         <v>259</v>
       </c>
     </row>
@@ -2366,29 +2396,29 @@
         <v>142</v>
       </c>
       <c r="E8" s="11"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="52" t="s">
+      <c r="F8" s="41"/>
+      <c r="G8" s="50" t="s">
         <v>146</v>
       </c>
       <c r="H8" s="11">
         <v>6</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="32" t="s">
         <v>19</v>
       </c>
       <c r="J8" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="K8" s="34" t="s">
+      <c r="K8" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="34" t="s">
+      <c r="L8" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="M8" s="34" t="s">
+      <c r="M8" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="N8" s="34"/>
+      <c r="N8" s="32"/>
       <c r="O8" s="11" t="s">
         <v>171</v>
       </c>
@@ -2410,11 +2440,11 @@
       <c r="U8" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="V8" s="59" t="s">
+      <c r="V8" s="56" t="s">
         <v>252</v>
       </c>
-      <c r="W8" s="59"/>
-      <c r="X8" s="65"/>
+      <c r="W8" s="56"/>
+      <c r="X8" s="62"/>
     </row>
     <row r="9" spans="1:190" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
@@ -2430,61 +2460,61 @@
         <v>142</v>
       </c>
       <c r="E9" s="18"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="51" t="s">
+      <c r="F9" s="42"/>
+      <c r="G9" s="49" t="s">
         <v>147</v>
       </c>
-      <c r="H9" s="39">
+      <c r="H9" s="37">
         <v>7</v>
       </c>
-      <c r="I9" s="40" t="s">
+      <c r="I9" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="J9" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="K9" s="40" t="s">
+      <c r="K9" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="40" t="s">
+      <c r="L9" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40" t="s">
+      <c r="M9" s="38"/>
+      <c r="N9" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="O9" s="39" t="s">
+      <c r="O9" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P9" s="39" t="s">
+      <c r="P9" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="41">
+      <c r="Q9" s="39">
         <v>6</v>
       </c>
-      <c r="R9" s="41" t="s">
+      <c r="R9" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="S9" s="41" t="s">
+      <c r="S9" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="T9" s="42" t="s">
+      <c r="T9" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="U9" s="41" t="s">
+      <c r="U9" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="V9" s="60" t="s">
+      <c r="V9" s="57" t="s">
         <v>250</v>
       </c>
-      <c r="W9" s="32" t="s">
+      <c r="W9" s="31" t="s">
         <v>263</v>
       </c>
-      <c r="X9" s="64">
+      <c r="X9" s="61">
         <v>42417</v>
       </c>
       <c r="Y9" s="6" t="s">
-        <v>264</v>
+        <v>269</v>
       </c>
       <c r="Z9" s="6"/>
       <c r="AA9" s="6"/>
@@ -2666,29 +2696,29 @@
         <v>142</v>
       </c>
       <c r="E10" s="11"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="52" t="s">
+      <c r="F10" s="41"/>
+      <c r="G10" s="50" t="s">
         <v>228</v>
       </c>
       <c r="H10" s="11">
         <v>8</v>
       </c>
-      <c r="I10" s="34" t="s">
+      <c r="I10" s="32" t="s">
         <v>19</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>229</v>
       </c>
-      <c r="K10" s="34" t="s">
+      <c r="K10" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="34" t="s">
+      <c r="L10" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="34" t="s">
+      <c r="M10" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="N10" s="34"/>
+      <c r="N10" s="32"/>
       <c r="O10" s="11" t="s">
         <v>173</v>
       </c>
@@ -2710,11 +2740,14 @@
       <c r="U10" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="V10" s="59" t="s">
+      <c r="V10" s="56" t="s">
         <v>253</v>
       </c>
-      <c r="W10" s="59"/>
-      <c r="X10" s="65"/>
+      <c r="W10" s="56"/>
+      <c r="X10" s="62"/>
+      <c r="Y10" s="3" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="11" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
@@ -2730,57 +2763,57 @@
         <v>142</v>
       </c>
       <c r="E11" s="11"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="115" t="s">
+      <c r="F11" s="41"/>
+      <c r="G11" s="87" t="s">
         <v>261</v>
       </c>
-      <c r="H11" s="83">
+      <c r="H11" s="80">
         <v>9</v>
       </c>
-      <c r="I11" s="84" t="s">
+      <c r="I11" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="83" t="s">
+      <c r="J11" s="80" t="s">
         <v>230</v>
       </c>
-      <c r="K11" s="84" t="s">
+      <c r="K11" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="84" t="s">
+      <c r="L11" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="84"/>
-      <c r="N11" s="84" t="s">
+      <c r="M11" s="81"/>
+      <c r="N11" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="O11" s="116" t="s">
+      <c r="O11" s="88" t="s">
         <v>217</v>
       </c>
-      <c r="P11" s="83" t="s">
+      <c r="P11" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="Q11" s="60">
+      <c r="Q11" s="57">
         <v>6</v>
       </c>
-      <c r="R11" s="60" t="s">
+      <c r="R11" s="57" t="s">
         <v>123</v>
       </c>
-      <c r="S11" s="60" t="s">
+      <c r="S11" s="57" t="s">
         <v>124</v>
       </c>
-      <c r="T11" s="117" t="s">
+      <c r="T11" s="89" t="s">
         <v>209</v>
       </c>
-      <c r="U11" s="60" t="s">
+      <c r="U11" s="57" t="s">
         <v>199</v>
       </c>
-      <c r="V11" s="60" t="s">
+      <c r="V11" s="57" t="s">
         <v>250</v>
       </c>
-      <c r="W11" s="111">
+      <c r="W11" s="83">
         <v>42416</v>
       </c>
-      <c r="X11" s="65" t="s">
+      <c r="X11" s="62" t="s">
         <v>259</v>
       </c>
     </row>
@@ -2798,57 +2831,59 @@
         <v>142</v>
       </c>
       <c r="E12" s="11"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="52" t="s">
+      <c r="F12" s="41"/>
+      <c r="G12" s="49" t="s">
         <v>148</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="37">
         <v>10</v>
       </c>
-      <c r="I12" s="34" t="s">
+      <c r="I12" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="J12" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="K12" s="34" t="s">
+      <c r="K12" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="34" t="s">
+      <c r="L12" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34" t="s">
+      <c r="M12" s="38"/>
+      <c r="N12" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="O12" s="11" t="s">
+      <c r="O12" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="P12" s="11" t="s">
+      <c r="P12" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" s="12">
+      <c r="Q12" s="39">
         <v>6</v>
       </c>
-      <c r="R12" s="12" t="s">
+      <c r="R12" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="S12" s="12" t="s">
+      <c r="S12" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="T12" s="13" t="s">
+      <c r="T12" s="40" t="s">
         <v>126</v>
       </c>
-      <c r="U12" s="12" t="s">
+      <c r="U12" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="V12" s="59" t="s">
+      <c r="V12" s="57" t="s">
         <v>251</v>
       </c>
-      <c r="W12" s="59"/>
-      <c r="X12" s="65"/>
+      <c r="W12" s="31"/>
+      <c r="X12" s="61">
+        <v>42418</v>
+      </c>
       <c r="Y12" s="3" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2865,29 +2900,29 @@
         <v>142</v>
       </c>
       <c r="E13" s="11"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="52" t="s">
+      <c r="F13" s="41"/>
+      <c r="G13" s="50" t="s">
         <v>149</v>
       </c>
       <c r="H13" s="11">
         <v>11</v>
       </c>
-      <c r="I13" s="34" t="s">
+      <c r="I13" s="32" t="s">
         <v>19</v>
       </c>
       <c r="J13" s="11" t="s">
         <v>232</v>
       </c>
-      <c r="K13" s="34" t="s">
+      <c r="K13" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="34" t="s">
+      <c r="L13" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="34" t="s">
+      <c r="M13" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="N13" s="34"/>
+      <c r="N13" s="32"/>
       <c r="O13" s="11" t="s">
         <v>175</v>
       </c>
@@ -2909,11 +2944,11 @@
       <c r="U13" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="V13" s="59" t="s">
+      <c r="V13" s="56" t="s">
         <v>254</v>
       </c>
-      <c r="W13" s="59"/>
-      <c r="X13" s="65"/>
+      <c r="W13" s="56"/>
+      <c r="X13" s="62"/>
     </row>
     <row r="14" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
@@ -2929,59 +2964,59 @@
         <v>142</v>
       </c>
       <c r="E14" s="11"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="51" t="s">
+      <c r="F14" s="41"/>
+      <c r="G14" s="49" t="s">
+        <v>264</v>
+      </c>
+      <c r="H14" s="37">
+        <v>12</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="K14" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="O14" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="P14" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q14" s="39">
+        <v>6</v>
+      </c>
+      <c r="R14" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="S14" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="T14" s="40" t="s">
+        <v>208</v>
+      </c>
+      <c r="U14" s="39" t="s">
+        <v>199</v>
+      </c>
+      <c r="V14" s="57" t="s">
+        <v>250</v>
+      </c>
+      <c r="W14" s="56"/>
+      <c r="X14" s="61">
+        <v>42417</v>
+      </c>
+      <c r="Y14" s="3" t="s">
         <v>265</v>
-      </c>
-      <c r="H14" s="39">
-        <v>12</v>
-      </c>
-      <c r="I14" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="39" t="s">
-        <v>233</v>
-      </c>
-      <c r="K14" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="L14" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="M14" s="40"/>
-      <c r="N14" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="O14" s="39" t="s">
-        <v>176</v>
-      </c>
-      <c r="P14" s="39" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q14" s="41">
-        <v>6</v>
-      </c>
-      <c r="R14" s="41" t="s">
-        <v>123</v>
-      </c>
-      <c r="S14" s="41" t="s">
-        <v>124</v>
-      </c>
-      <c r="T14" s="42" t="s">
-        <v>208</v>
-      </c>
-      <c r="U14" s="41" t="s">
-        <v>199</v>
-      </c>
-      <c r="V14" s="60" t="s">
-        <v>250</v>
-      </c>
-      <c r="W14" s="59"/>
-      <c r="X14" s="64">
-        <v>42417</v>
-      </c>
-      <c r="Y14" s="3" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="15" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2998,55 +3033,57 @@
         <v>142</v>
       </c>
       <c r="E15" s="11"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="52" t="s">
+      <c r="F15" s="41"/>
+      <c r="G15" s="49" t="s">
         <v>234</v>
       </c>
-      <c r="H15" s="11">
+      <c r="H15" s="37">
         <v>13</v>
       </c>
-      <c r="I15" s="34" t="s">
+      <c r="I15" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="11" t="s">
+      <c r="J15" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="K15" s="34" t="s">
+      <c r="K15" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="34" t="s">
+      <c r="L15" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34" t="s">
+      <c r="M15" s="38"/>
+      <c r="N15" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="O15" s="11" t="s">
+      <c r="O15" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="P15" s="11" t="s">
+      <c r="P15" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="Q15" s="12">
+      <c r="Q15" s="39">
         <v>6</v>
       </c>
-      <c r="R15" s="12" t="s">
+      <c r="R15" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="S15" s="12" t="s">
+      <c r="S15" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="T15" s="13" t="s">
+      <c r="T15" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="U15" s="12" t="s">
+      <c r="U15" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="V15" s="59" t="s">
+      <c r="V15" s="57" t="s">
         <v>251</v>
       </c>
-      <c r="W15" s="59"/>
-      <c r="X15" s="65"/>
+      <c r="W15" s="115"/>
+      <c r="X15" s="61">
+        <v>42418</v>
+      </c>
     </row>
     <row r="16" spans="1:190" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
@@ -3062,27 +3099,27 @@
         <v>142</v>
       </c>
       <c r="E16" s="11"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="52" t="s">
+      <c r="F16" s="41"/>
+      <c r="G16" s="50" t="s">
         <v>236</v>
       </c>
       <c r="H16" s="11">
         <v>14</v>
       </c>
-      <c r="I16" s="34" t="s">
+      <c r="I16" s="32" t="s">
         <v>20</v>
       </c>
       <c r="J16" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="K16" s="34" t="s">
+      <c r="K16" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="34" t="s">
+      <c r="L16" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34" t="s">
+      <c r="M16" s="32"/>
+      <c r="N16" s="32" t="s">
         <v>41</v>
       </c>
       <c r="O16" s="11" t="s">
@@ -3106,13 +3143,13 @@
       <c r="U16" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="V16" s="59" t="s">
+      <c r="V16" s="56" t="s">
         <v>250</v>
       </c>
-      <c r="W16" s="59"/>
-      <c r="X16" s="65"/>
-    </row>
-    <row r="17" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W16" s="56"/>
+      <c r="X16" s="62"/>
+    </row>
+    <row r="17" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -3126,57 +3163,60 @@
         <v>142</v>
       </c>
       <c r="E17" s="11"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="53" t="s">
+      <c r="F17" s="41"/>
+      <c r="G17" s="116" t="s">
         <v>150</v>
       </c>
-      <c r="H17" s="18">
+      <c r="H17" s="117">
         <v>15</v>
       </c>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="18" t="s">
+      <c r="J17" s="117" t="s">
         <v>161</v>
       </c>
-      <c r="K17" s="19" t="s">
+      <c r="K17" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="19" t="s">
+      <c r="L17" s="118" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19" t="s">
+      <c r="M17" s="118"/>
+      <c r="N17" s="118" t="s">
         <v>120</v>
       </c>
-      <c r="O17" s="18" t="s">
+      <c r="O17" s="117" t="s">
         <v>179</v>
       </c>
-      <c r="P17" s="18" t="s">
+      <c r="P17" s="117" t="s">
         <v>20</v>
       </c>
-      <c r="Q17" s="32">
+      <c r="Q17" s="119">
         <v>6</v>
       </c>
-      <c r="R17" s="32" t="s">
+      <c r="R17" s="119" t="s">
         <v>123</v>
       </c>
-      <c r="S17" s="32" t="s">
+      <c r="S17" s="119" t="s">
         <v>124</v>
       </c>
-      <c r="T17" s="33" t="s">
+      <c r="T17" s="120" t="s">
         <v>125</v>
       </c>
-      <c r="U17" s="32" t="s">
+      <c r="U17" s="119" t="s">
         <v>199</v>
       </c>
-      <c r="V17" s="59" t="s">
+      <c r="V17" s="119" t="s">
         <v>250</v>
       </c>
-      <c r="W17" s="59"/>
-      <c r="X17" s="65"/>
-    </row>
-    <row r="18" spans="1:24" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W17" s="119"/>
+      <c r="X17" s="121"/>
+      <c r="Y17" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>15</v>
       </c>
@@ -3190,27 +3230,27 @@
         <v>142</v>
       </c>
       <c r="E18" s="11"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="52" t="s">
+      <c r="F18" s="41"/>
+      <c r="G18" s="50" t="s">
         <v>151</v>
       </c>
       <c r="H18" s="11">
         <v>16</v>
       </c>
-      <c r="I18" s="34" t="s">
+      <c r="I18" s="32" t="s">
         <v>20</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="K18" s="34" t="s">
+      <c r="K18" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="34" t="s">
+      <c r="L18" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34" t="s">
+      <c r="M18" s="32"/>
+      <c r="N18" s="32" t="s">
         <v>39</v>
       </c>
       <c r="O18" s="11" t="s">
@@ -3234,13 +3274,13 @@
       <c r="U18" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="V18" s="59" t="s">
+      <c r="V18" s="56" t="s">
         <v>250</v>
       </c>
-      <c r="W18" s="59"/>
-      <c r="X18" s="65"/>
-    </row>
-    <row r="19" spans="1:24" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="W18" s="56"/>
+      <c r="X18" s="62"/>
+    </row>
+    <row r="19" spans="1:25" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>15</v>
       </c>
@@ -3256,57 +3296,57 @@
       <c r="E19" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="F19" s="43"/>
-      <c r="G19" s="54" t="s">
+      <c r="F19" s="41"/>
+      <c r="G19" s="51" t="s">
         <v>152</v>
       </c>
-      <c r="H19" s="55">
+      <c r="H19" s="52">
         <v>17</v>
       </c>
-      <c r="I19" s="56" t="s">
+      <c r="I19" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="55" t="s">
+      <c r="J19" s="52" t="s">
         <v>162</v>
       </c>
-      <c r="K19" s="56" t="s">
+      <c r="K19" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="L19" s="56" t="s">
+      <c r="L19" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="56"/>
-      <c r="N19" s="56" t="s">
+      <c r="M19" s="53"/>
+      <c r="N19" s="53" t="s">
         <v>121</v>
       </c>
-      <c r="O19" s="55" t="s">
+      <c r="O19" s="52" t="s">
         <v>181</v>
       </c>
-      <c r="P19" s="55" t="s">
+      <c r="P19" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="57">
+      <c r="Q19" s="54">
         <v>6</v>
       </c>
-      <c r="R19" s="57" t="s">
+      <c r="R19" s="54" t="s">
         <v>123</v>
       </c>
-      <c r="S19" s="57" t="s">
+      <c r="S19" s="54" t="s">
         <v>124</v>
       </c>
-      <c r="T19" s="58" t="s">
+      <c r="T19" s="55" t="s">
         <v>212</v>
       </c>
-      <c r="U19" s="57" t="s">
+      <c r="U19" s="54" t="s">
         <v>199</v>
       </c>
-      <c r="V19" s="66" t="s">
+      <c r="V19" s="63" t="s">
         <v>251</v>
       </c>
-      <c r="W19" s="66"/>
-      <c r="X19" s="67"/>
-    </row>
-    <row r="20" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W19" s="63"/>
+      <c r="X19" s="64"/>
+    </row>
+    <row r="20" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>15</v>
       </c>
@@ -3320,57 +3360,57 @@
         <v>192</v>
       </c>
       <c r="E20" s="8"/>
-      <c r="F20" s="68"/>
-      <c r="G20" s="72" t="s">
+      <c r="F20" s="65"/>
+      <c r="G20" s="69" t="s">
         <v>239</v>
       </c>
-      <c r="H20" s="73">
+      <c r="H20" s="70">
         <v>18</v>
       </c>
-      <c r="I20" s="74" t="s">
+      <c r="I20" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="73" t="s">
+      <c r="J20" s="70" t="s">
         <v>240</v>
       </c>
-      <c r="K20" s="74" t="s">
+      <c r="K20" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="L20" s="74" t="s">
+      <c r="L20" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="74"/>
-      <c r="N20" s="74" t="s">
+      <c r="M20" s="71"/>
+      <c r="N20" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="O20" s="73" t="s">
+      <c r="O20" s="70" t="s">
         <v>182</v>
       </c>
-      <c r="P20" s="73" t="s">
+      <c r="P20" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="75">
+      <c r="Q20" s="72">
         <v>6</v>
       </c>
-      <c r="R20" s="75" t="s">
+      <c r="R20" s="72" t="s">
         <v>123</v>
       </c>
-      <c r="S20" s="75" t="s">
+      <c r="S20" s="72" t="s">
         <v>124</v>
       </c>
-      <c r="T20" s="76" t="s">
+      <c r="T20" s="73" t="s">
         <v>209</v>
       </c>
-      <c r="U20" s="75" t="s">
+      <c r="U20" s="72" t="s">
         <v>199</v>
       </c>
-      <c r="V20" s="62" t="s">
+      <c r="V20" s="59" t="s">
         <v>251</v>
       </c>
-      <c r="W20" s="62"/>
-      <c r="X20" s="63"/>
-    </row>
-    <row r="21" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W20" s="59"/>
+      <c r="X20" s="60"/>
+    </row>
+    <row r="21" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>15</v>
       </c>
@@ -3384,17 +3424,17 @@
         <v>192</v>
       </c>
       <c r="E21" s="8"/>
-      <c r="F21" s="68"/>
-      <c r="G21" s="77" t="s">
+      <c r="F21" s="65"/>
+      <c r="G21" s="74" t="s">
         <v>153</v>
       </c>
-      <c r="H21" s="35">
+      <c r="H21" s="33">
         <v>19</v>
       </c>
       <c r="I21" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="35" t="s">
+      <c r="J21" s="33" t="s">
         <v>163</v>
       </c>
       <c r="K21" s="10" t="s">
@@ -3407,10 +3447,10 @@
       <c r="N21" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="O21" s="35" t="s">
+      <c r="O21" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="P21" s="35" t="s">
+      <c r="P21" s="33" t="s">
         <v>19</v>
       </c>
       <c r="Q21" s="5">
@@ -3428,13 +3468,13 @@
       <c r="U21" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="V21" s="59" t="s">
+      <c r="V21" s="56" t="s">
         <v>251</v>
       </c>
-      <c r="W21" s="59"/>
-      <c r="X21" s="65"/>
-    </row>
-    <row r="22" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W21" s="56"/>
+      <c r="X21" s="62"/>
+    </row>
+    <row r="22" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>15</v>
       </c>
@@ -3448,11 +3488,11 @@
         <v>192</v>
       </c>
       <c r="E22" s="8"/>
-      <c r="F22" s="68"/>
-      <c r="G22" s="77" t="s">
+      <c r="F22" s="65"/>
+      <c r="G22" s="74" t="s">
         <v>241</v>
       </c>
-      <c r="H22" s="35">
+      <c r="H22" s="33">
         <v>20</v>
       </c>
       <c r="I22" s="10" t="s">
@@ -3471,10 +3511,10 @@
       <c r="N22" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O22" s="35" t="s">
+      <c r="O22" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="P22" s="35" t="s">
+      <c r="P22" s="33" t="s">
         <v>19</v>
       </c>
       <c r="Q22" s="5">
@@ -3492,13 +3532,13 @@
       <c r="U22" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="V22" s="59" t="s">
+      <c r="V22" s="56" t="s">
         <v>250</v>
       </c>
-      <c r="W22" s="59"/>
-      <c r="X22" s="65"/>
-    </row>
-    <row r="23" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W22" s="56"/>
+      <c r="X22" s="62"/>
+    </row>
+    <row r="23" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>15</v>
       </c>
@@ -3512,17 +3552,17 @@
         <v>192</v>
       </c>
       <c r="E23" s="8"/>
-      <c r="F23" s="68"/>
-      <c r="G23" s="77" t="s">
+      <c r="F23" s="65"/>
+      <c r="G23" s="74" t="s">
         <v>154</v>
       </c>
-      <c r="H23" s="35">
+      <c r="H23" s="33">
         <v>21</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="35" t="s">
+      <c r="J23" s="33" t="s">
         <v>243</v>
       </c>
       <c r="K23" s="10" t="s">
@@ -3535,10 +3575,10 @@
       <c r="N23" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="O23" s="35" t="s">
+      <c r="O23" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="P23" s="35" t="s">
+      <c r="P23" s="33" t="s">
         <v>19</v>
       </c>
       <c r="Q23" s="5">
@@ -3556,13 +3596,13 @@
       <c r="U23" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="V23" s="59" t="s">
+      <c r="V23" s="56" t="s">
         <v>250</v>
       </c>
-      <c r="W23" s="59"/>
-      <c r="X23" s="65"/>
-    </row>
-    <row r="24" spans="1:24" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W23" s="56"/>
+      <c r="X23" s="62"/>
+    </row>
+    <row r="24" spans="1:25" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>15</v>
       </c>
@@ -3576,17 +3616,17 @@
         <v>192</v>
       </c>
       <c r="E24" s="8"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="77" t="s">
+      <c r="F24" s="65"/>
+      <c r="G24" s="74" t="s">
         <v>248</v>
       </c>
-      <c r="H24" s="35">
+      <c r="H24" s="33">
         <v>22</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="35" t="s">
+      <c r="J24" s="33" t="s">
         <v>164</v>
       </c>
       <c r="K24" s="10" t="s">
@@ -3599,10 +3639,10 @@
       <c r="N24" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="O24" s="35" t="s">
+      <c r="O24" s="33" t="s">
         <v>186</v>
       </c>
-      <c r="P24" s="35" t="s">
+      <c r="P24" s="33" t="s">
         <v>19</v>
       </c>
       <c r="Q24" s="5">
@@ -3620,13 +3660,13 @@
       <c r="U24" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="V24" s="59" t="s">
+      <c r="V24" s="56" t="s">
         <v>250</v>
       </c>
-      <c r="W24" s="59"/>
-      <c r="X24" s="65"/>
-    </row>
-    <row r="25" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="W24" s="56"/>
+      <c r="X24" s="62"/>
+    </row>
+    <row r="25" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>15</v>
       </c>
@@ -3640,11 +3680,11 @@
         <v>192</v>
       </c>
       <c r="E25" s="8"/>
-      <c r="F25" s="68"/>
-      <c r="G25" s="77" t="s">
+      <c r="F25" s="65"/>
+      <c r="G25" s="74" t="s">
         <v>155</v>
       </c>
-      <c r="H25" s="35">
+      <c r="H25" s="33">
         <v>23</v>
       </c>
       <c r="I25" s="10" t="s">
@@ -3663,10 +3703,10 @@
         <v>117</v>
       </c>
       <c r="N25" s="10"/>
-      <c r="O25" s="35" t="s">
+      <c r="O25" s="33" t="s">
         <v>187</v>
       </c>
-      <c r="P25" s="35" t="s">
+      <c r="P25" s="33" t="s">
         <v>19</v>
       </c>
       <c r="Q25" s="5">
@@ -3684,13 +3724,13 @@
       <c r="U25" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="V25" s="59" t="s">
+      <c r="V25" s="56" t="s">
         <v>254</v>
       </c>
-      <c r="W25" s="59"/>
-      <c r="X25" s="65"/>
-    </row>
-    <row r="26" spans="1:24" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="W25" s="56"/>
+      <c r="X25" s="62"/>
+    </row>
+    <row r="26" spans="1:25" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>15</v>
       </c>
@@ -3706,437 +3746,437 @@
       <c r="E26" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="F26" s="68"/>
-      <c r="G26" s="78" t="s">
+      <c r="F26" s="65"/>
+      <c r="G26" s="75" t="s">
         <v>156</v>
       </c>
-      <c r="H26" s="79">
+      <c r="H26" s="76">
         <v>24</v>
       </c>
-      <c r="I26" s="80" t="s">
+      <c r="I26" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="79" t="s">
+      <c r="J26" s="76" t="s">
         <v>195</v>
       </c>
-      <c r="K26" s="80" t="s">
+      <c r="K26" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="80" t="s">
+      <c r="L26" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="M26" s="80"/>
-      <c r="N26" s="80" t="s">
+      <c r="M26" s="77"/>
+      <c r="N26" s="77" t="s">
         <v>121</v>
       </c>
-      <c r="O26" s="79" t="s">
+      <c r="O26" s="76" t="s">
         <v>188</v>
       </c>
-      <c r="P26" s="79" t="s">
+      <c r="P26" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="81">
+      <c r="Q26" s="78">
         <v>6</v>
       </c>
-      <c r="R26" s="81" t="s">
+      <c r="R26" s="78" t="s">
         <v>123</v>
       </c>
-      <c r="S26" s="81" t="s">
+      <c r="S26" s="78" t="s">
         <v>124</v>
       </c>
-      <c r="T26" s="82" t="s">
+      <c r="T26" s="79" t="s">
         <v>136</v>
       </c>
-      <c r="U26" s="81" t="s">
+      <c r="U26" s="78" t="s">
         <v>199</v>
       </c>
-      <c r="V26" s="66" t="s">
+      <c r="V26" s="63" t="s">
         <v>251</v>
       </c>
-      <c r="W26" s="66"/>
-      <c r="X26" s="67"/>
-    </row>
-    <row r="27" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="27" t="s">
+      <c r="W26" s="63"/>
+      <c r="X26" s="64"/>
+    </row>
+    <row r="27" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="D27" s="28" t="s">
+      <c r="D27" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="69" t="s">
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="66" t="s">
         <v>244</v>
       </c>
-      <c r="H27" s="69">
+      <c r="H27" s="66">
         <v>25</v>
       </c>
-      <c r="I27" s="27" t="s">
+      <c r="I27" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="69" t="s">
+      <c r="J27" s="66" t="s">
         <v>194</v>
       </c>
-      <c r="K27" s="27" t="s">
+      <c r="K27" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="L27" s="27" t="s">
+      <c r="L27" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="M27" s="27"/>
-      <c r="N27" s="27" t="s">
+      <c r="M27" s="26"/>
+      <c r="N27" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="O27" s="69" t="s">
+      <c r="O27" s="66" t="s">
         <v>189</v>
       </c>
-      <c r="P27" s="69" t="s">
+      <c r="P27" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="70">
+      <c r="Q27" s="67">
         <v>6</v>
       </c>
-      <c r="R27" s="70" t="s">
+      <c r="R27" s="67" t="s">
         <v>123</v>
       </c>
-      <c r="S27" s="70" t="s">
+      <c r="S27" s="67" t="s">
         <v>124</v>
       </c>
-      <c r="T27" s="71" t="s">
+      <c r="T27" s="68" t="s">
         <v>214</v>
       </c>
-      <c r="U27" s="70" t="s">
+      <c r="U27" s="67" t="s">
         <v>199</v>
       </c>
-      <c r="V27" s="61" t="s">
+      <c r="V27" s="58" t="s">
         <v>251</v>
       </c>
-      <c r="W27" s="61"/>
-      <c r="X27" s="61"/>
-    </row>
-    <row r="28" spans="1:24" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="27" t="s">
+      <c r="W27" s="58"/>
+      <c r="X27" s="58"/>
+    </row>
+    <row r="28" spans="1:25" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="27" t="s">
         <v>193</v>
       </c>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28" t="s">
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="H28" s="28">
+      <c r="H28" s="27">
         <v>26</v>
       </c>
-      <c r="I28" s="29" t="s">
+      <c r="I28" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="28" t="s">
+      <c r="J28" s="27" t="s">
         <v>245</v>
       </c>
-      <c r="K28" s="29" t="s">
+      <c r="K28" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="L28" s="29" t="s">
+      <c r="L28" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29" t="s">
+      <c r="M28" s="28"/>
+      <c r="N28" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="O28" s="28" t="s">
+      <c r="O28" s="27" t="s">
         <v>190</v>
       </c>
-      <c r="P28" s="28" t="s">
+      <c r="P28" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q28" s="30">
+      <c r="Q28" s="29">
         <v>6</v>
       </c>
-      <c r="R28" s="30" t="s">
+      <c r="R28" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="S28" s="30" t="s">
+      <c r="S28" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="T28" s="31" t="s">
+      <c r="T28" s="30" t="s">
         <v>215</v>
       </c>
-      <c r="U28" s="30" t="s">
+      <c r="U28" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="V28" s="59" t="s">
+      <c r="V28" s="56" t="s">
         <v>251</v>
       </c>
-      <c r="W28" s="59"/>
-      <c r="X28" s="59"/>
-    </row>
-    <row r="29" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="s">
+      <c r="W28" s="56"/>
+      <c r="X28" s="56"/>
+    </row>
+    <row r="29" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="D29" s="28" t="s">
+      <c r="D29" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="83" t="s">
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="H29" s="83">
+      <c r="H29" s="80">
         <v>27</v>
       </c>
-      <c r="I29" s="84" t="s">
+      <c r="I29" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="83" t="s">
+      <c r="J29" s="80" t="s">
         <v>246</v>
       </c>
-      <c r="K29" s="84" t="s">
+      <c r="K29" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="L29" s="84" t="s">
+      <c r="L29" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="M29" s="84"/>
-      <c r="N29" s="84"/>
-      <c r="O29" s="83"/>
-      <c r="P29" s="83" t="s">
+      <c r="M29" s="81"/>
+      <c r="N29" s="81"/>
+      <c r="O29" s="80"/>
+      <c r="P29" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="Q29" s="83"/>
-      <c r="R29" s="83"/>
-      <c r="S29" s="83"/>
-      <c r="T29" s="85"/>
-      <c r="U29" s="83"/>
-      <c r="V29" s="60"/>
-      <c r="W29" s="60"/>
-      <c r="X29" s="59" t="s">
+      <c r="Q29" s="80"/>
+      <c r="R29" s="80"/>
+      <c r="S29" s="80"/>
+      <c r="T29" s="82"/>
+      <c r="U29" s="80"/>
+      <c r="V29" s="57"/>
+      <c r="W29" s="57"/>
+      <c r="X29" s="56" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="1:24" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="27" t="s">
+    <row r="30" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="D30" s="28" t="s">
+      <c r="D30" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28" t="s">
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="H30" s="28">
+      <c r="H30" s="27">
         <v>28</v>
       </c>
-      <c r="I30" s="29" t="s">
+      <c r="I30" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="J30" s="28" t="s">
+      <c r="J30" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="K30" s="29" t="s">
+      <c r="K30" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="L30" s="29" t="s">
+      <c r="L30" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="M30" s="29"/>
-      <c r="N30" s="29" t="s">
+      <c r="M30" s="28"/>
+      <c r="N30" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="O30" s="28" t="s">
+      <c r="O30" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="P30" s="28" t="s">
+      <c r="P30" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="Q30" s="30">
+      <c r="Q30" s="29">
         <v>6</v>
       </c>
-      <c r="R30" s="30" t="s">
+      <c r="R30" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="S30" s="30" t="s">
+      <c r="S30" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="T30" s="31" t="s">
+      <c r="T30" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="U30" s="30" t="s">
+      <c r="U30" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="V30" s="59" t="s">
+      <c r="V30" s="56" t="s">
         <v>251</v>
       </c>
-      <c r="W30" s="59"/>
-      <c r="X30" s="59"/>
-    </row>
-    <row r="31" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="27" t="s">
+      <c r="W30" s="56"/>
+      <c r="X30" s="56"/>
+    </row>
+    <row r="31" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="D31" s="28" t="s">
+      <c r="D31" s="27" t="s">
         <v>191</v>
       </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28" t="s">
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="H31" s="28">
+      <c r="H31" s="27">
         <v>29</v>
       </c>
-      <c r="I31" s="29" t="s">
+      <c r="I31" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="J31" s="28" t="s">
+      <c r="J31" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="K31" s="29" t="s">
+      <c r="K31" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="L31" s="29" t="s">
+      <c r="L31" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="M31" s="29"/>
-      <c r="N31" s="29" t="s">
+      <c r="M31" s="28"/>
+      <c r="N31" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="O31" s="28"/>
-      <c r="P31" s="28" t="s">
+      <c r="O31" s="27"/>
+      <c r="P31" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="Q31" s="30">
+      <c r="Q31" s="29">
         <v>6</v>
       </c>
-      <c r="R31" s="30" t="s">
+      <c r="R31" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="S31" s="30" t="s">
+      <c r="S31" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="T31" s="31" t="s">
+      <c r="T31" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="U31" s="30" t="s">
+      <c r="U31" s="29" t="s">
         <v>199</v>
       </c>
-      <c r="V31" s="59" t="s">
+      <c r="V31" s="56" t="s">
         <v>251</v>
       </c>
-      <c r="W31" s="59"/>
-      <c r="X31" s="59"/>
-    </row>
-    <row r="32" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="20"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
-      <c r="F32" s="21"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="22"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="22"/>
-      <c r="O32" s="21"/>
-      <c r="P32" s="21"/>
-      <c r="Q32" s="21"/>
-      <c r="R32" s="21"/>
-      <c r="S32" s="21"/>
-      <c r="T32" s="21"/>
-      <c r="U32" s="21"/>
+      <c r="W31" s="56"/>
+      <c r="X31" s="56"/>
+    </row>
+    <row r="32" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="19"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="20"/>
+      <c r="P32" s="20"/>
+      <c r="Q32" s="20"/>
+      <c r="R32" s="20"/>
+      <c r="S32" s="20"/>
+      <c r="T32" s="20"/>
+      <c r="U32" s="20"/>
     </row>
     <row r="33" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="23"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="23"/>
-      <c r="L33" s="23"/>
-      <c r="M33" s="23"/>
-      <c r="N33" s="23"/>
-      <c r="O33" s="24"/>
-      <c r="P33" s="24"/>
-      <c r="Q33" s="24"/>
-      <c r="R33" s="24"/>
-      <c r="S33" s="24"/>
-      <c r="T33" s="24"/>
-      <c r="U33" s="24"/>
-      <c r="V33" s="25"/>
+      <c r="A33" s="22"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="22"/>
+      <c r="N33" s="22"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="23"/>
+      <c r="R33" s="23"/>
+      <c r="S33" s="23"/>
+      <c r="T33" s="23"/>
+      <c r="U33" s="23"/>
+      <c r="V33" s="24"/>
       <c r="W33" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="X33" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="X33" s="3" t="s">
-        <v>269</v>
-      </c>
     </row>
     <row r="34" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="23"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="23"/>
-      <c r="L34" s="23"/>
-      <c r="M34" s="23"/>
-      <c r="N34" s="23"/>
-      <c r="O34" s="24"/>
-      <c r="P34" s="24"/>
-      <c r="Q34" s="24"/>
-      <c r="R34" s="24"/>
-      <c r="S34" s="24"/>
-      <c r="T34" s="24"/>
-      <c r="U34" s="24"/>
-      <c r="V34" s="25" t="s">
-        <v>267</v>
+      <c r="A34" s="22"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="22"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="23"/>
+      <c r="P34" s="23"/>
+      <c r="Q34" s="23"/>
+      <c r="R34" s="23"/>
+      <c r="S34" s="23"/>
+      <c r="T34" s="23"/>
+      <c r="U34" s="23"/>
+      <c r="V34" s="24" t="s">
+        <v>270</v>
       </c>
       <c r="W34" s="3" t="s">
         <v>260</v>
@@ -4146,156 +4186,156 @@
       </c>
     </row>
     <row r="35" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="23"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="23"/>
-      <c r="N35" s="23"/>
-      <c r="O35" s="24"/>
-      <c r="P35" s="24"/>
-      <c r="Q35" s="24"/>
-      <c r="R35" s="24"/>
-      <c r="S35" s="24"/>
-      <c r="T35" s="24"/>
-      <c r="U35" s="24"/>
-      <c r="V35" s="25" t="s">
-        <v>268</v>
+      <c r="A35" s="22"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22"/>
+      <c r="N35" s="22"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="23"/>
+      <c r="Q35" s="23"/>
+      <c r="R35" s="23"/>
+      <c r="S35" s="23"/>
+      <c r="T35" s="23"/>
+      <c r="U35" s="23"/>
+      <c r="V35" s="24" t="s">
+        <v>271</v>
       </c>
       <c r="W35" s="3" t="s">
         <v>262</v>
       </c>
       <c r="X35" s="3" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
     </row>
     <row r="36" spans="1:24" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="23"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="23"/>
-      <c r="L36" s="23"/>
-      <c r="M36" s="23"/>
-      <c r="N36" s="23"/>
-      <c r="O36" s="24"/>
-      <c r="P36" s="24"/>
-      <c r="Q36" s="24"/>
-      <c r="R36" s="24"/>
-      <c r="S36" s="24"/>
-      <c r="T36" s="24"/>
-      <c r="U36" s="24"/>
-      <c r="V36" s="25"/>
+      <c r="A36" s="22"/>
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="23"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="22"/>
+      <c r="N36" s="22"/>
+      <c r="O36" s="23"/>
+      <c r="P36" s="23"/>
+      <c r="Q36" s="23"/>
+      <c r="R36" s="23"/>
+      <c r="S36" s="23"/>
+      <c r="T36" s="23"/>
+      <c r="U36" s="23"/>
+      <c r="V36" s="24"/>
     </row>
     <row r="37" spans="1:24" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="23"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="23"/>
-      <c r="L37" s="23"/>
-      <c r="M37" s="23"/>
-      <c r="N37" s="23"/>
-      <c r="O37" s="24"/>
-      <c r="P37" s="24"/>
-      <c r="Q37" s="24"/>
-      <c r="R37" s="24"/>
-      <c r="S37" s="24"/>
-      <c r="T37" s="24"/>
-      <c r="U37" s="24"/>
-      <c r="V37" s="25"/>
+      <c r="A37" s="22"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
+      <c r="H37" s="23"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="23"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="22"/>
+      <c r="N37" s="22"/>
+      <c r="O37" s="23"/>
+      <c r="P37" s="23"/>
+      <c r="Q37" s="23"/>
+      <c r="R37" s="23"/>
+      <c r="S37" s="23"/>
+      <c r="T37" s="23"/>
+      <c r="U37" s="23"/>
+      <c r="V37" s="24"/>
     </row>
     <row r="38" spans="1:24" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="23"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="24"/>
-      <c r="K38" s="23"/>
-      <c r="L38" s="23"/>
-      <c r="M38" s="23"/>
-      <c r="N38" s="23"/>
-      <c r="O38" s="24"/>
-      <c r="P38" s="24"/>
-      <c r="Q38" s="24"/>
-      <c r="R38" s="24"/>
-      <c r="S38" s="24"/>
-      <c r="T38" s="24"/>
-      <c r="U38" s="24"/>
-      <c r="V38" s="25"/>
+      <c r="A38" s="22"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
+      <c r="H38" s="23"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="23"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="22"/>
+      <c r="N38" s="22"/>
+      <c r="O38" s="23"/>
+      <c r="P38" s="23"/>
+      <c r="Q38" s="23"/>
+      <c r="R38" s="23"/>
+      <c r="S38" s="23"/>
+      <c r="T38" s="23"/>
+      <c r="U38" s="23"/>
+      <c r="V38" s="24"/>
     </row>
     <row r="39" spans="1:24" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="23"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="24"/>
-      <c r="K39" s="23"/>
-      <c r="L39" s="23"/>
-      <c r="M39" s="23"/>
-      <c r="N39" s="23"/>
-      <c r="O39" s="24"/>
-      <c r="P39" s="24"/>
-      <c r="Q39" s="24"/>
-      <c r="R39" s="24"/>
-      <c r="S39" s="24"/>
-      <c r="T39" s="24"/>
-      <c r="U39" s="24"/>
-      <c r="V39" s="25"/>
+      <c r="A39" s="22"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="22"/>
+      <c r="L39" s="22"/>
+      <c r="M39" s="22"/>
+      <c r="N39" s="22"/>
+      <c r="O39" s="23"/>
+      <c r="P39" s="23"/>
+      <c r="Q39" s="23"/>
+      <c r="R39" s="23"/>
+      <c r="S39" s="23"/>
+      <c r="T39" s="23"/>
+      <c r="U39" s="23"/>
+      <c r="V39" s="24"/>
     </row>
     <row r="40" spans="1:24" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="25"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="26"/>
-      <c r="I40" s="26"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
-      <c r="L40" s="25"/>
-      <c r="M40" s="25"/>
-      <c r="N40" s="25"/>
-      <c r="O40" s="26"/>
-      <c r="P40" s="26"/>
-      <c r="Q40" s="26"/>
-      <c r="R40" s="25"/>
-      <c r="S40" s="25"/>
-      <c r="T40" s="25"/>
-      <c r="U40" s="25"/>
-      <c r="V40" s="25"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="24"/>
+      <c r="K40" s="24"/>
+      <c r="L40" s="24"/>
+      <c r="M40" s="24"/>
+      <c r="N40" s="24"/>
+      <c r="O40" s="25"/>
+      <c r="P40" s="25"/>
+      <c r="Q40" s="25"/>
+      <c r="R40" s="24"/>
+      <c r="S40" s="24"/>
+      <c r="T40" s="24"/>
+      <c r="U40" s="24"/>
+      <c r="V40" s="24"/>
     </row>
     <row r="54" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">

</xml_diff>

<commit_message>
Actualizando estado recursos MA_08_10_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="278">
   <si>
     <t>Asignatura</t>
   </si>
@@ -815,9 +815,6 @@
     <t>Reconoce las características de las líneas notables de un triángulo</t>
   </si>
   <si>
-    <t>Faltan 26</t>
-  </si>
-  <si>
     <t>Esperando imágenes</t>
   </si>
   <si>
@@ -830,28 +827,40 @@
     <t>En espera de solicitud gráfica.</t>
   </si>
   <si>
-    <t>En proceso 0</t>
-  </si>
-  <si>
     <t>Recurso regresado al autor</t>
   </si>
   <si>
     <t>Recurso offLine, esperando imágenes, Pedro ya lo subio a GRECO</t>
   </si>
   <si>
-    <t>Listos 9</t>
-  </si>
-  <si>
-    <t>Faltan 20</t>
-  </si>
-  <si>
     <t>En proceso 6</t>
   </si>
   <si>
-    <t>faltan 20</t>
-  </si>
-  <si>
     <t>Regreso a la autora con comentarios 18/02/2016</t>
+  </si>
+  <si>
+    <t>Autora ya desbloqueo</t>
+  </si>
+  <si>
+    <t>autora ya desbloqueo</t>
+  </si>
+  <si>
+    <t>En proceso 2</t>
+  </si>
+  <si>
+    <t>Faltan 24</t>
+  </si>
+  <si>
+    <t>Listos 11</t>
+  </si>
+  <si>
+    <t>Faltan 18</t>
+  </si>
+  <si>
+    <t>Listos 5</t>
+  </si>
+  <si>
+    <t>faltan 18</t>
   </si>
 </sst>
 </file>
@@ -1252,7 +1261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1454,21 +1463,6 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1517,81 +1511,6 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1611,6 +1530,117 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1919,9 +1949,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GH90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+      <selection pane="bottomLeft" activeCell="W21" sqref="W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1953,94 +1983,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="95" t="s">
+      <c r="B1" s="103" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="106" t="s">
+      <c r="C1" s="114" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="97" t="s">
+      <c r="D1" s="105" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="95" t="s">
+      <c r="E1" s="103" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="90" t="s">
+      <c r="F1" s="100" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="99" t="s">
+      <c r="G1" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="91" t="s">
+      <c r="H1" s="101" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="90" t="s">
+      <c r="I1" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="103" t="s">
+      <c r="J1" s="111" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="101" t="s">
+      <c r="K1" s="109" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="99" t="s">
+      <c r="L1" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="105" t="s">
+      <c r="M1" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="105"/>
-      <c r="O1" s="93" t="s">
+      <c r="N1" s="113"/>
+      <c r="O1" s="92" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="93" t="s">
+      <c r="P1" s="92" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="109" t="s">
+      <c r="Q1" s="94" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="113" t="s">
+      <c r="R1" s="98" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="109" t="s">
+      <c r="S1" s="94" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="111" t="s">
+      <c r="T1" s="96" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="109" t="s">
+      <c r="U1" s="94" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:190" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="98"/>
-      <c r="B2" s="96"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="108"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="91"/>
-      <c r="J2" s="104"/>
-      <c r="K2" s="102"/>
-      <c r="L2" s="100"/>
+      <c r="A2" s="106"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="102"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="110"/>
+      <c r="L2" s="108"/>
       <c r="M2" s="43" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="94"/>
-      <c r="P2" s="94"/>
-      <c r="Q2" s="110"/>
-      <c r="R2" s="114"/>
-      <c r="S2" s="110"/>
-      <c r="T2" s="112"/>
-      <c r="U2" s="110"/>
+      <c r="O2" s="93"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="95"/>
+      <c r="R2" s="99"/>
+      <c r="S2" s="95"/>
+      <c r="T2" s="97"/>
+      <c r="U2" s="95"/>
       <c r="V2" s="36" t="s">
         <v>255</v>
       </c>
@@ -2331,51 +2361,51 @@
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="41"/>
-      <c r="G7" s="84" t="s">
+      <c r="G7" s="79" t="s">
         <v>145</v>
       </c>
-      <c r="H7" s="80">
+      <c r="H7" s="75">
         <v>5</v>
       </c>
-      <c r="I7" s="81" t="s">
+      <c r="I7" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="80" t="s">
+      <c r="J7" s="75" t="s">
         <v>226</v>
       </c>
-      <c r="K7" s="85" t="s">
+      <c r="K7" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="81" t="s">
+      <c r="L7" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="81"/>
-      <c r="N7" s="81"/>
-      <c r="O7" s="80" t="s">
+      <c r="M7" s="76"/>
+      <c r="N7" s="76"/>
+      <c r="O7" s="75" t="s">
         <v>170</v>
       </c>
-      <c r="P7" s="80" t="s">
+      <c r="P7" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="86">
+      <c r="Q7" s="81">
         <v>9</v>
       </c>
-      <c r="R7" s="86" t="s">
+      <c r="R7" s="81" t="s">
         <v>128</v>
       </c>
-      <c r="S7" s="86" t="s">
+      <c r="S7" s="81" t="s">
         <v>219</v>
       </c>
-      <c r="T7" s="86" t="s">
+      <c r="T7" s="81" t="s">
         <v>220</v>
       </c>
-      <c r="U7" s="86" t="s">
+      <c r="U7" s="81" t="s">
         <v>221</v>
       </c>
       <c r="V7" s="57" t="s">
         <v>222</v>
       </c>
-      <c r="W7" s="83">
+      <c r="W7" s="78">
         <v>42416</v>
       </c>
       <c r="X7" s="62" t="s">
@@ -2508,13 +2538,13 @@
         <v>250</v>
       </c>
       <c r="W9" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="X9" s="61">
         <v>42417</v>
       </c>
       <c r="Y9" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="Z9" s="6"/>
       <c r="AA9" s="6"/>
@@ -2746,7 +2776,7 @@
       <c r="W10" s="56"/>
       <c r="X10" s="62"/>
       <c r="Y10" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2764,32 +2794,32 @@
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="41"/>
-      <c r="G11" s="87" t="s">
+      <c r="G11" s="82" t="s">
         <v>261</v>
       </c>
-      <c r="H11" s="80">
+      <c r="H11" s="75">
         <v>9</v>
       </c>
-      <c r="I11" s="81" t="s">
+      <c r="I11" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="80" t="s">
+      <c r="J11" s="75" t="s">
         <v>230</v>
       </c>
-      <c r="K11" s="81" t="s">
+      <c r="K11" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="81" t="s">
+      <c r="L11" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="81"/>
-      <c r="N11" s="81" t="s">
+      <c r="M11" s="76"/>
+      <c r="N11" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="O11" s="88" t="s">
+      <c r="O11" s="83" t="s">
         <v>217</v>
       </c>
-      <c r="P11" s="80" t="s">
+      <c r="P11" s="75" t="s">
         <v>19</v>
       </c>
       <c r="Q11" s="57">
@@ -2801,7 +2831,7 @@
       <c r="S11" s="57" t="s">
         <v>124</v>
       </c>
-      <c r="T11" s="89" t="s">
+      <c r="T11" s="84" t="s">
         <v>209</v>
       </c>
       <c r="U11" s="57" t="s">
@@ -2810,7 +2840,7 @@
       <c r="V11" s="57" t="s">
         <v>250</v>
       </c>
-      <c r="W11" s="83">
+      <c r="W11" s="78">
         <v>42416</v>
       </c>
       <c r="X11" s="62" t="s">
@@ -2883,7 +2913,7 @@
         <v>42418</v>
       </c>
       <c r="Y12" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2966,7 +2996,7 @@
       <c r="E14" s="11"/>
       <c r="F14" s="41"/>
       <c r="G14" s="49" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H14" s="37">
         <v>12</v>
@@ -3016,7 +3046,7 @@
         <v>42417</v>
       </c>
       <c r="Y14" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3080,7 +3110,7 @@
       <c r="V15" s="57" t="s">
         <v>251</v>
       </c>
-      <c r="W15" s="115"/>
+      <c r="W15" s="85"/>
       <c r="X15" s="61">
         <v>42418</v>
       </c>
@@ -3164,56 +3194,56 @@
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="41"/>
-      <c r="G17" s="116" t="s">
+      <c r="G17" s="86" t="s">
         <v>150</v>
       </c>
-      <c r="H17" s="117">
+      <c r="H17" s="87">
         <v>15</v>
       </c>
-      <c r="I17" s="118" t="s">
+      <c r="I17" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="117" t="s">
+      <c r="J17" s="87" t="s">
         <v>161</v>
       </c>
-      <c r="K17" s="118" t="s">
+      <c r="K17" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="118" t="s">
+      <c r="L17" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="118"/>
-      <c r="N17" s="118" t="s">
+      <c r="M17" s="88"/>
+      <c r="N17" s="88" t="s">
         <v>120</v>
       </c>
-      <c r="O17" s="117" t="s">
+      <c r="O17" s="87" t="s">
         <v>179</v>
       </c>
-      <c r="P17" s="117" t="s">
+      <c r="P17" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="Q17" s="119">
+      <c r="Q17" s="89">
         <v>6</v>
       </c>
-      <c r="R17" s="119" t="s">
+      <c r="R17" s="89" t="s">
         <v>123</v>
       </c>
-      <c r="S17" s="119" t="s">
+      <c r="S17" s="89" t="s">
         <v>124</v>
       </c>
-      <c r="T17" s="120" t="s">
+      <c r="T17" s="90" t="s">
         <v>125</v>
       </c>
-      <c r="U17" s="119" t="s">
+      <c r="U17" s="89" t="s">
         <v>199</v>
       </c>
-      <c r="V17" s="119" t="s">
+      <c r="V17" s="89" t="s">
         <v>250</v>
       </c>
-      <c r="W17" s="119"/>
-      <c r="X17" s="121"/>
+      <c r="W17" s="89"/>
+      <c r="X17" s="91"/>
       <c r="Y17" s="3" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3279,6 +3309,9 @@
       </c>
       <c r="W18" s="56"/>
       <c r="X18" s="62"/>
+      <c r="Y18" s="3" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="19" spans="1:25" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
@@ -3345,6 +3378,9 @@
       </c>
       <c r="W19" s="63"/>
       <c r="X19" s="64"/>
+      <c r="Y19" s="3" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="20" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
@@ -3361,54 +3397,58 @@
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="65"/>
-      <c r="G20" s="69" t="s">
+      <c r="G20" s="123" t="s">
         <v>239</v>
       </c>
-      <c r="H20" s="70">
+      <c r="H20" s="124">
         <v>18</v>
       </c>
-      <c r="I20" s="71" t="s">
+      <c r="I20" s="125" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="70" t="s">
+      <c r="J20" s="124" t="s">
         <v>240</v>
       </c>
-      <c r="K20" s="71" t="s">
+      <c r="K20" s="125" t="s">
         <v>20</v>
       </c>
-      <c r="L20" s="71" t="s">
+      <c r="L20" s="125" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="71"/>
-      <c r="N20" s="71" t="s">
+      <c r="M20" s="125"/>
+      <c r="N20" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="O20" s="70" t="s">
+      <c r="O20" s="124" t="s">
         <v>182</v>
       </c>
-      <c r="P20" s="70" t="s">
+      <c r="P20" s="124" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="72">
+      <c r="Q20" s="126">
         <v>6</v>
       </c>
-      <c r="R20" s="72" t="s">
+      <c r="R20" s="126" t="s">
         <v>123</v>
       </c>
-      <c r="S20" s="72" t="s">
+      <c r="S20" s="126" t="s">
         <v>124</v>
       </c>
-      <c r="T20" s="73" t="s">
+      <c r="T20" s="127" t="s">
         <v>209</v>
       </c>
-      <c r="U20" s="72" t="s">
+      <c r="U20" s="126" t="s">
         <v>199</v>
       </c>
-      <c r="V20" s="59" t="s">
+      <c r="V20" s="122" t="s">
         <v>251</v>
       </c>
-      <c r="W20" s="59"/>
-      <c r="X20" s="60"/>
+      <c r="W20" s="128">
+        <v>42418</v>
+      </c>
+      <c r="X20" s="60" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="21" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
@@ -3425,54 +3465,58 @@
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="65"/>
-      <c r="G21" s="74" t="s">
+      <c r="G21" s="117" t="s">
         <v>153</v>
       </c>
-      <c r="H21" s="33">
+      <c r="H21" s="118">
         <v>19</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="33" t="s">
+      <c r="J21" s="118" t="s">
         <v>163</v>
       </c>
-      <c r="K21" s="10" t="s">
+      <c r="K21" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="L21" s="10" t="s">
+      <c r="L21" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10" t="s">
+      <c r="M21" s="119"/>
+      <c r="N21" s="119" t="s">
         <v>23</v>
       </c>
-      <c r="O21" s="33" t="s">
+      <c r="O21" s="118" t="s">
         <v>183</v>
       </c>
-      <c r="P21" s="33" t="s">
+      <c r="P21" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="Q21" s="5">
+      <c r="Q21" s="120">
         <v>6</v>
       </c>
-      <c r="R21" s="5" t="s">
+      <c r="R21" s="120" t="s">
         <v>123</v>
       </c>
-      <c r="S21" s="5" t="s">
+      <c r="S21" s="120" t="s">
         <v>124</v>
       </c>
-      <c r="T21" s="15" t="s">
+      <c r="T21" s="121" t="s">
         <v>133</v>
       </c>
-      <c r="U21" s="5" t="s">
+      <c r="U21" s="120" t="s">
         <v>199</v>
       </c>
-      <c r="V21" s="56" t="s">
+      <c r="V21" s="57" t="s">
         <v>251</v>
       </c>
-      <c r="W21" s="56"/>
-      <c r="X21" s="62"/>
+      <c r="W21" s="78">
+        <v>42418</v>
+      </c>
+      <c r="X21" s="62" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="22" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
@@ -3489,7 +3533,7 @@
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="65"/>
-      <c r="G22" s="74" t="s">
+      <c r="G22" s="69" t="s">
         <v>241</v>
       </c>
       <c r="H22" s="33">
@@ -3553,7 +3597,7 @@
       </c>
       <c r="E23" s="8"/>
       <c r="F23" s="65"/>
-      <c r="G23" s="74" t="s">
+      <c r="G23" s="69" t="s">
         <v>154</v>
       </c>
       <c r="H23" s="33">
@@ -3617,7 +3661,7 @@
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="65"/>
-      <c r="G24" s="74" t="s">
+      <c r="G24" s="69" t="s">
         <v>248</v>
       </c>
       <c r="H24" s="33">
@@ -3681,7 +3725,7 @@
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="65"/>
-      <c r="G25" s="74" t="s">
+      <c r="G25" s="69" t="s">
         <v>155</v>
       </c>
       <c r="H25" s="33">
@@ -3747,47 +3791,47 @@
         <v>127</v>
       </c>
       <c r="F26" s="65"/>
-      <c r="G26" s="75" t="s">
+      <c r="G26" s="70" t="s">
         <v>156</v>
       </c>
-      <c r="H26" s="76">
+      <c r="H26" s="71">
         <v>24</v>
       </c>
-      <c r="I26" s="77" t="s">
+      <c r="I26" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="76" t="s">
+      <c r="J26" s="71" t="s">
         <v>195</v>
       </c>
-      <c r="K26" s="77" t="s">
+      <c r="K26" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="77" t="s">
+      <c r="L26" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="M26" s="77"/>
-      <c r="N26" s="77" t="s">
+      <c r="M26" s="72"/>
+      <c r="N26" s="72" t="s">
         <v>121</v>
       </c>
-      <c r="O26" s="76" t="s">
+      <c r="O26" s="71" t="s">
         <v>188</v>
       </c>
-      <c r="P26" s="76" t="s">
+      <c r="P26" s="71" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="78">
+      <c r="Q26" s="73">
         <v>6</v>
       </c>
-      <c r="R26" s="78" t="s">
+      <c r="R26" s="73" t="s">
         <v>123</v>
       </c>
-      <c r="S26" s="78" t="s">
+      <c r="S26" s="73" t="s">
         <v>124</v>
       </c>
-      <c r="T26" s="79" t="s">
+      <c r="T26" s="74" t="s">
         <v>136</v>
       </c>
-      <c r="U26" s="78" t="s">
+      <c r="U26" s="73" t="s">
         <v>199</v>
       </c>
       <c r="V26" s="63" t="s">
@@ -3939,35 +3983,35 @@
       </c>
       <c r="E29" s="27"/>
       <c r="F29" s="27"/>
-      <c r="G29" s="80" t="s">
+      <c r="G29" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="H29" s="80">
+      <c r="H29" s="75">
         <v>27</v>
       </c>
-      <c r="I29" s="81" t="s">
+      <c r="I29" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="80" t="s">
+      <c r="J29" s="75" t="s">
         <v>246</v>
       </c>
-      <c r="K29" s="81" t="s">
+      <c r="K29" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="L29" s="81" t="s">
+      <c r="L29" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="M29" s="81"/>
-      <c r="N29" s="81"/>
-      <c r="O29" s="80"/>
-      <c r="P29" s="80" t="s">
+      <c r="M29" s="76"/>
+      <c r="N29" s="76"/>
+      <c r="O29" s="75"/>
+      <c r="P29" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="Q29" s="80"/>
-      <c r="R29" s="80"/>
-      <c r="S29" s="80"/>
-      <c r="T29" s="82"/>
-      <c r="U29" s="80"/>
+      <c r="Q29" s="75"/>
+      <c r="R29" s="75"/>
+      <c r="S29" s="75"/>
+      <c r="T29" s="77"/>
+      <c r="U29" s="75"/>
       <c r="V29" s="57"/>
       <c r="W29" s="57"/>
       <c r="X29" s="56" t="s">
@@ -4147,10 +4191,10 @@
       <c r="U33" s="23"/>
       <c r="V33" s="24"/>
       <c r="W33" s="3" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="X33" s="3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="34" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4176,13 +4220,13 @@
       <c r="T34" s="23"/>
       <c r="U34" s="23"/>
       <c r="V34" s="24" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="W34" s="3" t="s">
         <v>260</v>
       </c>
       <c r="X34" s="3" t="s">
-        <v>260</v>
+        <v>276</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4208,13 +4252,13 @@
       <c r="T35" s="23"/>
       <c r="U35" s="23"/>
       <c r="V35" s="24" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="W35" s="3" t="s">
-        <v>262</v>
+        <v>273</v>
       </c>
       <c r="X35" s="3" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="36" spans="1:24" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4524,12 +4568,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4544,6 +4582,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Solicitud gráfica recurso MA_08_09_REC60
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="280">
   <si>
     <t>Asignatura</t>
   </si>
@@ -867,9 +867,6 @@
   </si>
   <si>
     <t>Recurso offline en la carpeta de github</t>
-  </si>
-  <si>
-    <t>Regreso a la autora (29/02/2016) pues no es clara la solicitud gráfica</t>
   </si>
 </sst>
 </file>
@@ -929,7 +926,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1035,12 +1032,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1270,7 +1261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1562,12 +1553,63 @@
     <xf numFmtId="14" fontId="3" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1585,81 +1627,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1969,7 +1936,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z11" sqref="Z11"/>
+      <selection pane="bottomLeft" activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2001,94 +1968,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="106" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="110" t="s">
+      <c r="B1" s="104" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="121" t="s">
+      <c r="C1" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="112" t="s">
+      <c r="D1" s="106" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="110" t="s">
+      <c r="E1" s="104" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="107" t="s">
+      <c r="F1" s="99" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="114" t="s">
+      <c r="G1" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="108" t="s">
+      <c r="H1" s="100" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="107" t="s">
+      <c r="I1" s="99" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="118" t="s">
+      <c r="J1" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="116" t="s">
+      <c r="K1" s="110" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="114" t="s">
+      <c r="L1" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="120" t="s">
+      <c r="M1" s="114" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="120"/>
-      <c r="O1" s="99" t="s">
+      <c r="N1" s="114"/>
+      <c r="O1" s="102" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="99" t="s">
+      <c r="P1" s="102" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="101" t="s">
+      <c r="Q1" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="105" t="s">
+      <c r="R1" s="122" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="101" t="s">
+      <c r="S1" s="118" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="103" t="s">
+      <c r="T1" s="120" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="101" t="s">
+      <c r="U1" s="118" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:190" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="113"/>
-      <c r="B2" s="111"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="108"/>
-      <c r="J2" s="119"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="115"/>
+      <c r="A2" s="107"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="109"/>
       <c r="M2" s="42" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="100"/>
-      <c r="P2" s="100"/>
-      <c r="Q2" s="102"/>
-      <c r="R2" s="106"/>
-      <c r="S2" s="102"/>
-      <c r="T2" s="104"/>
-      <c r="U2" s="102"/>
+      <c r="O2" s="103"/>
+      <c r="P2" s="103"/>
+      <c r="Q2" s="119"/>
+      <c r="R2" s="123"/>
+      <c r="S2" s="119"/>
+      <c r="T2" s="121"/>
+      <c r="U2" s="119"/>
       <c r="V2" s="35" t="s">
         <v>254</v>
       </c>
@@ -2449,57 +2416,57 @@
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="40"/>
-      <c r="G8" s="124" t="s">
+      <c r="G8" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="H8" s="125">
+      <c r="H8" s="36">
         <v>6</v>
       </c>
-      <c r="I8" s="126" t="s">
+      <c r="I8" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="127" t="s">
+      <c r="J8" s="82" t="s">
         <v>227</v>
       </c>
-      <c r="K8" s="126" t="s">
+      <c r="K8" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="126" t="s">
+      <c r="L8" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="M8" s="126" t="s">
+      <c r="M8" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="N8" s="126"/>
-      <c r="O8" s="125" t="s">
+      <c r="N8" s="37"/>
+      <c r="O8" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="P8" s="125" t="s">
+      <c r="P8" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="128">
+      <c r="Q8" s="38">
         <v>6</v>
       </c>
-      <c r="R8" s="128" t="s">
+      <c r="R8" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="S8" s="128" t="s">
+      <c r="S8" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="T8" s="129" t="s">
+      <c r="T8" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="U8" s="128" t="s">
+      <c r="U8" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="V8" s="128" t="s">
+      <c r="V8" s="46" t="s">
         <v>251</v>
       </c>
-      <c r="W8" s="128"/>
-      <c r="X8" s="130"/>
-      <c r="Y8" s="131" t="s">
-        <v>280</v>
-      </c>
+      <c r="W8" s="30"/>
+      <c r="X8" s="49">
+        <v>42429</v>
+      </c>
+      <c r="Y8" s="6"/>
     </row>
     <row r="9" spans="1:190" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
@@ -4620,6 +4587,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4634,12 +4607,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Edición cuaderno de estudio MA_08_11_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
@@ -1264,7 +1264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1415,21 +1415,6 @@
     <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1472,9 +1457,6 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="15" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1520,6 +1502,36 @@
     <xf numFmtId="0" fontId="3" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="14" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="14" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1529,12 +1541,6 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1577,31 +1583,7 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="14" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="14" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1910,9 +1892,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GH90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23:U23"/>
+      <selection pane="bottomLeft" activeCell="V20" sqref="V20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1944,94 +1926,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="103" t="s">
+      <c r="C1" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="94" t="s">
+      <c r="D1" s="96" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="92" t="s">
+      <c r="E1" s="94" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="87" t="s">
+      <c r="F1" s="91" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="96" t="s">
+      <c r="G1" s="98" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="88" t="s">
+      <c r="H1" s="92" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="87" t="s">
+      <c r="I1" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="100" t="s">
+      <c r="J1" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="98" t="s">
+      <c r="K1" s="100" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="96" t="s">
+      <c r="L1" s="98" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="102" t="s">
+      <c r="M1" s="104" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="102"/>
-      <c r="O1" s="90" t="s">
+      <c r="N1" s="104"/>
+      <c r="O1" s="83" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="90" t="s">
+      <c r="P1" s="83" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="106" t="s">
+      <c r="Q1" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="110" t="s">
+      <c r="R1" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="106" t="s">
+      <c r="S1" s="85" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="108" t="s">
+      <c r="T1" s="87" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="106" t="s">
+      <c r="U1" s="85" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:190" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="95"/>
-      <c r="B2" s="93"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="97"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="101"/>
-      <c r="K2" s="99"/>
-      <c r="L2" s="97"/>
+      <c r="A2" s="97"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="106"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="107"/>
+      <c r="G2" s="99"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="92"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="101"/>
+      <c r="L2" s="99"/>
       <c r="M2" s="31" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="91"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="107"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="107"/>
-      <c r="T2" s="109"/>
-      <c r="U2" s="107"/>
+      <c r="O2" s="84"/>
+      <c r="P2" s="84"/>
+      <c r="Q2" s="86"/>
+      <c r="R2" s="90"/>
+      <c r="S2" s="86"/>
+      <c r="T2" s="88"/>
+      <c r="U2" s="86"/>
       <c r="V2" s="24" t="s">
         <v>254</v>
       </c>
@@ -2057,56 +2039,56 @@
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="29"/>
-      <c r="G3" s="74" t="s">
+      <c r="G3" s="68" t="s">
         <v>223</v>
       </c>
-      <c r="H3" s="75">
+      <c r="H3" s="69">
         <v>1</v>
       </c>
-      <c r="I3" s="76" t="s">
+      <c r="I3" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="76" t="s">
+      <c r="J3" s="70" t="s">
         <v>224</v>
       </c>
-      <c r="K3" s="76" t="s">
+      <c r="K3" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="76" t="s">
+      <c r="L3" s="70" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="76" t="s">
+      <c r="M3" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="76"/>
-      <c r="O3" s="75" t="s">
+      <c r="N3" s="70"/>
+      <c r="O3" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="P3" s="75" t="s">
+      <c r="P3" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="77">
+      <c r="Q3" s="71">
         <v>6</v>
       </c>
-      <c r="R3" s="77" t="s">
+      <c r="R3" s="71" t="s">
         <v>130</v>
       </c>
-      <c r="S3" s="77" t="s">
+      <c r="S3" s="71" t="s">
         <v>131</v>
       </c>
-      <c r="T3" s="78" t="s">
+      <c r="T3" s="72" t="s">
         <v>197</v>
       </c>
-      <c r="U3" s="77" t="s">
+      <c r="U3" s="71" t="s">
         <v>198</v>
       </c>
-      <c r="V3" s="57" t="s">
+      <c r="V3" s="52" t="s">
         <v>251</v>
       </c>
-      <c r="W3" s="73">
+      <c r="W3" s="67">
         <v>42422</v>
       </c>
-      <c r="X3" s="79">
+      <c r="X3" s="73">
         <v>42422</v>
       </c>
     </row>
@@ -2401,7 +2383,7 @@
       <c r="I8" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="65" t="s">
+      <c r="J8" s="60" t="s">
         <v>227</v>
       </c>
       <c r="K8" s="26" t="s">
@@ -2742,7 +2724,7 @@
         <v>252</v>
       </c>
       <c r="W10" s="21"/>
-      <c r="X10" s="86"/>
+      <c r="X10" s="80"/>
       <c r="Y10" s="3" t="s">
         <v>264</v>
       </c>
@@ -3235,56 +3217,56 @@
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="29"/>
-      <c r="G18" s="52" t="s">
+      <c r="G18" s="48" t="s">
         <v>151</v>
       </c>
-      <c r="H18" s="53">
+      <c r="H18" s="41">
         <v>16</v>
       </c>
-      <c r="I18" s="54" t="s">
+      <c r="I18" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="53" t="s">
+      <c r="J18" s="41" t="s">
         <v>238</v>
       </c>
-      <c r="K18" s="54" t="s">
+      <c r="K18" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="54" t="s">
+      <c r="L18" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="M18" s="54"/>
-      <c r="N18" s="54" t="s">
+      <c r="M18" s="42"/>
+      <c r="N18" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="O18" s="53" t="s">
+      <c r="O18" s="41" t="s">
         <v>180</v>
       </c>
-      <c r="P18" s="53" t="s">
+      <c r="P18" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="Q18" s="55">
+      <c r="Q18" s="34">
         <v>6</v>
       </c>
-      <c r="R18" s="55" t="s">
+      <c r="R18" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="S18" s="55" t="s">
+      <c r="S18" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T18" s="56" t="s">
+      <c r="T18" s="50" t="s">
         <v>211</v>
       </c>
-      <c r="U18" s="55" t="s">
+      <c r="U18" s="34" t="s">
         <v>199</v>
       </c>
       <c r="V18" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="W18" s="71">
+      <c r="W18" s="44">
         <v>42447</v>
       </c>
-      <c r="X18" s="112">
+      <c r="X18" s="81">
         <v>42419</v>
       </c>
     </row>
@@ -3305,56 +3287,56 @@
         <v>127</v>
       </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="58" t="s">
+      <c r="G19" s="53" t="s">
         <v>152</v>
       </c>
-      <c r="H19" s="59">
+      <c r="H19" s="54">
         <v>17</v>
       </c>
-      <c r="I19" s="60" t="s">
+      <c r="I19" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="59" t="s">
+      <c r="J19" s="54" t="s">
         <v>162</v>
       </c>
-      <c r="K19" s="60" t="s">
+      <c r="K19" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="L19" s="60" t="s">
+      <c r="L19" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="60"/>
-      <c r="N19" s="60" t="s">
+      <c r="M19" s="55"/>
+      <c r="N19" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="O19" s="59" t="s">
+      <c r="O19" s="54" t="s">
         <v>181</v>
       </c>
-      <c r="P19" s="59" t="s">
+      <c r="P19" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="61">
+      <c r="Q19" s="56">
         <v>6</v>
       </c>
-      <c r="R19" s="61" t="s">
+      <c r="R19" s="56" t="s">
         <v>123</v>
       </c>
-      <c r="S19" s="61" t="s">
+      <c r="S19" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="T19" s="62" t="s">
+      <c r="T19" s="57" t="s">
         <v>212</v>
       </c>
-      <c r="U19" s="61" t="s">
+      <c r="U19" s="56" t="s">
         <v>199</v>
       </c>
-      <c r="V19" s="63" t="s">
+      <c r="V19" s="58" t="s">
         <v>250</v>
       </c>
-      <c r="W19" s="113">
+      <c r="W19" s="82">
         <v>42419</v>
       </c>
-      <c r="X19" s="64">
+      <c r="X19" s="59">
         <v>42419</v>
       </c>
     </row>
@@ -3373,53 +3355,53 @@
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="40"/>
-      <c r="G20" s="67" t="s">
+      <c r="G20" s="62" t="s">
         <v>239</v>
       </c>
-      <c r="H20" s="68">
+      <c r="H20" s="63">
         <v>18</v>
       </c>
-      <c r="I20" s="69" t="s">
+      <c r="I20" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="68" t="s">
+      <c r="J20" s="63" t="s">
         <v>240</v>
       </c>
-      <c r="K20" s="69" t="s">
+      <c r="K20" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="L20" s="69" t="s">
+      <c r="L20" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="69"/>
-      <c r="N20" s="69" t="s">
+      <c r="M20" s="64"/>
+      <c r="N20" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="O20" s="68" t="s">
+      <c r="O20" s="63" t="s">
         <v>182</v>
       </c>
-      <c r="P20" s="68" t="s">
+      <c r="P20" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="57">
+      <c r="Q20" s="52">
         <v>6</v>
       </c>
-      <c r="R20" s="57" t="s">
+      <c r="R20" s="52" t="s">
         <v>123</v>
       </c>
-      <c r="S20" s="57" t="s">
+      <c r="S20" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="T20" s="70" t="s">
+      <c r="T20" s="65" t="s">
         <v>209</v>
       </c>
-      <c r="U20" s="57" t="s">
+      <c r="U20" s="52" t="s">
         <v>199</v>
       </c>
-      <c r="V20" s="57" t="s">
+      <c r="V20" s="52" t="s">
         <v>250</v>
       </c>
-      <c r="W20" s="66">
+      <c r="W20" s="61">
         <v>42418</v>
       </c>
       <c r="X20" s="36" t="s">
@@ -3509,56 +3491,56 @@
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="40"/>
-      <c r="G22" s="52" t="s">
+      <c r="G22" s="48" t="s">
         <v>241</v>
       </c>
-      <c r="H22" s="53">
+      <c r="H22" s="41">
         <v>20</v>
       </c>
-      <c r="I22" s="54" t="s">
+      <c r="I22" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="114" t="s">
+      <c r="J22" s="108" t="s">
         <v>242</v>
       </c>
-      <c r="K22" s="54" t="s">
+      <c r="K22" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="L22" s="54" t="s">
+      <c r="L22" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="M22" s="54"/>
-      <c r="N22" s="54" t="s">
+      <c r="M22" s="42"/>
+      <c r="N22" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="O22" s="53" t="s">
+      <c r="O22" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="P22" s="53" t="s">
+      <c r="P22" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="Q22" s="55">
+      <c r="Q22" s="34">
         <v>6</v>
       </c>
-      <c r="R22" s="55" t="s">
+      <c r="R22" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="S22" s="55" t="s">
+      <c r="S22" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T22" s="56" t="s">
+      <c r="T22" s="50" t="s">
         <v>200</v>
       </c>
-      <c r="U22" s="55" t="s">
+      <c r="U22" s="34" t="s">
         <v>199</v>
       </c>
       <c r="V22" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="W22" s="71">
+      <c r="W22" s="44">
         <v>42447</v>
       </c>
-      <c r="X22" s="112">
+      <c r="X22" s="81">
         <v>42419</v>
       </c>
     </row>
@@ -3723,7 +3705,7 @@
       <c r="I25" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="65" t="s">
+      <c r="J25" s="60" t="s">
         <v>248</v>
       </c>
       <c r="K25" s="26" t="s">
@@ -3761,7 +3743,7 @@
         <v>253</v>
       </c>
       <c r="W25" s="27"/>
-      <c r="X25" s="86" t="s">
+      <c r="X25" s="80" t="s">
         <v>280</v>
       </c>
     </row>
@@ -3782,54 +3764,54 @@
         <v>127</v>
       </c>
       <c r="F26" s="40"/>
-      <c r="G26" s="58" t="s">
+      <c r="G26" s="53" t="s">
         <v>156</v>
       </c>
-      <c r="H26" s="59">
+      <c r="H26" s="54">
         <v>24</v>
       </c>
-      <c r="I26" s="60" t="s">
+      <c r="I26" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="59" t="s">
+      <c r="J26" s="54" t="s">
         <v>195</v>
       </c>
-      <c r="K26" s="60" t="s">
+      <c r="K26" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="60" t="s">
+      <c r="L26" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="M26" s="60"/>
-      <c r="N26" s="60" t="s">
+      <c r="M26" s="55"/>
+      <c r="N26" s="55" t="s">
         <v>121</v>
       </c>
-      <c r="O26" s="59" t="s">
+      <c r="O26" s="54" t="s">
         <v>188</v>
       </c>
-      <c r="P26" s="59" t="s">
+      <c r="P26" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="61">
+      <c r="Q26" s="56">
         <v>6</v>
       </c>
-      <c r="R26" s="61" t="s">
+      <c r="R26" s="56" t="s">
         <v>123</v>
       </c>
-      <c r="S26" s="61" t="s">
+      <c r="S26" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="T26" s="62" t="s">
+      <c r="T26" s="57" t="s">
         <v>136</v>
       </c>
-      <c r="U26" s="61" t="s">
+      <c r="U26" s="56" t="s">
         <v>199</v>
       </c>
-      <c r="V26" s="61" t="s">
+      <c r="V26" s="56" t="s">
         <v>250</v>
       </c>
       <c r="W26" s="39"/>
-      <c r="X26" s="64">
+      <c r="X26" s="59">
         <v>42419</v>
       </c>
     </row>
@@ -3848,54 +3830,54 @@
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
-      <c r="G27" s="82" t="s">
+      <c r="G27" s="76" t="s">
         <v>278</v>
       </c>
-      <c r="H27" s="82">
+      <c r="H27" s="76">
         <v>25</v>
       </c>
-      <c r="I27" s="83" t="s">
+      <c r="I27" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="82" t="s">
+      <c r="J27" s="76" t="s">
         <v>194</v>
       </c>
-      <c r="K27" s="83" t="s">
+      <c r="K27" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="L27" s="83" t="s">
+      <c r="L27" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="M27" s="83"/>
-      <c r="N27" s="83" t="s">
+      <c r="M27" s="77"/>
+      <c r="N27" s="77" t="s">
         <v>120</v>
       </c>
-      <c r="O27" s="82" t="s">
+      <c r="O27" s="76" t="s">
         <v>189</v>
       </c>
-      <c r="P27" s="82" t="s">
+      <c r="P27" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="84">
+      <c r="Q27" s="78">
         <v>6</v>
       </c>
-      <c r="R27" s="84" t="s">
+      <c r="R27" s="78" t="s">
         <v>123</v>
       </c>
-      <c r="S27" s="84" t="s">
+      <c r="S27" s="78" t="s">
         <v>124</v>
       </c>
-      <c r="T27" s="85" t="s">
+      <c r="T27" s="79" t="s">
         <v>214</v>
       </c>
-      <c r="U27" s="84" t="s">
+      <c r="U27" s="78" t="s">
         <v>199</v>
       </c>
-      <c r="V27" s="80" t="s">
+      <c r="V27" s="74" t="s">
         <v>250</v>
       </c>
       <c r="W27" s="35"/>
-      <c r="X27" s="81">
+      <c r="X27" s="75">
         <v>42422</v>
       </c>
       <c r="Y27" s="3" t="s">
@@ -3964,7 +3946,7 @@
         <v>250</v>
       </c>
       <c r="W28" s="33"/>
-      <c r="X28" s="72">
+      <c r="X28" s="66">
         <v>42423</v>
       </c>
     </row>
@@ -4080,7 +4062,7 @@
         <v>250</v>
       </c>
       <c r="W30" s="21"/>
-      <c r="X30" s="72">
+      <c r="X30" s="66">
         <v>42420</v>
       </c>
     </row>
@@ -4146,7 +4128,7 @@
       <c r="W31" s="44">
         <v>42420</v>
       </c>
-      <c r="X31" s="72">
+      <c r="X31" s="66">
         <v>42420</v>
       </c>
       <c r="Y31" s="3" t="s">
@@ -4577,12 +4559,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4597,6 +4573,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Recurso off line con imágenes
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="279">
   <si>
     <t>Asignatura</t>
   </si>
@@ -815,9 +815,6 @@
     <t>Se debe cambiar motor, recurso off-line enviado a Oliver</t>
   </si>
   <si>
-    <t>Recurso offLine, esperando imágenes, Pedro ya lo subio a GRECO</t>
-  </si>
-  <si>
     <t>Listos 5</t>
   </si>
   <si>
@@ -860,10 +857,13 @@
     <t>Falta la imagen 3</t>
   </si>
   <si>
-    <t>Recurso offline debe subir Pedro y enviar a corrección de estilo</t>
-  </si>
-  <si>
     <t>Me falta ubicar bien las imágenes</t>
+  </si>
+  <si>
+    <t>Recurso offline en carpeta github</t>
+  </si>
+  <si>
+    <t>Recurso offline, falta la imagen 4, sin no la entregan quitar ultima pestaña</t>
   </si>
 </sst>
 </file>
@@ -1264,7 +1264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1538,84 +1538,6 @@
     <xf numFmtId="0" fontId="4" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1630,6 +1552,81 @@
     </xf>
     <xf numFmtId="14" fontId="3" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1937,9 +1934,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GH90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z32" sqref="Z32"/>
+      <selection pane="bottomLeft" activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1971,94 +1968,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="99" t="s">
+      <c r="B1" s="109" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="110" t="s">
+      <c r="C1" s="120" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="101" t="s">
+      <c r="D1" s="111" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="99" t="s">
+      <c r="E1" s="109" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="94" t="s">
+      <c r="F1" s="106" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="103" t="s">
+      <c r="G1" s="113" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="95" t="s">
+      <c r="H1" s="107" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="94" t="s">
+      <c r="I1" s="106" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="107" t="s">
+      <c r="J1" s="117" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="105" t="s">
+      <c r="K1" s="115" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="103" t="s">
+      <c r="L1" s="113" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="109" t="s">
+      <c r="M1" s="119" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="109"/>
-      <c r="O1" s="97" t="s">
+      <c r="N1" s="119"/>
+      <c r="O1" s="98" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="97" t="s">
+      <c r="P1" s="98" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="113" t="s">
+      <c r="Q1" s="100" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="117" t="s">
+      <c r="R1" s="104" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="113" t="s">
+      <c r="S1" s="100" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="115" t="s">
+      <c r="T1" s="102" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="113" t="s">
+      <c r="U1" s="100" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:190" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="102"/>
-      <c r="B2" s="100"/>
-      <c r="C2" s="111"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="96"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="108"/>
-      <c r="K2" s="106"/>
-      <c r="L2" s="104"/>
+      <c r="A2" s="112"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="110"/>
+      <c r="F2" s="122"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="107"/>
+      <c r="J2" s="118"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="114"/>
       <c r="M2" s="31" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
-      <c r="Q2" s="114"/>
-      <c r="R2" s="118"/>
-      <c r="S2" s="114"/>
-      <c r="T2" s="116"/>
-      <c r="U2" s="114"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="99"/>
+      <c r="Q2" s="101"/>
+      <c r="R2" s="105"/>
+      <c r="S2" s="101"/>
+      <c r="T2" s="103"/>
+      <c r="U2" s="101"/>
       <c r="V2" s="24" t="s">
         <v>254</v>
       </c>
@@ -2271,7 +2268,7 @@
         <v>42416</v>
       </c>
       <c r="Y5" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:190" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2491,58 +2488,60 @@
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="30"/>
-      <c r="G9" s="32" t="s">
+      <c r="G9" s="76" t="s">
         <v>147</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="77">
         <v>7</v>
       </c>
-      <c r="I9" s="26" t="s">
+      <c r="I9" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="25" t="s">
+      <c r="J9" s="77" t="s">
         <v>160</v>
       </c>
-      <c r="K9" s="26" t="s">
+      <c r="K9" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="26" t="s">
+      <c r="L9" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26" t="s">
+      <c r="M9" s="78"/>
+      <c r="N9" s="78" t="s">
         <v>120</v>
       </c>
-      <c r="O9" s="25" t="s">
+      <c r="O9" s="77" t="s">
         <v>172</v>
       </c>
-      <c r="P9" s="25" t="s">
+      <c r="P9" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="Q9" s="27">
+      <c r="Q9" s="79">
         <v>6</v>
       </c>
-      <c r="R9" s="27" t="s">
+      <c r="R9" s="79" t="s">
         <v>123</v>
       </c>
-      <c r="S9" s="27" t="s">
+      <c r="S9" s="79" t="s">
         <v>124</v>
       </c>
-      <c r="T9" s="28" t="s">
+      <c r="T9" s="80" t="s">
         <v>125</v>
       </c>
-      <c r="U9" s="27" t="s">
+      <c r="U9" s="79" t="s">
         <v>199</v>
       </c>
       <c r="V9" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="W9" s="21"/>
-      <c r="X9" s="37">
+      <c r="W9" s="81">
+        <v>42451</v>
+      </c>
+      <c r="X9" s="73">
         <v>42417</v>
       </c>
       <c r="Y9" s="5" t="s">
-        <v>262</v>
+        <v>278</v>
       </c>
       <c r="Z9" s="5"/>
       <c r="AA9" s="5"/>
@@ -2976,7 +2975,7 @@
         <v>42443</v>
       </c>
       <c r="Y13" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3246,7 +3245,7 @@
         <v>42419</v>
       </c>
       <c r="Y17" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3656,7 +3655,7 @@
         <v>42419</v>
       </c>
       <c r="X23" s="38" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="1:25" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3790,7 +3789,7 @@
       </c>
       <c r="W25" s="27"/>
       <c r="X25" s="72" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:25" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3879,7 +3878,7 @@
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="68" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H27" s="68">
         <v>25</v>
@@ -3929,7 +3928,7 @@
         <v>42422</v>
       </c>
       <c r="Y27" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="28" spans="1:25" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3993,7 +3992,9 @@
       <c r="V28" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="W28" s="93"/>
+      <c r="W28" s="81">
+        <v>42451</v>
+      </c>
       <c r="X28" s="43">
         <v>42423</v>
       </c>
@@ -4066,60 +4067,60 @@
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
-      <c r="G30" s="119" t="s">
+      <c r="G30" s="93" t="s">
         <v>139</v>
       </c>
-      <c r="H30" s="119">
+      <c r="H30" s="93">
         <v>28</v>
       </c>
-      <c r="I30" s="120" t="s">
+      <c r="I30" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="J30" s="119" t="s">
+      <c r="J30" s="93" t="s">
         <v>165</v>
       </c>
-      <c r="K30" s="120" t="s">
+      <c r="K30" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="L30" s="120" t="s">
+      <c r="L30" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="M30" s="120"/>
-      <c r="N30" s="120" t="s">
+      <c r="M30" s="94"/>
+      <c r="N30" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="O30" s="119" t="s">
+      <c r="O30" s="93" t="s">
         <v>129</v>
       </c>
-      <c r="P30" s="119" t="s">
+      <c r="P30" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="Q30" s="121">
+      <c r="Q30" s="95">
         <v>6</v>
       </c>
-      <c r="R30" s="121" t="s">
+      <c r="R30" s="95" t="s">
         <v>123</v>
       </c>
-      <c r="S30" s="121" t="s">
+      <c r="S30" s="95" t="s">
         <v>124</v>
       </c>
-      <c r="T30" s="122" t="s">
+      <c r="T30" s="96" t="s">
         <v>137</v>
       </c>
-      <c r="U30" s="121" t="s">
+      <c r="U30" s="95" t="s">
         <v>199</v>
       </c>
-      <c r="V30" s="121" t="s">
+      <c r="V30" s="95" t="s">
         <v>250</v>
       </c>
-      <c r="W30" s="123">
+      <c r="W30" s="97">
         <v>42450</v>
       </c>
       <c r="X30" s="43">
         <v>42420</v>
       </c>
       <c r="Y30" s="3" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="31" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4235,10 +4236,10 @@
       <c r="U33" s="16"/>
       <c r="V33" s="17"/>
       <c r="W33" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="X33" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="34" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4264,13 +4265,13 @@
       <c r="T34" s="16"/>
       <c r="U34" s="16"/>
       <c r="V34" s="17" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="W34" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="X34" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4296,13 +4297,13 @@
       <c r="T35" s="16"/>
       <c r="U35" s="16"/>
       <c r="V35" s="17" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="W35" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="X35" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36" spans="1:24" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4612,12 +4613,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4632,6 +4627,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Recurso offline con imágenes
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
@@ -1481,6 +1481,30 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1490,12 +1514,6 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1536,24 +1554,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1864,7 +1864,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y9" sqref="Y9"/>
+      <selection pane="bottomLeft" activeCell="Y17" sqref="Y17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1896,94 +1896,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="95" t="s">
+      <c r="C1" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="86" t="s">
+      <c r="D1" s="92" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="84" t="s">
+      <c r="E1" s="90" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="79" t="s">
+      <c r="F1" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="88" t="s">
+      <c r="G1" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="80" t="s">
+      <c r="H1" s="88" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="79" t="s">
+      <c r="I1" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="92" t="s">
+      <c r="J1" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="90" t="s">
+      <c r="K1" s="96" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="88" t="s">
+      <c r="L1" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="94" t="s">
+      <c r="M1" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="94"/>
-      <c r="O1" s="82" t="s">
+      <c r="N1" s="100"/>
+      <c r="O1" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="82" t="s">
+      <c r="P1" s="79" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="98" t="s">
+      <c r="Q1" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="102" t="s">
+      <c r="R1" s="85" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="98" t="s">
+      <c r="S1" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="100" t="s">
+      <c r="T1" s="83" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="98" t="s">
+      <c r="U1" s="81" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:190" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="87"/>
-      <c r="B2" s="85"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="91"/>
-      <c r="L2" s="89"/>
+      <c r="A2" s="93"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="99"/>
+      <c r="K2" s="97"/>
+      <c r="L2" s="95"/>
       <c r="M2" s="31" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="99"/>
-      <c r="R2" s="103"/>
-      <c r="S2" s="99"/>
-      <c r="T2" s="101"/>
-      <c r="U2" s="99"/>
+      <c r="O2" s="80"/>
+      <c r="P2" s="80"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="86"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="84"/>
+      <c r="U2" s="82"/>
       <c r="V2" s="24" t="s">
         <v>254</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>249</v>
       </c>
       <c r="W17" s="21"/>
-      <c r="X17" s="37">
+      <c r="X17" s="70">
         <v>42419</v>
       </c>
       <c r="Y17" s="3" t="s">
@@ -4544,12 +4544,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4564,6 +4558,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Recursos offline con imágenes
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
+++ b/fuentes/contenidos/grado08/guion09/ESCALETA_MA_08_09_CO.xlsx
@@ -800,9 +800,6 @@
     <t>Imágenes</t>
   </si>
   <si>
-    <t>Duda sobre si se puede debido al tamaño</t>
-  </si>
-  <si>
     <t>No se necesita</t>
   </si>
   <si>
@@ -861,6 +858,9 @@
   </si>
   <si>
     <t>Recurso offline en la carpeta de github, faltan dos imágenes</t>
+  </si>
+  <si>
+    <t>Off line, toca cambiar el motor paara que funcione</t>
   </si>
 </sst>
 </file>
@@ -1249,7 +1249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1352,9 +1352,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="16" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1415,9 +1412,6 @@
     <xf numFmtId="0" fontId="3" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1484,12 +1478,63 @@
     <xf numFmtId="14" fontId="3" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1508,56 +1553,8 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="14" fontId="3" fillId="14" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1865,9 +1862,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GH90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y7" sqref="Y7"/>
+      <selection pane="bottomLeft" activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1899,94 +1896,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:190" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="91" t="s">
+      <c r="B1" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="102" t="s">
+      <c r="C1" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="93" t="s">
+      <c r="D1" s="85" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="91" t="s">
+      <c r="E1" s="83" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="88" t="s">
+      <c r="F1" s="78" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="95" t="s">
+      <c r="G1" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="H1" s="79" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="88" t="s">
+      <c r="I1" s="78" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="99" t="s">
+      <c r="J1" s="91" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="97" t="s">
+      <c r="K1" s="89" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="95" t="s">
+      <c r="L1" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="101" t="s">
+      <c r="M1" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="101"/>
-      <c r="O1" s="80" t="s">
+      <c r="N1" s="93"/>
+      <c r="O1" s="81" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="80" t="s">
+      <c r="P1" s="81" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="82" t="s">
+      <c r="Q1" s="97" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="86" t="s">
+      <c r="R1" s="101" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="82" t="s">
+      <c r="S1" s="97" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="84" t="s">
+      <c r="T1" s="99" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="82" t="s">
+      <c r="U1" s="97" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:190" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="94"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="96"/>
+      <c r="A2" s="86"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="92"/>
+      <c r="K2" s="90"/>
+      <c r="L2" s="88"/>
       <c r="M2" s="31" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="83"/>
-      <c r="R2" s="87"/>
-      <c r="S2" s="83"/>
-      <c r="T2" s="85"/>
-      <c r="U2" s="83"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="98"/>
+      <c r="R2" s="102"/>
+      <c r="S2" s="98"/>
+      <c r="T2" s="100"/>
+      <c r="U2" s="98"/>
       <c r="V2" s="24" t="s">
         <v>254</v>
       </c>
@@ -2012,56 +2009,56 @@
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="29"/>
-      <c r="G3" s="77" t="s">
+      <c r="G3" s="75" t="s">
         <v>223</v>
       </c>
-      <c r="H3" s="53">
+      <c r="H3" s="52">
         <v>1</v>
       </c>
-      <c r="I3" s="54" t="s">
+      <c r="I3" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="53" t="s">
         <v>224</v>
       </c>
-      <c r="K3" s="54" t="s">
+      <c r="K3" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="54" t="s">
+      <c r="L3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="54" t="s">
+      <c r="M3" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="N3" s="54"/>
-      <c r="O3" s="53" t="s">
+      <c r="N3" s="53"/>
+      <c r="O3" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="P3" s="53" t="s">
+      <c r="P3" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="49">
+      <c r="Q3" s="48">
         <v>6</v>
       </c>
-      <c r="R3" s="49" t="s">
+      <c r="R3" s="48" t="s">
         <v>130</v>
       </c>
-      <c r="S3" s="49" t="s">
+      <c r="S3" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="T3" s="55" t="s">
+      <c r="T3" s="54" t="s">
         <v>197</v>
       </c>
-      <c r="U3" s="49" t="s">
+      <c r="U3" s="48" t="s">
         <v>198</v>
       </c>
-      <c r="V3" s="49" t="s">
+      <c r="V3" s="48" t="s">
         <v>251</v>
       </c>
-      <c r="W3" s="51">
+      <c r="W3" s="50">
         <v>42422</v>
       </c>
-      <c r="X3" s="78">
+      <c r="X3" s="76">
         <v>42422</v>
       </c>
     </row>
@@ -2080,56 +2077,56 @@
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="29"/>
-      <c r="G4" s="71" t="s">
+      <c r="G4" s="69" t="s">
         <v>246</v>
       </c>
-      <c r="H4" s="72">
+      <c r="H4" s="70">
         <v>2</v>
       </c>
-      <c r="I4" s="73" t="s">
+      <c r="I4" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="72" t="s">
+      <c r="J4" s="70" t="s">
         <v>158</v>
       </c>
-      <c r="K4" s="73" t="s">
+      <c r="K4" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="73" t="s">
+      <c r="L4" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="73"/>
-      <c r="N4" s="73" t="s">
+      <c r="M4" s="71"/>
+      <c r="N4" s="71" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="72" t="s">
+      <c r="O4" s="70" t="s">
         <v>167</v>
       </c>
-      <c r="P4" s="72" t="s">
+      <c r="P4" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="Q4" s="74">
+      <c r="Q4" s="72">
         <v>6</v>
       </c>
-      <c r="R4" s="74" t="s">
+      <c r="R4" s="72" t="s">
         <v>123</v>
       </c>
-      <c r="S4" s="74" t="s">
+      <c r="S4" s="72" t="s">
         <v>124</v>
       </c>
-      <c r="T4" s="75" t="s">
+      <c r="T4" s="73" t="s">
         <v>134</v>
       </c>
-      <c r="U4" s="74" t="s">
+      <c r="U4" s="72" t="s">
         <v>199</v>
       </c>
       <c r="V4" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="W4" s="76">
+      <c r="W4" s="74">
         <v>42453</v>
       </c>
-      <c r="X4" s="62">
+      <c r="X4" s="60">
         <v>42416</v>
       </c>
     </row>
@@ -2148,32 +2145,32 @@
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="29"/>
-      <c r="G5" s="46" t="s">
+      <c r="G5" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="H5" s="39">
+      <c r="H5" s="38">
         <v>3</v>
       </c>
-      <c r="I5" s="40" t="s">
+      <c r="I5" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="39" t="s">
+      <c r="J5" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="K5" s="40" t="s">
+      <c r="K5" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L5" s="40" t="s">
+      <c r="L5" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M5" s="40"/>
-      <c r="N5" s="40" t="s">
+      <c r="M5" s="39"/>
+      <c r="N5" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="O5" s="39" t="s">
+      <c r="O5" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="P5" s="39" t="s">
+      <c r="P5" s="38" t="s">
         <v>19</v>
       </c>
       <c r="Q5" s="34">
@@ -2185,7 +2182,7 @@
       <c r="S5" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T5" s="48" t="s">
+      <c r="T5" s="47" t="s">
         <v>202</v>
       </c>
       <c r="U5" s="34" t="s">
@@ -2194,10 +2191,10 @@
       <c r="V5" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="W5" s="42">
+      <c r="W5" s="41">
         <v>42450</v>
       </c>
-      <c r="X5" s="62">
+      <c r="X5" s="60">
         <v>42416</v>
       </c>
     </row>
@@ -2236,7 +2233,7 @@
       </c>
       <c r="M6" s="26"/>
       <c r="N6" s="26" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="O6" s="25" t="s">
         <v>169</v>
@@ -2263,11 +2260,11 @@
         <v>249</v>
       </c>
       <c r="W6" s="21"/>
-      <c r="X6" s="62">
+      <c r="X6" s="60">
         <v>42416</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>257</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2285,55 +2282,55 @@
       </c>
       <c r="E7" s="9"/>
       <c r="F7" s="29"/>
-      <c r="G7" s="43" t="s">
+      <c r="G7" s="42" t="s">
         <v>145</v>
       </c>
-      <c r="H7" s="39">
+      <c r="H7" s="38">
         <v>5</v>
       </c>
-      <c r="I7" s="40" t="s">
+      <c r="I7" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="39" t="s">
+      <c r="J7" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="K7" s="44" t="s">
+      <c r="K7" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="40" t="s">
+      <c r="L7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="40"/>
-      <c r="N7" s="40"/>
-      <c r="O7" s="39" t="s">
+      <c r="M7" s="39"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="P7" s="39" t="s">
+      <c r="P7" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="45">
+      <c r="Q7" s="44">
         <v>9</v>
       </c>
-      <c r="R7" s="45" t="s">
+      <c r="R7" s="44" t="s">
         <v>128</v>
       </c>
-      <c r="S7" s="45" t="s">
+      <c r="S7" s="44" t="s">
         <v>219</v>
       </c>
-      <c r="T7" s="45" t="s">
+      <c r="T7" s="44" t="s">
         <v>220</v>
       </c>
-      <c r="U7" s="45" t="s">
+      <c r="U7" s="44" t="s">
         <v>221</v>
       </c>
       <c r="V7" s="34" t="s">
         <v>222</v>
       </c>
-      <c r="W7" s="42">
+      <c r="W7" s="41">
         <v>42416</v>
       </c>
-      <c r="X7" s="37" t="s">
-        <v>258</v>
+      <c r="X7" s="36" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2351,32 +2348,32 @@
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="29"/>
-      <c r="G8" s="46" t="s">
+      <c r="G8" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="H8" s="39">
+      <c r="H8" s="38">
         <v>6</v>
       </c>
-      <c r="I8" s="40" t="s">
+      <c r="I8" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="64" t="s">
+      <c r="J8" s="62" t="s">
         <v>227</v>
       </c>
-      <c r="K8" s="40" t="s">
+      <c r="K8" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="40" t="s">
+      <c r="L8" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="M8" s="40" t="s">
+      <c r="M8" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="N8" s="40"/>
-      <c r="O8" s="39" t="s">
+      <c r="N8" s="39"/>
+      <c r="O8" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="P8" s="39" t="s">
+      <c r="P8" s="38" t="s">
         <v>19</v>
       </c>
       <c r="Q8" s="34">
@@ -2388,7 +2385,7 @@
       <c r="S8" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="T8" s="48" t="s">
+      <c r="T8" s="47" t="s">
         <v>132</v>
       </c>
       <c r="U8" s="34" t="s">
@@ -2397,10 +2394,10 @@
       <c r="V8" s="34" t="s">
         <v>251</v>
       </c>
-      <c r="W8" s="76">
+      <c r="W8" s="74">
         <v>42453</v>
       </c>
-      <c r="X8" s="36">
+      <c r="X8" s="60">
         <v>42429</v>
       </c>
       <c r="Y8" s="5"/>
@@ -2420,32 +2417,32 @@
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="30"/>
-      <c r="G9" s="46" t="s">
+      <c r="G9" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="H9" s="39">
+      <c r="H9" s="38">
         <v>7</v>
       </c>
-      <c r="I9" s="40" t="s">
+      <c r="I9" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="J9" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="K9" s="40" t="s">
+      <c r="K9" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="40" t="s">
+      <c r="L9" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="40"/>
-      <c r="N9" s="40" t="s">
+      <c r="M9" s="39"/>
+      <c r="N9" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="O9" s="39" t="s">
+      <c r="O9" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="P9" s="39" t="s">
+      <c r="P9" s="38" t="s">
         <v>20</v>
       </c>
       <c r="Q9" s="34">
@@ -2457,7 +2454,7 @@
       <c r="S9" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T9" s="48" t="s">
+      <c r="T9" s="47" t="s">
         <v>125</v>
       </c>
       <c r="U9" s="34" t="s">
@@ -2466,10 +2463,10 @@
       <c r="V9" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="W9" s="42">
+      <c r="W9" s="41">
         <v>42451</v>
       </c>
-      <c r="X9" s="62">
+      <c r="X9" s="60">
         <v>42417</v>
       </c>
       <c r="Y9" s="5"/>
@@ -2654,32 +2651,32 @@
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="29"/>
-      <c r="G10" s="46" t="s">
+      <c r="G10" s="45" t="s">
         <v>228</v>
       </c>
-      <c r="H10" s="39">
+      <c r="H10" s="38">
         <v>8</v>
       </c>
-      <c r="I10" s="40" t="s">
+      <c r="I10" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="39" t="s">
+      <c r="J10" s="38" t="s">
         <v>229</v>
       </c>
-      <c r="K10" s="40" t="s">
+      <c r="K10" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="40" t="s">
+      <c r="L10" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="M10" s="40" t="s">
+      <c r="M10" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="N10" s="40"/>
-      <c r="O10" s="39" t="s">
+      <c r="N10" s="39"/>
+      <c r="O10" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="P10" s="39" t="s">
+      <c r="P10" s="38" t="s">
         <v>19</v>
       </c>
       <c r="Q10" s="34">
@@ -2691,7 +2688,7 @@
       <c r="S10" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="T10" s="48" t="s">
+      <c r="T10" s="47" t="s">
         <v>204</v>
       </c>
       <c r="U10" s="34" t="s">
@@ -2700,12 +2697,12 @@
       <c r="V10" s="34" t="s">
         <v>252</v>
       </c>
-      <c r="W10" s="42">
+      <c r="W10" s="41">
         <v>42451</v>
       </c>
-      <c r="X10" s="70"/>
+      <c r="X10" s="68"/>
       <c r="Y10" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2723,32 +2720,32 @@
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="29"/>
-      <c r="G11" s="46" t="s">
-        <v>259</v>
-      </c>
-      <c r="H11" s="39">
+      <c r="G11" s="45" t="s">
+        <v>258</v>
+      </c>
+      <c r="H11" s="38">
         <v>9</v>
       </c>
-      <c r="I11" s="40" t="s">
+      <c r="I11" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="39" t="s">
+      <c r="J11" s="38" t="s">
         <v>230</v>
       </c>
-      <c r="K11" s="40" t="s">
+      <c r="K11" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L11" s="40" t="s">
+      <c r="L11" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M11" s="40"/>
-      <c r="N11" s="40" t="s">
+      <c r="M11" s="39"/>
+      <c r="N11" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="O11" s="47" t="s">
+      <c r="O11" s="46" t="s">
         <v>217</v>
       </c>
-      <c r="P11" s="39" t="s">
+      <c r="P11" s="38" t="s">
         <v>19</v>
       </c>
       <c r="Q11" s="34">
@@ -2760,7 +2757,7 @@
       <c r="S11" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T11" s="48" t="s">
+      <c r="T11" s="47" t="s">
         <v>209</v>
       </c>
       <c r="U11" s="34" t="s">
@@ -2769,11 +2766,11 @@
       <c r="V11" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="W11" s="42">
+      <c r="W11" s="41">
         <v>42416</v>
       </c>
-      <c r="X11" s="37" t="s">
-        <v>258</v>
+      <c r="X11" s="36" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2791,32 +2788,32 @@
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="29"/>
-      <c r="G12" s="46" t="s">
+      <c r="G12" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="H12" s="39">
+      <c r="H12" s="38">
         <v>10</v>
       </c>
-      <c r="I12" s="40" t="s">
+      <c r="I12" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="39" t="s">
+      <c r="J12" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="K12" s="40" t="s">
+      <c r="K12" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L12" s="40" t="s">
+      <c r="L12" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M12" s="40"/>
-      <c r="N12" s="40" t="s">
+      <c r="M12" s="39"/>
+      <c r="N12" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="O12" s="39" t="s">
+      <c r="O12" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="P12" s="39" t="s">
+      <c r="P12" s="38" t="s">
         <v>19</v>
       </c>
       <c r="Q12" s="34">
@@ -2828,7 +2825,7 @@
       <c r="S12" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T12" s="48" t="s">
+      <c r="T12" s="47" t="s">
         <v>126</v>
       </c>
       <c r="U12" s="34" t="s">
@@ -2837,10 +2834,10 @@
       <c r="V12" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="W12" s="42">
+      <c r="W12" s="41">
         <v>42451</v>
       </c>
-      <c r="X12" s="62">
+      <c r="X12" s="60">
         <v>42418</v>
       </c>
     </row>
@@ -2859,32 +2856,32 @@
       </c>
       <c r="E13" s="9"/>
       <c r="F13" s="29"/>
-      <c r="G13" s="46" t="s">
+      <c r="G13" s="45" t="s">
         <v>149</v>
       </c>
-      <c r="H13" s="39">
+      <c r="H13" s="38">
         <v>11</v>
       </c>
-      <c r="I13" s="40" t="s">
+      <c r="I13" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="39" t="s">
+      <c r="J13" s="38" t="s">
         <v>232</v>
       </c>
-      <c r="K13" s="40" t="s">
+      <c r="K13" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="40" t="s">
+      <c r="L13" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="M13" s="40" t="s">
+      <c r="M13" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="N13" s="40"/>
-      <c r="O13" s="39" t="s">
+      <c r="N13" s="39"/>
+      <c r="O13" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="P13" s="39" t="s">
+      <c r="P13" s="38" t="s">
         <v>19</v>
       </c>
       <c r="Q13" s="34">
@@ -2896,7 +2893,7 @@
       <c r="S13" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="T13" s="48" t="s">
+      <c r="T13" s="47" t="s">
         <v>206</v>
       </c>
       <c r="U13" s="34" t="s">
@@ -2905,14 +2902,14 @@
       <c r="V13" s="34" t="s">
         <v>253</v>
       </c>
-      <c r="W13" s="42">
+      <c r="W13" s="41">
         <v>42450</v>
       </c>
-      <c r="X13" s="62">
+      <c r="X13" s="60">
         <v>42443</v>
       </c>
       <c r="Y13" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2930,32 +2927,32 @@
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="29"/>
-      <c r="G14" s="46" t="s">
-        <v>260</v>
-      </c>
-      <c r="H14" s="39">
+      <c r="G14" s="45" t="s">
+        <v>259</v>
+      </c>
+      <c r="H14" s="38">
         <v>12</v>
       </c>
-      <c r="I14" s="40" t="s">
+      <c r="I14" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="39" t="s">
+      <c r="J14" s="38" t="s">
         <v>233</v>
       </c>
-      <c r="K14" s="40" t="s">
+      <c r="K14" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="40" t="s">
+      <c r="L14" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="40"/>
-      <c r="N14" s="40" t="s">
+      <c r="M14" s="39"/>
+      <c r="N14" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="O14" s="39" t="s">
+      <c r="O14" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="P14" s="39" t="s">
+      <c r="P14" s="38" t="s">
         <v>19</v>
       </c>
       <c r="Q14" s="34">
@@ -2967,7 +2964,7 @@
       <c r="S14" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T14" s="48" t="s">
+      <c r="T14" s="47" t="s">
         <v>208</v>
       </c>
       <c r="U14" s="34" t="s">
@@ -2977,11 +2974,11 @@
         <v>249</v>
       </c>
       <c r="W14" s="33"/>
-      <c r="X14" s="62">
+      <c r="X14" s="60">
         <v>42417</v>
       </c>
       <c r="Y14" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:190" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2999,32 +2996,32 @@
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="29"/>
-      <c r="G15" s="46" t="s">
+      <c r="G15" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="H15" s="39">
+      <c r="H15" s="38">
         <v>13</v>
       </c>
-      <c r="I15" s="40" t="s">
+      <c r="I15" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="39" t="s">
+      <c r="J15" s="38" t="s">
         <v>235</v>
       </c>
-      <c r="K15" s="40" t="s">
+      <c r="K15" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L15" s="40" t="s">
+      <c r="L15" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M15" s="40"/>
-      <c r="N15" s="40" t="s">
+      <c r="M15" s="39"/>
+      <c r="N15" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="O15" s="39" t="s">
+      <c r="O15" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="P15" s="39" t="s">
+      <c r="P15" s="38" t="s">
         <v>19</v>
       </c>
       <c r="Q15" s="34">
@@ -3036,7 +3033,7 @@
       <c r="S15" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T15" s="48" t="s">
+      <c r="T15" s="47" t="s">
         <v>210</v>
       </c>
       <c r="U15" s="34" t="s">
@@ -3045,10 +3042,10 @@
       <c r="V15" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="W15" s="42">
+      <c r="W15" s="41">
         <v>42451</v>
       </c>
-      <c r="X15" s="62">
+      <c r="X15" s="60">
         <v>42418</v>
       </c>
     </row>
@@ -3067,32 +3064,32 @@
       </c>
       <c r="E16" s="9"/>
       <c r="F16" s="29"/>
-      <c r="G16" s="46" t="s">
+      <c r="G16" s="45" t="s">
         <v>236</v>
       </c>
-      <c r="H16" s="39">
+      <c r="H16" s="38">
         <v>14</v>
       </c>
-      <c r="I16" s="40" t="s">
+      <c r="I16" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="39" t="s">
+      <c r="J16" s="38" t="s">
         <v>237</v>
       </c>
-      <c r="K16" s="40" t="s">
+      <c r="K16" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L16" s="40" t="s">
+      <c r="L16" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M16" s="40"/>
-      <c r="N16" s="40" t="s">
+      <c r="M16" s="39"/>
+      <c r="N16" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="O16" s="39" t="s">
+      <c r="O16" s="38" t="s">
         <v>178</v>
       </c>
-      <c r="P16" s="39" t="s">
+      <c r="P16" s="38" t="s">
         <v>19</v>
       </c>
       <c r="Q16" s="34">
@@ -3104,7 +3101,7 @@
       <c r="S16" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T16" s="48" t="s">
+      <c r="T16" s="47" t="s">
         <v>138</v>
       </c>
       <c r="U16" s="34" t="s">
@@ -3114,7 +3111,7 @@
         <v>249</v>
       </c>
       <c r="W16" s="21"/>
-      <c r="X16" s="36">
+      <c r="X16" s="60">
         <v>42431</v>
       </c>
     </row>
@@ -3133,60 +3130,60 @@
       </c>
       <c r="E17" s="9"/>
       <c r="F17" s="29"/>
-      <c r="G17" s="71" t="s">
+      <c r="G17" s="69" t="s">
         <v>150</v>
       </c>
-      <c r="H17" s="72">
+      <c r="H17" s="70">
         <v>15</v>
       </c>
-      <c r="I17" s="73" t="s">
+      <c r="I17" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="72" t="s">
+      <c r="J17" s="70" t="s">
         <v>161</v>
       </c>
-      <c r="K17" s="73" t="s">
+      <c r="K17" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="L17" s="73" t="s">
+      <c r="L17" s="71" t="s">
         <v>8</v>
       </c>
-      <c r="M17" s="73"/>
-      <c r="N17" s="73" t="s">
+      <c r="M17" s="71"/>
+      <c r="N17" s="71" t="s">
         <v>120</v>
       </c>
-      <c r="O17" s="72" t="s">
+      <c r="O17" s="70" t="s">
         <v>179</v>
       </c>
-      <c r="P17" s="72" t="s">
+      <c r="P17" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="Q17" s="74">
+      <c r="Q17" s="72">
         <v>6</v>
       </c>
-      <c r="R17" s="74" t="s">
+      <c r="R17" s="72" t="s">
         <v>123</v>
       </c>
-      <c r="S17" s="74" t="s">
+      <c r="S17" s="72" t="s">
         <v>124</v>
       </c>
-      <c r="T17" s="75" t="s">
+      <c r="T17" s="73" t="s">
         <v>125</v>
       </c>
-      <c r="U17" s="74" t="s">
+      <c r="U17" s="72" t="s">
         <v>199</v>
       </c>
       <c r="V17" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="W17" s="76">
+      <c r="W17" s="74">
         <v>42423</v>
       </c>
-      <c r="X17" s="62">
+      <c r="X17" s="60">
         <v>42419</v>
       </c>
       <c r="Y17" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3204,32 +3201,32 @@
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="29"/>
-      <c r="G18" s="46" t="s">
+      <c r="G18" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="H18" s="39">
+      <c r="H18" s="38">
         <v>16</v>
       </c>
-      <c r="I18" s="40" t="s">
+      <c r="I18" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="39" t="s">
+      <c r="J18" s="38" t="s">
         <v>238</v>
       </c>
-      <c r="K18" s="40" t="s">
+      <c r="K18" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="40" t="s">
+      <c r="L18" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M18" s="40"/>
-      <c r="N18" s="40" t="s">
+      <c r="M18" s="39"/>
+      <c r="N18" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="O18" s="39" t="s">
+      <c r="O18" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="P18" s="39" t="s">
+      <c r="P18" s="38" t="s">
         <v>19</v>
       </c>
       <c r="Q18" s="34">
@@ -3241,7 +3238,7 @@
       <c r="S18" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T18" s="48" t="s">
+      <c r="T18" s="47" t="s">
         <v>211</v>
       </c>
       <c r="U18" s="34" t="s">
@@ -3250,10 +3247,10 @@
       <c r="V18" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="W18" s="42">
+      <c r="W18" s="41">
         <v>42447</v>
       </c>
-      <c r="X18" s="62">
+      <c r="X18" s="60">
         <v>42419</v>
       </c>
     </row>
@@ -3274,56 +3271,56 @@
         <v>127</v>
       </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="66" t="s">
+      <c r="G19" s="64" t="s">
         <v>152</v>
       </c>
-      <c r="H19" s="67">
+      <c r="H19" s="65">
         <v>17</v>
       </c>
-      <c r="I19" s="68" t="s">
+      <c r="I19" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="67" t="s">
+      <c r="J19" s="65" t="s">
         <v>162</v>
       </c>
-      <c r="K19" s="68" t="s">
+      <c r="K19" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="L19" s="68" t="s">
+      <c r="L19" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="M19" s="68"/>
-      <c r="N19" s="68" t="s">
+      <c r="M19" s="66"/>
+      <c r="N19" s="66" t="s">
         <v>121</v>
       </c>
-      <c r="O19" s="67" t="s">
+      <c r="O19" s="65" t="s">
         <v>181</v>
       </c>
-      <c r="P19" s="67" t="s">
+      <c r="P19" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="Q19" s="50">
+      <c r="Q19" s="49">
         <v>6</v>
       </c>
-      <c r="R19" s="50" t="s">
+      <c r="R19" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="S19" s="50" t="s">
+      <c r="S19" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="T19" s="69" t="s">
+      <c r="T19" s="67" t="s">
         <v>212</v>
       </c>
-      <c r="U19" s="50" t="s">
+      <c r="U19" s="49" t="s">
         <v>199</v>
       </c>
-      <c r="V19" s="50" t="s">
+      <c r="V19" s="49" t="s">
         <v>250</v>
       </c>
-      <c r="W19" s="63">
+      <c r="W19" s="61">
         <v>42419</v>
       </c>
-      <c r="X19" s="65">
+      <c r="X19" s="63">
         <v>42419</v>
       </c>
     </row>
@@ -3341,58 +3338,58 @@
         <v>192</v>
       </c>
       <c r="E20" s="7"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="52" t="s">
+      <c r="F20" s="37"/>
+      <c r="G20" s="51" t="s">
         <v>239</v>
       </c>
-      <c r="H20" s="53">
+      <c r="H20" s="52">
         <v>18</v>
       </c>
-      <c r="I20" s="54" t="s">
+      <c r="I20" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="J20" s="53" t="s">
+      <c r="J20" s="52" t="s">
         <v>240</v>
       </c>
-      <c r="K20" s="54" t="s">
+      <c r="K20" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="L20" s="54" t="s">
+      <c r="L20" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="M20" s="54"/>
-      <c r="N20" s="54" t="s">
+      <c r="M20" s="53"/>
+      <c r="N20" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="O20" s="53" t="s">
+      <c r="O20" s="52" t="s">
         <v>182</v>
       </c>
-      <c r="P20" s="53" t="s">
+      <c r="P20" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="49">
+      <c r="Q20" s="48">
         <v>6</v>
       </c>
-      <c r="R20" s="49" t="s">
+      <c r="R20" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="S20" s="49" t="s">
+      <c r="S20" s="48" t="s">
         <v>124</v>
       </c>
-      <c r="T20" s="55" t="s">
+      <c r="T20" s="54" t="s">
         <v>209</v>
       </c>
-      <c r="U20" s="49" t="s">
+      <c r="U20" s="48" t="s">
         <v>199</v>
       </c>
-      <c r="V20" s="49" t="s">
+      <c r="V20" s="48" t="s">
         <v>250</v>
       </c>
-      <c r="W20" s="51">
+      <c r="W20" s="50">
         <v>42418</v>
       </c>
       <c r="X20" s="35" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3409,33 +3406,33 @@
         <v>192</v>
       </c>
       <c r="E21" s="7"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="46" t="s">
+      <c r="F21" s="37"/>
+      <c r="G21" s="45" t="s">
         <v>153</v>
       </c>
-      <c r="H21" s="39">
+      <c r="H21" s="38">
         <v>19</v>
       </c>
-      <c r="I21" s="40" t="s">
+      <c r="I21" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J21" s="39" t="s">
+      <c r="J21" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="K21" s="40" t="s">
+      <c r="K21" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L21" s="40" t="s">
+      <c r="L21" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M21" s="40"/>
-      <c r="N21" s="40" t="s">
+      <c r="M21" s="39"/>
+      <c r="N21" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="O21" s="39" t="s">
+      <c r="O21" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="P21" s="39" t="s">
+      <c r="P21" s="38" t="s">
         <v>19</v>
       </c>
       <c r="Q21" s="34">
@@ -3447,7 +3444,7 @@
       <c r="S21" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T21" s="48" t="s">
+      <c r="T21" s="47" t="s">
         <v>133</v>
       </c>
       <c r="U21" s="34" t="s">
@@ -3456,11 +3453,11 @@
       <c r="V21" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="W21" s="42">
+      <c r="W21" s="41">
         <v>42418</v>
       </c>
-      <c r="X21" s="37" t="s">
-        <v>258</v>
+      <c r="X21" s="36" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -3477,33 +3474,33 @@
         <v>192</v>
       </c>
       <c r="E22" s="7"/>
-      <c r="F22" s="38"/>
-      <c r="G22" s="46" t="s">
+      <c r="F22" s="37"/>
+      <c r="G22" s="45" t="s">
         <v>241</v>
       </c>
-      <c r="H22" s="39">
+      <c r="H22" s="38">
         <v>20</v>
       </c>
-      <c r="I22" s="40" t="s">
+      <c r="I22" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="64" t="s">
+      <c r="J22" s="62" t="s">
         <v>242</v>
       </c>
-      <c r="K22" s="40" t="s">
+      <c r="K22" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L22" s="40" t="s">
+      <c r="L22" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M22" s="40"/>
-      <c r="N22" s="40" t="s">
+      <c r="M22" s="39"/>
+      <c r="N22" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="O22" s="39" t="s">
+      <c r="O22" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="P22" s="39" t="s">
+      <c r="P22" s="38" t="s">
         <v>19</v>
       </c>
       <c r="Q22" s="34">
@@ -3515,7 +3512,7 @@
       <c r="S22" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T22" s="48" t="s">
+      <c r="T22" s="47" t="s">
         <v>200</v>
       </c>
       <c r="U22" s="34" t="s">
@@ -3524,10 +3521,10 @@
       <c r="V22" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="W22" s="42">
+      <c r="W22" s="41">
         <v>42447</v>
       </c>
-      <c r="X22" s="62">
+      <c r="X22" s="60">
         <v>42419</v>
       </c>
     </row>
@@ -3545,33 +3542,33 @@
         <v>192</v>
       </c>
       <c r="E23" s="7"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="46" t="s">
+      <c r="F23" s="37"/>
+      <c r="G23" s="45" t="s">
         <v>154</v>
       </c>
-      <c r="H23" s="39">
+      <c r="H23" s="38">
         <v>21</v>
       </c>
-      <c r="I23" s="40" t="s">
+      <c r="I23" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J23" s="39" t="s">
+      <c r="J23" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="K23" s="40" t="s">
+      <c r="K23" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="40" t="s">
+      <c r="L23" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M23" s="40"/>
-      <c r="N23" s="40" t="s">
+      <c r="M23" s="39"/>
+      <c r="N23" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="O23" s="39" t="s">
+      <c r="O23" s="38" t="s">
         <v>185</v>
       </c>
-      <c r="P23" s="39" t="s">
+      <c r="P23" s="38" t="s">
         <v>19</v>
       </c>
       <c r="Q23" s="34">
@@ -3583,7 +3580,7 @@
       <c r="S23" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T23" s="48" t="s">
+      <c r="T23" s="47" t="s">
         <v>213</v>
       </c>
       <c r="U23" s="34" t="s">
@@ -3592,11 +3589,11 @@
       <c r="V23" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="W23" s="42">
+      <c r="W23" s="41">
         <v>42419</v>
       </c>
-      <c r="X23" s="37" t="s">
-        <v>264</v>
+      <c r="X23" s="36" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="24" spans="1:25" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3613,33 +3610,33 @@
         <v>192</v>
       </c>
       <c r="E24" s="7"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="46" t="s">
+      <c r="F24" s="37"/>
+      <c r="G24" s="45" t="s">
         <v>247</v>
       </c>
-      <c r="H24" s="39">
+      <c r="H24" s="38">
         <v>22</v>
       </c>
-      <c r="I24" s="40" t="s">
+      <c r="I24" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J24" s="39" t="s">
+      <c r="J24" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="K24" s="40" t="s">
+      <c r="K24" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L24" s="40" t="s">
+      <c r="L24" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M24" s="40"/>
-      <c r="N24" s="40" t="s">
+      <c r="M24" s="39"/>
+      <c r="N24" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="O24" s="39" t="s">
+      <c r="O24" s="38" t="s">
         <v>186</v>
       </c>
-      <c r="P24" s="39" t="s">
+      <c r="P24" s="38" t="s">
         <v>19</v>
       </c>
       <c r="Q24" s="34">
@@ -3651,7 +3648,7 @@
       <c r="S24" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T24" s="48" t="s">
+      <c r="T24" s="47" t="s">
         <v>201</v>
       </c>
       <c r="U24" s="34" t="s">
@@ -3660,10 +3657,10 @@
       <c r="V24" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="W24" s="42">
+      <c r="W24" s="41">
         <v>42450</v>
       </c>
-      <c r="X24" s="62">
+      <c r="X24" s="60">
         <v>42423</v>
       </c>
     </row>
@@ -3681,33 +3678,33 @@
         <v>192</v>
       </c>
       <c r="E25" s="7"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="46" t="s">
+      <c r="F25" s="37"/>
+      <c r="G25" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="H25" s="39">
+      <c r="H25" s="38">
         <v>23</v>
       </c>
-      <c r="I25" s="40" t="s">
+      <c r="I25" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J25" s="64" t="s">
+      <c r="J25" s="62" t="s">
         <v>248</v>
       </c>
-      <c r="K25" s="40" t="s">
+      <c r="K25" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L25" s="40" t="s">
+      <c r="L25" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="M25" s="40" t="s">
+      <c r="M25" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="N25" s="40"/>
-      <c r="O25" s="39" t="s">
+      <c r="N25" s="39"/>
+      <c r="O25" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="P25" s="39" t="s">
+      <c r="P25" s="38" t="s">
         <v>19</v>
       </c>
       <c r="Q25" s="34">
@@ -3719,7 +3716,7 @@
       <c r="S25" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="T25" s="48" t="s">
+      <c r="T25" s="47" t="s">
         <v>207</v>
       </c>
       <c r="U25" s="34" t="s">
@@ -3728,11 +3725,11 @@
       <c r="V25" s="34" t="s">
         <v>253</v>
       </c>
-      <c r="W25" s="42">
+      <c r="W25" s="41">
         <v>42451</v>
       </c>
-      <c r="X25" s="70" t="s">
-        <v>272</v>
+      <c r="X25" s="68" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="26" spans="1:25" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -3751,57 +3748,57 @@
       <c r="E26" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="F26" s="38"/>
-      <c r="G26" s="66" t="s">
+      <c r="F26" s="37"/>
+      <c r="G26" s="64" t="s">
         <v>156</v>
       </c>
-      <c r="H26" s="67">
+      <c r="H26" s="65">
         <v>24</v>
       </c>
-      <c r="I26" s="68" t="s">
+      <c r="I26" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="67" t="s">
+      <c r="J26" s="65" t="s">
         <v>195</v>
       </c>
-      <c r="K26" s="68" t="s">
+      <c r="K26" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="68" t="s">
+      <c r="L26" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="M26" s="68"/>
-      <c r="N26" s="68" t="s">
+      <c r="M26" s="66"/>
+      <c r="N26" s="66" t="s">
         <v>121</v>
       </c>
-      <c r="O26" s="67" t="s">
+      <c r="O26" s="65" t="s">
         <v>188</v>
       </c>
-      <c r="P26" s="67" t="s">
+      <c r="P26" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="Q26" s="50">
+      <c r="Q26" s="49">
         <v>6</v>
       </c>
-      <c r="R26" s="50" t="s">
+      <c r="R26" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="S26" s="50" t="s">
+      <c r="S26" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="T26" s="69" t="s">
+      <c r="T26" s="67" t="s">
         <v>136</v>
       </c>
-      <c r="U26" s="50" t="s">
+      <c r="U26" s="49" t="s">
         <v>199</v>
       </c>
-      <c r="V26" s="50" t="s">
+      <c r="V26" s="49" t="s">
         <v>250</v>
       </c>
-      <c r="W26" s="63">
+      <c r="W26" s="61">
         <v>42450</v>
       </c>
-      <c r="X26" s="65">
+      <c r="X26" s="63">
         <v>42419</v>
       </c>
     </row>
@@ -3820,60 +3817,60 @@
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
-      <c r="G27" s="58" t="s">
-        <v>271</v>
-      </c>
-      <c r="H27" s="58">
+      <c r="G27" s="56" t="s">
+        <v>270</v>
+      </c>
+      <c r="H27" s="56">
         <v>25</v>
       </c>
-      <c r="I27" s="59" t="s">
+      <c r="I27" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="J27" s="58" t="s">
+      <c r="J27" s="56" t="s">
         <v>194</v>
       </c>
-      <c r="K27" s="59" t="s">
+      <c r="K27" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="L27" s="59" t="s">
+      <c r="L27" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="M27" s="59"/>
-      <c r="N27" s="59" t="s">
+      <c r="M27" s="57"/>
+      <c r="N27" s="57" t="s">
         <v>120</v>
       </c>
-      <c r="O27" s="58" t="s">
+      <c r="O27" s="56" t="s">
         <v>189</v>
       </c>
-      <c r="P27" s="58" t="s">
+      <c r="P27" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="Q27" s="60">
+      <c r="Q27" s="58">
         <v>6</v>
       </c>
-      <c r="R27" s="60" t="s">
+      <c r="R27" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="S27" s="60" t="s">
+      <c r="S27" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="T27" s="61" t="s">
+      <c r="T27" s="59" t="s">
         <v>214</v>
       </c>
-      <c r="U27" s="60" t="s">
+      <c r="U27" s="58" t="s">
         <v>199</v>
       </c>
-      <c r="V27" s="56" t="s">
+      <c r="V27" s="55" t="s">
         <v>250</v>
       </c>
-      <c r="W27" s="79">
+      <c r="W27" s="77">
         <v>42453</v>
       </c>
-      <c r="X27" s="57">
+      <c r="X27" s="103">
         <v>42422</v>
       </c>
       <c r="Y27" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:25" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3891,32 +3888,32 @@
       </c>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
-      <c r="G28" s="39" t="s">
+      <c r="G28" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="H28" s="39">
+      <c r="H28" s="38">
         <v>26</v>
       </c>
-      <c r="I28" s="40" t="s">
+      <c r="I28" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J28" s="39" t="s">
+      <c r="J28" s="38" t="s">
         <v>244</v>
       </c>
-      <c r="K28" s="40" t="s">
+      <c r="K28" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L28" s="40" t="s">
+      <c r="L28" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M28" s="40"/>
-      <c r="N28" s="40" t="s">
+      <c r="M28" s="39"/>
+      <c r="N28" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="O28" s="39" t="s">
+      <c r="O28" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="P28" s="39" t="s">
+      <c r="P28" s="38" t="s">
         <v>19</v>
       </c>
       <c r="Q28" s="34">
@@ -3928,7 +3925,7 @@
       <c r="S28" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T28" s="48" t="s">
+      <c r="T28" s="47" t="s">
         <v>215</v>
       </c>
       <c r="U28" s="34" t="s">
@@ -3937,14 +3934,14 @@
       <c r="V28" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="W28" s="42">
+      <c r="W28" s="41">
         <v>42451</v>
       </c>
-      <c r="X28" s="42">
+      <c r="X28" s="41">
         <v>42423</v>
       </c>
       <c r="Y28" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="29" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -3962,39 +3959,39 @@
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
-      <c r="G29" s="39" t="s">
+      <c r="G29" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="H29" s="39">
+      <c r="H29" s="38">
         <v>27</v>
       </c>
-      <c r="I29" s="40" t="s">
+      <c r="I29" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="39" t="s">
+      <c r="J29" s="38" t="s">
         <v>245</v>
       </c>
-      <c r="K29" s="40" t="s">
+      <c r="K29" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L29" s="40" t="s">
+      <c r="L29" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="M29" s="40"/>
-      <c r="N29" s="40"/>
-      <c r="O29" s="39"/>
-      <c r="P29" s="39" t="s">
+      <c r="M29" s="39"/>
+      <c r="N29" s="39"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="Q29" s="39"/>
-      <c r="R29" s="39"/>
-      <c r="S29" s="39"/>
-      <c r="T29" s="41"/>
-      <c r="U29" s="39"/>
+      <c r="Q29" s="38"/>
+      <c r="R29" s="38"/>
+      <c r="S29" s="38"/>
+      <c r="T29" s="40"/>
+      <c r="U29" s="38"/>
       <c r="V29" s="34"/>
       <c r="W29" s="34"/>
       <c r="X29" s="33" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="30" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4012,32 +4009,32 @@
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
-      <c r="G30" s="39" t="s">
+      <c r="G30" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="H30" s="39">
+      <c r="H30" s="38">
         <v>28</v>
       </c>
-      <c r="I30" s="40" t="s">
+      <c r="I30" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J30" s="39" t="s">
+      <c r="J30" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="K30" s="40" t="s">
+      <c r="K30" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L30" s="40" t="s">
+      <c r="L30" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M30" s="40"/>
-      <c r="N30" s="40" t="s">
+      <c r="M30" s="39"/>
+      <c r="N30" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="O30" s="39" t="s">
+      <c r="O30" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="P30" s="39" t="s">
+      <c r="P30" s="38" t="s">
         <v>19</v>
       </c>
       <c r="Q30" s="34">
@@ -4049,7 +4046,7 @@
       <c r="S30" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T30" s="48" t="s">
+      <c r="T30" s="47" t="s">
         <v>137</v>
       </c>
       <c r="U30" s="34" t="s">
@@ -4058,10 +4055,10 @@
       <c r="V30" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="W30" s="42">
+      <c r="W30" s="41">
         <v>42452</v>
       </c>
-      <c r="X30" s="42">
+      <c r="X30" s="41">
         <v>42420</v>
       </c>
     </row>
@@ -4080,30 +4077,30 @@
       </c>
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
-      <c r="G31" s="39" t="s">
+      <c r="G31" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="H31" s="39">
+      <c r="H31" s="38">
         <v>29</v>
       </c>
-      <c r="I31" s="40" t="s">
+      <c r="I31" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="J31" s="39" t="s">
+      <c r="J31" s="38" t="s">
         <v>196</v>
       </c>
-      <c r="K31" s="40" t="s">
+      <c r="K31" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="L31" s="40" t="s">
+      <c r="L31" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="M31" s="40"/>
-      <c r="N31" s="40" t="s">
+      <c r="M31" s="39"/>
+      <c r="N31" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="O31" s="39"/>
-      <c r="P31" s="39" t="s">
+      <c r="O31" s="38"/>
+      <c r="P31" s="38" t="s">
         <v>20</v>
       </c>
       <c r="Q31" s="34">
@@ -4115,7 +4112,7 @@
       <c r="S31" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="T31" s="48" t="s">
+      <c r="T31" s="47" t="s">
         <v>216</v>
       </c>
       <c r="U31" s="34" t="s">
@@ -4124,10 +4121,10 @@
       <c r="V31" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="W31" s="42">
+      <c r="W31" s="41">
         <v>42420</v>
       </c>
-      <c r="X31" s="42">
+      <c r="X31" s="41">
         <v>42420</v>
       </c>
     </row>
@@ -4178,10 +4175,10 @@
       <c r="U33" s="16"/>
       <c r="V33" s="17"/>
       <c r="W33" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="X33" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="34" spans="1:24" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4207,13 +4204,13 @@
       <c r="T34" s="16"/>
       <c r="U34" s="16"/>
       <c r="V34" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="W34" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="X34" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -4239,13 +4236,13 @@
       <c r="T35" s="16"/>
       <c r="U35" s="16"/>
       <c r="V35" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="W35" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="X35" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="36" spans="1:24" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -4555,6 +4552,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4569,12 +4572,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>